<commit_message>
minor fixed on management summary
</commit_message>
<xml_diff>
--- a/Checklists/Mobile_App_Security_Checklist.xlsx
+++ b/Checklists/Mobile_App_Security_Checklist.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="17460" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="28340" yWindow="-3400" windowWidth="33600" windowHeight="15540" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="6" r:id="rId1"/>
@@ -695,9 +695,6 @@
     <t>V5: Network Communication</t>
   </si>
   <si>
-    <t>V6: Environmental Interaction</t>
-  </si>
-  <si>
     <t>V7: Code Quality and Build Settings</t>
   </si>
   <si>
@@ -909,6 +906,48 @@
   </si>
   <si>
     <t>0.8.1</t>
+  </si>
+  <si>
+    <t>Name of Tester:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">After consultation with &lt;Customer&gt; it was decided that only Level 1 requrirements are applicable to &lt;AppName&gt;. </t>
+  </si>
+  <si>
+    <t>All available functions within the App &lt;AppName&gt;.</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Initial draft</t>
+  </si>
+  <si>
+    <t>Merging of three diffeent templates</t>
+  </si>
+  <si>
+    <t>Adding Spider Chart</t>
+  </si>
+  <si>
+    <t>Rework, adding links to Testing Guide</t>
+  </si>
+  <si>
+    <t>0.9.2</t>
+  </si>
+  <si>
+    <t>QA (and sync version number with MASVS)</t>
+  </si>
+  <si>
+    <t>Free security features offered by the toolchain, such as byte-code minification, stack protection, PIE support and automatic reference counting, are activated.</t>
+  </si>
+  <si>
+    <t>0.9.3</t>
+  </si>
+  <si>
+    <t>Sync with MASVS (merge 7.9 into 7.8)</t>
   </si>
   <si>
     <r>
@@ -922,50 +961,11 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">
-Based on the OWASP Mobile Application Security Verification Standard 0.9.2</t>
+Based on the OWASP Mobile Application Security Verification Standard 0.9.3</t>
     </r>
   </si>
   <si>
-    <t>Name of Tester:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">After consultation with &lt;Customer&gt; it was decided that only Level 1 requrirements are applicable to &lt;AppName&gt;. </t>
-  </si>
-  <si>
-    <t>All available functions within the App &lt;AppName&gt;.</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Initial draft</t>
-  </si>
-  <si>
-    <t>Merging of three diffeent templates</t>
-  </si>
-  <si>
-    <t>Adding Spider Chart</t>
-  </si>
-  <si>
-    <t>Rework, adding links to Testing Guide</t>
-  </si>
-  <si>
-    <t>0.9.2</t>
-  </si>
-  <si>
-    <t>QA (and sync version number with MASVS)</t>
-  </si>
-  <si>
-    <t>Free security features offered by the toolchain, such as byte-code minification, stack protection, PIE support and automatic reference counting, are activated.</t>
-  </si>
-  <si>
-    <t>0.9.3</t>
-  </si>
-  <si>
-    <t>Sync with MASVS (merge 7.9 into 7.8)</t>
+    <t>V6: Platform Interaction</t>
   </si>
 </sst>
 </file>
@@ -1709,7 +1709,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -1884,16 +1884,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -1922,9 +1912,36 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1958,23 +1975,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="21" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="20" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="22" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="13" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2013,26 +2024,11 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="21" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="20" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="22" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="62">
@@ -2236,7 +2232,7 @@
                   <c:v>V5: Network Communication</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>V6: Environmental Interaction</c:v>
+                  <c:v>V6: Platform Interaction</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>V7: Code Quality and Build Settings</c:v>
@@ -2289,11 +2285,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2131820368"/>
-        <c:axId val="-2098782304"/>
+        <c:axId val="-2102952128"/>
+        <c:axId val="-2097814896"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="-2131820368"/>
+        <c:axId val="-2102952128"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2330,7 +2326,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2098782304"/>
+        <c:crossAx val="-2097814896"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -2338,7 +2334,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2098782304"/>
+        <c:axId val="-2097814896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2383,7 +2379,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2131820368"/>
+        <c:crossAx val="-2102952128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2571,7 +2567,7 @@
                   <c:v>V5: Network Communication</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>V6: Environmental Interaction</c:v>
+                  <c:v>V6: Platform Interaction</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>V7: Code Quality and Build Settings</c:v>
@@ -2624,11 +2620,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2132377680"/>
-        <c:axId val="-2132682256"/>
+        <c:axId val="-2132462752"/>
+        <c:axId val="-2102414192"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="-2132377680"/>
+        <c:axId val="-2132462752"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2665,7 +2661,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2132682256"/>
+        <c:crossAx val="-2102414192"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -2673,7 +2669,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2132682256"/>
+        <c:axId val="-2102414192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2718,7 +2714,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2132377680"/>
+        <c:crossAx val="-2132462752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3246,7 +3242,7 @@
   <dimension ref="B1:D45"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="B9" sqref="B9:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3258,48 +3254,48 @@
   <sheetData>
     <row r="1" spans="2:4" ht="8" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B2" s="86" t="s">
-        <v>292</v>
-      </c>
-      <c r="C2" s="87"/>
-      <c r="D2" s="88"/>
+      <c r="B2" s="92" t="s">
+        <v>305</v>
+      </c>
+      <c r="C2" s="93"/>
+      <c r="D2" s="94"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="89"/>
-      <c r="C3" s="90"/>
-      <c r="D3" s="91"/>
+      <c r="B3" s="95"/>
+      <c r="C3" s="96"/>
+      <c r="D3" s="97"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B4" s="89"/>
-      <c r="C4" s="90"/>
-      <c r="D4" s="91"/>
+      <c r="B4" s="95"/>
+      <c r="C4" s="96"/>
+      <c r="D4" s="97"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="89"/>
-      <c r="C5" s="90"/>
-      <c r="D5" s="91"/>
+      <c r="B5" s="95"/>
+      <c r="C5" s="96"/>
+      <c r="D5" s="97"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B6" s="89"/>
-      <c r="C6" s="90"/>
-      <c r="D6" s="91"/>
+      <c r="B6" s="95"/>
+      <c r="C6" s="96"/>
+      <c r="D6" s="97"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B7" s="89"/>
-      <c r="C7" s="90"/>
-      <c r="D7" s="91"/>
+      <c r="B7" s="95"/>
+      <c r="C7" s="96"/>
+      <c r="D7" s="97"/>
     </row>
     <row r="8" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="92"/>
-      <c r="C8" s="93"/>
-      <c r="D8" s="94"/>
+      <c r="B8" s="98"/>
+      <c r="C8" s="99"/>
+      <c r="D8" s="100"/>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B9" s="95" t="s">
+      <c r="B9" s="101" t="s">
         <v>198</v>
       </c>
-      <c r="C9" s="96"/>
-      <c r="D9" s="97"/>
+      <c r="C9" s="89"/>
+      <c r="D9" s="90"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
@@ -3309,62 +3305,62 @@
       <c r="D10" s="3"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B11" s="82" t="s">
+      <c r="B11" s="87" t="s">
         <v>176</v>
       </c>
-      <c r="C11" s="83"/>
+      <c r="C11" s="88"/>
       <c r="D11" s="13"/>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B12" s="84" t="s">
+      <c r="B12" s="82" t="s">
         <v>177</v>
       </c>
-      <c r="C12" s="85"/>
+      <c r="C12" s="91"/>
       <c r="D12" s="13"/>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B13" s="82" t="s">
+      <c r="B13" s="87" t="s">
         <v>187</v>
       </c>
-      <c r="C13" s="83"/>
-      <c r="D13" s="69"/>
+      <c r="C13" s="88"/>
+      <c r="D13" s="13"/>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B14" s="82" t="s">
+      <c r="B14" s="87" t="s">
         <v>178</v>
       </c>
-      <c r="C14" s="83"/>
-      <c r="D14" s="70"/>
+      <c r="C14" s="88"/>
+      <c r="D14" s="13"/>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B15" s="82" t="s">
+      <c r="B15" s="87" t="s">
+        <v>291</v>
+      </c>
+      <c r="C15" s="88"/>
+      <c r="D15" s="13"/>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B16" s="87" t="s">
+        <v>197</v>
+      </c>
+      <c r="C16" s="88"/>
+      <c r="D16" s="13" t="s">
         <v>293</v>
       </c>
-      <c r="C15" s="83"/>
-      <c r="D15" s="70"/>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B16" s="82" t="s">
-        <v>197</v>
-      </c>
-      <c r="C16" s="83"/>
-      <c r="D16" s="71" t="s">
-        <v>295</v>
-      </c>
     </row>
     <row r="17" spans="2:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="82" t="s">
+      <c r="B17" s="87" t="s">
         <v>199</v>
       </c>
-      <c r="C17" s="83"/>
-      <c r="D17" s="71" t="s">
-        <v>294</v>
+      <c r="C17" s="88"/>
+      <c r="D17" s="13" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B18" s="96"/>
-      <c r="C18" s="96"/>
-      <c r="D18" s="97"/>
+      <c r="B18" s="89"/>
+      <c r="C18" s="89"/>
+      <c r="D18" s="90"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
@@ -3378,40 +3374,40 @@
         <v>179</v>
       </c>
       <c r="C20" s="5"/>
-      <c r="D20" s="70"/>
+      <c r="D20" s="13"/>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B21" s="82" t="s">
+      <c r="B21" s="87" t="s">
         <v>189</v>
       </c>
-      <c r="C21" s="83"/>
-      <c r="D21" s="70"/>
+      <c r="C21" s="88"/>
+      <c r="D21" s="13"/>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B22" s="82" t="s">
+      <c r="B22" s="87" t="s">
         <v>190</v>
       </c>
-      <c r="C22" s="83"/>
-      <c r="D22" s="70"/>
+      <c r="C22" s="88"/>
+      <c r="D22" s="13"/>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B23" s="82" t="s">
+      <c r="B23" s="87" t="s">
         <v>191</v>
       </c>
-      <c r="C23" s="83"/>
-      <c r="D23" s="70"/>
+      <c r="C23" s="88"/>
+      <c r="D23" s="13"/>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B24" s="82" t="s">
+      <c r="B24" s="87" t="s">
         <v>192</v>
       </c>
-      <c r="C24" s="83"/>
-      <c r="D24" s="70"/>
+      <c r="C24" s="88"/>
+      <c r="D24" s="13"/>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B25" s="96"/>
-      <c r="C25" s="96"/>
-      <c r="D25" s="97"/>
+      <c r="B25" s="89"/>
+      <c r="C25" s="89"/>
+      <c r="D25" s="90"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
@@ -3421,44 +3417,44 @@
       <c r="D26" s="3"/>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="79" t="s">
         <v>179</v>
       </c>
-      <c r="C27" s="5"/>
-      <c r="D27" s="70"/>
+      <c r="C27" s="80"/>
+      <c r="D27" s="13"/>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B28" s="82" t="s">
+      <c r="B28" s="87" t="s">
         <v>180</v>
       </c>
-      <c r="C28" s="83"/>
-      <c r="D28" s="70"/>
+      <c r="C28" s="88"/>
+      <c r="D28" s="13"/>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B29" s="82" t="s">
+      <c r="B29" s="87" t="s">
         <v>190</v>
       </c>
-      <c r="C29" s="83"/>
-      <c r="D29" s="70"/>
+      <c r="C29" s="88"/>
+      <c r="D29" s="13"/>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B30" s="82" t="s">
+      <c r="B30" s="87" t="s">
         <v>191</v>
       </c>
-      <c r="C30" s="83"/>
-      <c r="D30" s="70"/>
+      <c r="C30" s="88"/>
+      <c r="D30" s="13"/>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B31" s="82" t="s">
+      <c r="B31" s="87" t="s">
         <v>194</v>
       </c>
-      <c r="C31" s="83"/>
-      <c r="D31" s="70"/>
+      <c r="C31" s="88"/>
+      <c r="D31" s="13"/>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B32" s="96"/>
-      <c r="C32" s="96"/>
-      <c r="D32" s="97"/>
+      <c r="B32" s="89"/>
+      <c r="C32" s="89"/>
+      <c r="D32" s="90"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
@@ -3468,97 +3464,95 @@
       <c r="D33" s="3"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B34" s="98"/>
-      <c r="C34" s="99"/>
-      <c r="D34" s="100"/>
+      <c r="B34" s="84"/>
+      <c r="C34" s="85"/>
+      <c r="D34" s="86"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B35" s="84" t="s">
+      <c r="B35" s="82" t="s">
         <v>182</v>
       </c>
-      <c r="C35" s="101"/>
-      <c r="D35" s="72"/>
+      <c r="C35" s="83"/>
+      <c r="D35" s="69"/>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B36" s="84" t="s">
+      <c r="B36" s="82" t="s">
         <v>183</v>
       </c>
-      <c r="C36" s="101"/>
-      <c r="D36" s="72"/>
+      <c r="C36" s="83"/>
+      <c r="D36" s="69"/>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B37" s="84" t="s">
+      <c r="B37" s="82" t="s">
         <v>184</v>
       </c>
-      <c r="C37" s="101"/>
-      <c r="D37" s="72"/>
+      <c r="C37" s="83"/>
+      <c r="D37" s="69"/>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B38" s="84" t="s">
+      <c r="B38" s="82" t="s">
         <v>185</v>
       </c>
-      <c r="C38" s="101"/>
-      <c r="D38" s="73"/>
+      <c r="C38" s="83"/>
+      <c r="D38" s="70"/>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B39" s="84" t="s">
+      <c r="B39" s="82" t="s">
         <v>186</v>
       </c>
-      <c r="C39" s="101"/>
-      <c r="D39" s="72"/>
+      <c r="C39" s="83"/>
+      <c r="D39" s="69"/>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B40" s="98"/>
-      <c r="C40" s="99"/>
-      <c r="D40" s="100"/>
+      <c r="B40" s="84"/>
+      <c r="C40" s="85"/>
+      <c r="D40" s="86"/>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B41" s="84" t="s">
+      <c r="B41" s="82" t="s">
         <v>182</v>
       </c>
-      <c r="C41" s="101"/>
-      <c r="D41" s="72"/>
+      <c r="C41" s="83"/>
+      <c r="D41" s="69"/>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B42" s="84" t="s">
+      <c r="B42" s="82" t="s">
         <v>183</v>
       </c>
-      <c r="C42" s="101"/>
-      <c r="D42" s="72"/>
+      <c r="C42" s="83"/>
+      <c r="D42" s="69"/>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B43" s="84" t="s">
+      <c r="B43" s="82" t="s">
         <v>184</v>
       </c>
-      <c r="C43" s="101"/>
-      <c r="D43" s="72"/>
+      <c r="C43" s="83"/>
+      <c r="D43" s="69"/>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B44" s="84" t="s">
+      <c r="B44" s="82" t="s">
         <v>185</v>
       </c>
-      <c r="C44" s="101"/>
-      <c r="D44" s="73"/>
+      <c r="C44" s="83"/>
+      <c r="D44" s="70"/>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B45" s="84" t="s">
+      <c r="B45" s="82" t="s">
         <v>186</v>
       </c>
-      <c r="C45" s="101"/>
-      <c r="D45" s="72"/>
+      <c r="C45" s="83"/>
+      <c r="D45" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B2:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B15:C15"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B34:D34"/>
@@ -3573,20 +3567,17 @@
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B2:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="B41:C41"/>
   </mergeCells>
-  <dataValidations xWindow="728" yWindow="526" count="3">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Insert date testing occurred" sqref="D13"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Insert city, state and address or building number" sqref="D12"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Insert complete agency name" sqref="D11"/>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
@@ -3597,8 +3588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:X50"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A9" zoomScale="88" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView showGridLines="0" topLeftCell="A34" zoomScale="88" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -3631,11 +3622,11 @@
       <c r="F3" s="9"/>
     </row>
     <row r="4" spans="2:24" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="B4" s="102"/>
-      <c r="C4" s="102"/>
-      <c r="D4" s="102"/>
-      <c r="E4" s="102"/>
-      <c r="F4" s="102"/>
+      <c r="B4" s="106"/>
+      <c r="C4" s="106"/>
+      <c r="D4" s="106"/>
+      <c r="E4" s="106"/>
+      <c r="F4" s="106"/>
     </row>
     <row r="5" spans="2:24" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="21"/>
@@ -3650,16 +3641,16 @@
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
       <c r="F6" s="22"/>
-      <c r="G6" s="112" t="s">
+      <c r="G6" s="116" t="s">
         <v>210</v>
       </c>
-      <c r="H6" s="113"/>
-      <c r="I6" s="114"/>
-      <c r="V6" s="112" t="s">
+      <c r="H6" s="117"/>
+      <c r="I6" s="118"/>
+      <c r="V6" s="116" t="s">
         <v>210</v>
       </c>
-      <c r="W6" s="113"/>
-      <c r="X6" s="114"/>
+      <c r="W6" s="117"/>
+      <c r="X6" s="118"/>
     </row>
     <row r="7" spans="2:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="14"/>
@@ -3674,18 +3665,18 @@
       <c r="D8" s="21"/>
       <c r="E8" s="21"/>
       <c r="F8" s="21"/>
-      <c r="G8" s="103" t="e">
+      <c r="G8" s="107" t="e">
         <f>AVERAGE(G43:G50)*5</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H8" s="104"/>
-      <c r="I8" s="105"/>
-      <c r="V8" s="103" t="e">
+      <c r="H8" s="108"/>
+      <c r="I8" s="109"/>
+      <c r="V8" s="107" t="e">
         <f>AVERAGE(K43:K50)*5</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="W8" s="104"/>
-      <c r="X8" s="105"/>
+      <c r="W8" s="108"/>
+      <c r="X8" s="109"/>
     </row>
     <row r="9" spans="2:24" ht="91" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="22"/>
@@ -3693,12 +3684,12 @@
       <c r="D9" s="22"/>
       <c r="E9" s="22"/>
       <c r="F9" s="22"/>
-      <c r="G9" s="106"/>
-      <c r="H9" s="107"/>
-      <c r="I9" s="108"/>
-      <c r="V9" s="106"/>
-      <c r="W9" s="107"/>
-      <c r="X9" s="108"/>
+      <c r="G9" s="110"/>
+      <c r="H9" s="111"/>
+      <c r="I9" s="112"/>
+      <c r="V9" s="110"/>
+      <c r="W9" s="111"/>
+      <c r="X9" s="112"/>
     </row>
     <row r="10" spans="2:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="14"/>
@@ -3706,12 +3697,12 @@
       <c r="D10" s="14"/>
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
-      <c r="G10" s="106"/>
-      <c r="H10" s="107"/>
-      <c r="I10" s="108"/>
-      <c r="V10" s="106"/>
-      <c r="W10" s="107"/>
-      <c r="X10" s="108"/>
+      <c r="G10" s="110"/>
+      <c r="H10" s="111"/>
+      <c r="I10" s="112"/>
+      <c r="V10" s="110"/>
+      <c r="W10" s="111"/>
+      <c r="X10" s="112"/>
     </row>
     <row r="11" spans="2:24" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B11" s="14"/>
@@ -3719,19 +3710,19 @@
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
-      <c r="G11" s="109"/>
-      <c r="H11" s="110"/>
-      <c r="I11" s="111"/>
-      <c r="V11" s="109"/>
-      <c r="W11" s="110"/>
-      <c r="X11" s="111"/>
+      <c r="G11" s="113"/>
+      <c r="H11" s="114"/>
+      <c r="I11" s="115"/>
+      <c r="V11" s="113"/>
+      <c r="W11" s="114"/>
+      <c r="X11" s="115"/>
     </row>
     <row r="12" spans="2:24" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="115"/>
-      <c r="C12" s="115"/>
-      <c r="D12" s="115"/>
-      <c r="E12" s="115"/>
-      <c r="F12" s="115"/>
+      <c r="B12" s="102"/>
+      <c r="C12" s="102"/>
+      <c r="D12" s="102"/>
+      <c r="E12" s="102"/>
+      <c r="F12" s="102"/>
     </row>
     <row r="13" spans="2:24" ht="15" x14ac:dyDescent="0.2">
       <c r="B13" s="15"/>
@@ -3755,11 +3746,11 @@
       <c r="F15" s="14"/>
     </row>
     <row r="16" spans="2:24" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="115"/>
-      <c r="C16" s="115"/>
-      <c r="D16" s="115"/>
-      <c r="E16" s="115"/>
-      <c r="F16" s="115"/>
+      <c r="B16" s="102"/>
+      <c r="C16" s="102"/>
+      <c r="D16" s="102"/>
+      <c r="E16" s="102"/>
+      <c r="F16" s="102"/>
     </row>
     <row r="17" spans="2:6" ht="15" x14ac:dyDescent="0.2">
       <c r="B17" s="15"/>
@@ -3812,18 +3803,18 @@
     </row>
     <row r="35" spans="3:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="41" spans="3:11" x14ac:dyDescent="0.15">
-      <c r="D41" s="116" t="s">
+      <c r="D41" s="103" t="s">
         <v>208</v>
       </c>
-      <c r="E41" s="117"/>
-      <c r="F41" s="117"/>
-      <c r="G41" s="118"/>
-      <c r="H41" s="116" t="s">
+      <c r="E41" s="104"/>
+      <c r="F41" s="104"/>
+      <c r="G41" s="105"/>
+      <c r="H41" s="103" t="s">
         <v>209</v>
       </c>
-      <c r="I41" s="117"/>
-      <c r="J41" s="117"/>
-      <c r="K41" s="118"/>
+      <c r="I41" s="104"/>
+      <c r="J41" s="104"/>
+      <c r="K41" s="105"/>
     </row>
     <row r="42" spans="3:11" x14ac:dyDescent="0.15">
       <c r="D42" s="18" t="s">
@@ -4038,19 +4029,19 @@
     </row>
     <row r="48" spans="3:11" x14ac:dyDescent="0.15">
       <c r="C48" s="12" t="s">
-        <v>220</v>
+        <v>306</v>
       </c>
       <c r="D48" s="10">
-        <f>COUNTIFS('Security Requirements - Android'!F67:F74,'Security Requirements - Android'!B81)</f>
+        <f>COUNTIFS('Security Requirements - Android'!F56:F65,'Security Requirements - Android'!B81)</f>
         <v>0</v>
       </c>
       <c r="E48" s="10">
-        <f>COUNTIFS('Security Requirements - Android'!F67:F74,'Security Requirements - Android'!B82)</f>
+        <f>COUNTIFS('Security Requirements - Android'!F56:F65,'Security Requirements - Android'!B82)</f>
         <v>0</v>
       </c>
       <c r="F48" s="10">
-        <f>COUNTIFS('Security Requirements - Android'!F67:F74,'Security Requirements - Android'!B83)</f>
-        <v>8</v>
+        <f>COUNTIFS('Security Requirements - Android'!F56:F65,'Security Requirements - Android'!B83)</f>
+        <v>10</v>
       </c>
       <c r="G48" s="20" t="e">
         <f t="shared" si="0"/>
@@ -4075,7 +4066,7 @@
     </row>
     <row r="49" spans="3:11" x14ac:dyDescent="0.15">
       <c r="C49" s="12" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D49" s="10">
         <f>COUNTIFS('Security Requirements - Android'!F67:F74,'Security Requirements - Android'!B81)</f>
@@ -4086,8 +4077,8 @@
         <v>0</v>
       </c>
       <c r="F49" s="10">
-        <f>COUNTIFS('Security Requirements - Android'!F67:F74,'Security Requirements - Android'!B8)</f>
-        <v>0</v>
+        <f>COUNTIFS('Security Requirements - Android'!F67:F74,'Security Requirements - Android'!B83)</f>
+        <v>8</v>
       </c>
       <c r="G49" s="20" t="e">
         <f t="shared" si="0"/>
@@ -4112,7 +4103,7 @@
     </row>
     <row r="50" spans="3:11" x14ac:dyDescent="0.15">
       <c r="C50" s="12" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D50" s="10">
         <f>COUNTIFS('Anti-RE - Android'!E4:E19,'Security Requirements - Android'!B81)</f>
@@ -4149,6 +4140,8 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="V6:X6"/>
+    <mergeCell ref="V8:X11"/>
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="B16:F16"/>
     <mergeCell ref="D41:G41"/>
@@ -4156,8 +4149,6 @@
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="G8:I11"/>
     <mergeCell ref="G6:I6"/>
-    <mergeCell ref="V6:X6"/>
-    <mergeCell ref="V8:X11"/>
   </mergeCells>
   <conditionalFormatting sqref="F14">
     <cfRule type="iconSet" priority="3">
@@ -4197,8 +4188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H87"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4284,9 +4275,9 @@
         <v>172</v>
       </c>
       <c r="G5" s="52" t="s">
-        <v>227</v>
-      </c>
-      <c r="H5" s="121"/>
+        <v>226</v>
+      </c>
+      <c r="H5" s="81"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B6" s="35" t="s">
@@ -4305,9 +4296,9 @@
         <v>172</v>
       </c>
       <c r="G6" s="52" t="s">
-        <v>227</v>
-      </c>
-      <c r="H6" s="121"/>
+        <v>226</v>
+      </c>
+      <c r="H6" s="81"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B7" s="35" t="s">
@@ -4326,9 +4317,9 @@
         <v>172</v>
       </c>
       <c r="G7" s="52" t="s">
-        <v>227</v>
-      </c>
-      <c r="H7" s="121"/>
+        <v>226</v>
+      </c>
+      <c r="H7" s="81"/>
     </row>
     <row r="8" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B8" s="35" t="s">
@@ -4347,9 +4338,9 @@
         <v>172</v>
       </c>
       <c r="G8" s="52" t="s">
-        <v>227</v>
-      </c>
-      <c r="H8" s="121"/>
+        <v>226</v>
+      </c>
+      <c r="H8" s="81"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B9" s="35" t="s">
@@ -4368,9 +4359,9 @@
         <v>172</v>
       </c>
       <c r="G9" s="52" t="s">
-        <v>227</v>
-      </c>
-      <c r="H9" s="121"/>
+        <v>226</v>
+      </c>
+      <c r="H9" s="81"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B10" s="35" t="s">
@@ -4387,9 +4378,9 @@
         <v>172</v>
       </c>
       <c r="G10" s="52" t="s">
-        <v>227</v>
-      </c>
-      <c r="H10" s="121"/>
+        <v>226</v>
+      </c>
+      <c r="H10" s="81"/>
     </row>
     <row r="11" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B11" s="35" t="s">
@@ -4406,9 +4397,9 @@
         <v>172</v>
       </c>
       <c r="G11" s="52" t="s">
-        <v>227</v>
-      </c>
-      <c r="H11" s="121"/>
+        <v>226</v>
+      </c>
+      <c r="H11" s="81"/>
     </row>
     <row r="12" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B12" s="35" t="s">
@@ -4425,9 +4416,9 @@
         <v>172</v>
       </c>
       <c r="G12" s="52" t="s">
-        <v>227</v>
-      </c>
-      <c r="H12" s="121"/>
+        <v>226</v>
+      </c>
+      <c r="H12" s="81"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B13" s="35" t="s">
@@ -4444,9 +4435,9 @@
         <v>172</v>
       </c>
       <c r="G13" s="52" t="s">
-        <v>227</v>
-      </c>
-      <c r="H13" s="121"/>
+        <v>226</v>
+      </c>
+      <c r="H13" s="81"/>
     </row>
     <row r="14" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B14" s="35" t="s">
@@ -4463,9 +4454,9 @@
         <v>172</v>
       </c>
       <c r="G14" s="52" t="s">
-        <v>227</v>
-      </c>
-      <c r="H14" s="121"/>
+        <v>226</v>
+      </c>
+      <c r="H14" s="81"/>
     </row>
     <row r="15" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B15" s="35" t="s">
@@ -4482,9 +4473,9 @@
         <v>172</v>
       </c>
       <c r="G15" s="52" t="s">
-        <v>227</v>
-      </c>
-      <c r="H15" s="121"/>
+        <v>226</v>
+      </c>
+      <c r="H15" s="81"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B16" s="35" t="s">
@@ -4501,9 +4492,9 @@
         <v>172</v>
       </c>
       <c r="G16" s="52" t="s">
-        <v>227</v>
-      </c>
-      <c r="H16" s="121"/>
+        <v>226</v>
+      </c>
+      <c r="H16" s="81"/>
     </row>
     <row r="17" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B17" s="35" t="s">
@@ -4520,9 +4511,9 @@
         <v>172</v>
       </c>
       <c r="G17" s="52" t="s">
-        <v>227</v>
-      </c>
-      <c r="H17" s="121"/>
+        <v>226</v>
+      </c>
+      <c r="H17" s="81"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B18" s="38" t="s">
@@ -4554,9 +4545,9 @@
         <v>172</v>
       </c>
       <c r="G19" s="57" t="s">
-        <v>223</v>
-      </c>
-      <c r="H19" s="121"/>
+        <v>222</v>
+      </c>
+      <c r="H19" s="81"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B20" s="55" t="s">
@@ -4575,9 +4566,9 @@
         <v>172</v>
       </c>
       <c r="G20" s="57" t="s">
-        <v>224</v>
-      </c>
-      <c r="H20" s="121"/>
+        <v>223</v>
+      </c>
+      <c r="H20" s="81"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B21" s="55" t="s">
@@ -4596,9 +4587,9 @@
         <v>172</v>
       </c>
       <c r="G21" s="57" t="s">
-        <v>225</v>
-      </c>
-      <c r="H21" s="121"/>
+        <v>224</v>
+      </c>
+      <c r="H21" s="81"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B22" s="55" t="s">
@@ -4617,9 +4608,9 @@
         <v>172</v>
       </c>
       <c r="G22" s="63" t="s">
-        <v>226</v>
-      </c>
-      <c r="H22" s="121"/>
+        <v>225</v>
+      </c>
+      <c r="H22" s="81"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B23" s="55" t="s">
@@ -4638,9 +4629,9 @@
         <v>172</v>
       </c>
       <c r="G23" s="63" t="s">
-        <v>228</v>
-      </c>
-      <c r="H23" s="121"/>
+        <v>227</v>
+      </c>
+      <c r="H23" s="81"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B24" s="55" t="s">
@@ -4659,9 +4650,9 @@
         <v>172</v>
       </c>
       <c r="G24" s="63" t="s">
-        <v>229</v>
-      </c>
-      <c r="H24" s="121"/>
+        <v>228</v>
+      </c>
+      <c r="H24" s="81"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B25" s="55" t="s">
@@ -4680,9 +4671,9 @@
         <v>172</v>
       </c>
       <c r="G25" s="63" t="s">
-        <v>290</v>
-      </c>
-      <c r="H25" s="121"/>
+        <v>289</v>
+      </c>
+      <c r="H25" s="81"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B26" s="55" t="s">
@@ -4699,9 +4690,9 @@
         <v>172</v>
       </c>
       <c r="G26" s="63" t="s">
-        <v>230</v>
-      </c>
-      <c r="H26" s="121"/>
+        <v>229</v>
+      </c>
+      <c r="H26" s="81"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B27" s="55" t="s">
@@ -4718,9 +4709,9 @@
         <v>172</v>
       </c>
       <c r="G27" s="63" t="s">
-        <v>231</v>
-      </c>
-      <c r="H27" s="121"/>
+        <v>230</v>
+      </c>
+      <c r="H27" s="81"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B28" s="55" t="s">
@@ -4737,9 +4728,9 @@
         <v>172</v>
       </c>
       <c r="G28" s="63" t="s">
-        <v>232</v>
-      </c>
-      <c r="H28" s="121"/>
+        <v>231</v>
+      </c>
+      <c r="H28" s="81"/>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B29" s="55" t="s">
@@ -4756,9 +4747,9 @@
         <v>172</v>
       </c>
       <c r="G29" s="63" t="s">
-        <v>233</v>
-      </c>
-      <c r="H29" s="121"/>
+        <v>232</v>
+      </c>
+      <c r="H29" s="81"/>
     </row>
     <row r="30" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B30" s="55" t="s">
@@ -4775,9 +4766,9 @@
         <v>172</v>
       </c>
       <c r="G30" s="63" t="s">
-        <v>234</v>
-      </c>
-      <c r="H30" s="121"/>
+        <v>233</v>
+      </c>
+      <c r="H30" s="81"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B31" s="38" t="s">
@@ -4809,9 +4800,9 @@
         <v>172</v>
       </c>
       <c r="G32" s="63" t="s">
-        <v>235</v>
-      </c>
-      <c r="H32" s="121"/>
+        <v>234</v>
+      </c>
+      <c r="H32" s="81"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B33" s="55" t="s">
@@ -4830,9 +4821,9 @@
         <v>172</v>
       </c>
       <c r="G33" s="63" t="s">
-        <v>236</v>
-      </c>
-      <c r="H33" s="121"/>
+        <v>235</v>
+      </c>
+      <c r="H33" s="81"/>
     </row>
     <row r="34" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B34" s="55" t="s">
@@ -4851,9 +4842,9 @@
         <v>172</v>
       </c>
       <c r="G34" s="63" t="s">
-        <v>237</v>
-      </c>
-      <c r="H34" s="121"/>
+        <v>236</v>
+      </c>
+      <c r="H34" s="81"/>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B35" s="55" t="s">
@@ -4872,9 +4863,9 @@
         <v>172</v>
       </c>
       <c r="G35" s="63" t="s">
-        <v>238</v>
-      </c>
-      <c r="H35" s="121"/>
+        <v>237</v>
+      </c>
+      <c r="H35" s="81"/>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B36" s="55" t="s">
@@ -4893,9 +4884,9 @@
         <v>172</v>
       </c>
       <c r="G36" s="63" t="s">
-        <v>239</v>
-      </c>
-      <c r="H36" s="121"/>
+        <v>238</v>
+      </c>
+      <c r="H36" s="81"/>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B37" s="55" t="s">
@@ -4914,9 +4905,9 @@
         <v>172</v>
       </c>
       <c r="G37" s="63" t="s">
-        <v>235</v>
-      </c>
-      <c r="H37" s="121"/>
+        <v>234</v>
+      </c>
+      <c r="H37" s="81"/>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B38" s="38" t="s">
@@ -4948,9 +4939,9 @@
         <v>172</v>
       </c>
       <c r="G39" s="63" t="s">
-        <v>240</v>
-      </c>
-      <c r="H39" s="121"/>
+        <v>239</v>
+      </c>
+      <c r="H39" s="81"/>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B40" s="55" t="s">
@@ -4969,9 +4960,9 @@
         <v>172</v>
       </c>
       <c r="G40" s="63" t="s">
-        <v>241</v>
-      </c>
-      <c r="H40" s="121"/>
+        <v>240</v>
+      </c>
+      <c r="H40" s="81"/>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B41" s="55" t="s">
@@ -4990,9 +4981,9 @@
         <v>172</v>
       </c>
       <c r="G41" s="63" t="s">
-        <v>242</v>
-      </c>
-      <c r="H41" s="121"/>
+        <v>241</v>
+      </c>
+      <c r="H41" s="81"/>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B42" s="55" t="s">
@@ -5011,9 +5002,9 @@
         <v>172</v>
       </c>
       <c r="G42" s="63" t="s">
-        <v>243</v>
-      </c>
-      <c r="H42" s="121"/>
+        <v>242</v>
+      </c>
+      <c r="H42" s="81"/>
     </row>
     <row r="43" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B43" s="55" t="s">
@@ -5032,9 +5023,9 @@
         <v>172</v>
       </c>
       <c r="G43" s="63" t="s">
-        <v>244</v>
-      </c>
-      <c r="H43" s="121"/>
+        <v>243</v>
+      </c>
+      <c r="H43" s="81"/>
     </row>
     <row r="44" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B44" s="55" t="s">
@@ -5051,9 +5042,9 @@
         <v>172</v>
       </c>
       <c r="G44" s="63" t="s">
-        <v>245</v>
-      </c>
-      <c r="H44" s="121"/>
+        <v>244</v>
+      </c>
+      <c r="H44" s="81"/>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B45" s="55" t="s">
@@ -5070,9 +5061,9 @@
         <v>172</v>
       </c>
       <c r="G45" s="63" t="s">
-        <v>246</v>
-      </c>
-      <c r="H45" s="121"/>
+        <v>245</v>
+      </c>
+      <c r="H45" s="81"/>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B46" s="55" t="s">
@@ -5089,9 +5080,9 @@
         <v>172</v>
       </c>
       <c r="G46" s="63" t="s">
-        <v>247</v>
-      </c>
-      <c r="H46" s="121"/>
+        <v>246</v>
+      </c>
+      <c r="H46" s="81"/>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B47" s="55" t="s">
@@ -5108,9 +5099,9 @@
         <v>172</v>
       </c>
       <c r="G47" s="63" t="s">
-        <v>248</v>
-      </c>
-      <c r="H47" s="121"/>
+        <v>247</v>
+      </c>
+      <c r="H47" s="81"/>
     </row>
     <row r="48" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B48" s="55" t="s">
@@ -5127,9 +5118,9 @@
         <v>172</v>
       </c>
       <c r="G48" s="63" t="s">
-        <v>249</v>
-      </c>
-      <c r="H48" s="121"/>
+        <v>248</v>
+      </c>
+      <c r="H48" s="81"/>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B49" s="38" t="s">
@@ -5161,9 +5152,9 @@
         <v>172</v>
       </c>
       <c r="G50" s="63" t="s">
-        <v>250</v>
-      </c>
-      <c r="H50" s="121"/>
+        <v>249</v>
+      </c>
+      <c r="H50" s="81"/>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B51" s="55" t="s">
@@ -5182,9 +5173,9 @@
         <v>172</v>
       </c>
       <c r="G51" s="63" t="s">
-        <v>251</v>
-      </c>
-      <c r="H51" s="121"/>
+        <v>250</v>
+      </c>
+      <c r="H51" s="81"/>
     </row>
     <row r="52" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B52" s="55" t="s">
@@ -5203,9 +5194,9 @@
         <v>172</v>
       </c>
       <c r="G52" s="63" t="s">
-        <v>252</v>
-      </c>
-      <c r="H52" s="121"/>
+        <v>251</v>
+      </c>
+      <c r="H52" s="81"/>
     </row>
     <row r="53" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B53" s="55" t="s">
@@ -5222,9 +5213,9 @@
         <v>172</v>
       </c>
       <c r="G53" s="63" t="s">
-        <v>253</v>
-      </c>
-      <c r="H53" s="121"/>
+        <v>252</v>
+      </c>
+      <c r="H53" s="81"/>
     </row>
     <row r="54" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B54" s="55" t="s">
@@ -5241,16 +5232,16 @@
         <v>172</v>
       </c>
       <c r="G54" s="63" t="s">
-        <v>254</v>
-      </c>
-      <c r="H54" s="121"/>
+        <v>253</v>
+      </c>
+      <c r="H54" s="81"/>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B55" s="38" t="s">
         <v>44</v>
       </c>
       <c r="C55" s="39" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D55" s="39"/>
       <c r="E55" s="54"/>
@@ -5275,9 +5266,9 @@
         <v>172</v>
       </c>
       <c r="G56" s="63" t="s">
-        <v>255</v>
-      </c>
-      <c r="H56" s="121"/>
+        <v>254</v>
+      </c>
+      <c r="H56" s="81"/>
     </row>
     <row r="57" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B57" s="55" t="s">
@@ -5296,9 +5287,9 @@
         <v>172</v>
       </c>
       <c r="G57" s="63" t="s">
-        <v>256</v>
-      </c>
-      <c r="H57" s="121"/>
+        <v>255</v>
+      </c>
+      <c r="H57" s="81"/>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B58" s="55" t="s">
@@ -5317,9 +5308,9 @@
         <v>172</v>
       </c>
       <c r="G58" s="63" t="s">
-        <v>257</v>
-      </c>
-      <c r="H58" s="121"/>
+        <v>256</v>
+      </c>
+      <c r="H58" s="81"/>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B59" s="55" t="s">
@@ -5338,9 +5329,9 @@
         <v>172</v>
       </c>
       <c r="G59" s="63" t="s">
-        <v>258</v>
-      </c>
-      <c r="H59" s="121"/>
+        <v>257</v>
+      </c>
+      <c r="H59" s="81"/>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B60" s="55" t="s">
@@ -5359,9 +5350,9 @@
         <v>172</v>
       </c>
       <c r="G60" s="63" t="s">
-        <v>259</v>
-      </c>
-      <c r="H60" s="121"/>
+        <v>258</v>
+      </c>
+      <c r="H60" s="81"/>
     </row>
     <row r="61" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B61" s="55" t="s">
@@ -5380,9 +5371,9 @@
         <v>172</v>
       </c>
       <c r="G61" s="63" t="s">
-        <v>260</v>
-      </c>
-      <c r="H61" s="121"/>
+        <v>259</v>
+      </c>
+      <c r="H61" s="81"/>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B62" s="55" t="s">
@@ -5401,9 +5392,9 @@
         <v>172</v>
       </c>
       <c r="G62" s="63" t="s">
-        <v>261</v>
-      </c>
-      <c r="H62" s="121"/>
+        <v>260</v>
+      </c>
+      <c r="H62" s="81"/>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B63" s="55" t="s">
@@ -5422,9 +5413,9 @@
         <v>172</v>
       </c>
       <c r="G63" s="63" t="s">
-        <v>262</v>
-      </c>
-      <c r="H63" s="121"/>
+        <v>261</v>
+      </c>
+      <c r="H63" s="81"/>
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B64" s="55" t="s">
@@ -5443,9 +5434,9 @@
         <v>172</v>
       </c>
       <c r="G64" s="63" t="s">
-        <v>263</v>
-      </c>
-      <c r="H64" s="121"/>
+        <v>262</v>
+      </c>
+      <c r="H64" s="81"/>
     </row>
     <row r="65" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B65" s="58" t="s">
@@ -5462,9 +5453,9 @@
         <v>172</v>
       </c>
       <c r="G65" s="63" t="s">
-        <v>264</v>
-      </c>
-      <c r="H65" s="121"/>
+        <v>263</v>
+      </c>
+      <c r="H65" s="81"/>
     </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B66" s="38" t="s">
@@ -5496,9 +5487,9 @@
         <v>172</v>
       </c>
       <c r="G67" s="63" t="s">
-        <v>265</v>
-      </c>
-      <c r="H67" s="121"/>
+        <v>264</v>
+      </c>
+      <c r="H67" s="81"/>
     </row>
     <row r="68" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B68" s="55" t="s">
@@ -5517,9 +5508,9 @@
         <v>172</v>
       </c>
       <c r="G68" s="64" t="s">
-        <v>266</v>
-      </c>
-      <c r="H68" s="121"/>
+        <v>265</v>
+      </c>
+      <c r="H68" s="81"/>
     </row>
     <row r="69" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B69" s="55" t="s">
@@ -5538,9 +5529,9 @@
         <v>172</v>
       </c>
       <c r="G69" s="63" t="s">
-        <v>267</v>
-      </c>
-      <c r="H69" s="121"/>
+        <v>266</v>
+      </c>
+      <c r="H69" s="81"/>
     </row>
     <row r="70" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B70" s="55" t="s">
@@ -5559,9 +5550,9 @@
         <v>172</v>
       </c>
       <c r="G70" s="63" t="s">
-        <v>268</v>
-      </c>
-      <c r="H70" s="121"/>
+        <v>267</v>
+      </c>
+      <c r="H70" s="81"/>
     </row>
     <row r="71" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B71" s="55" t="s">
@@ -5580,9 +5571,9 @@
         <v>172</v>
       </c>
       <c r="G71" s="65" t="s">
-        <v>270</v>
-      </c>
-      <c r="H71" s="121"/>
+        <v>269</v>
+      </c>
+      <c r="H71" s="81"/>
     </row>
     <row r="72" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B72" s="55" t="s">
@@ -5601,9 +5592,9 @@
         <v>172</v>
       </c>
       <c r="G72" s="63" t="s">
-        <v>271</v>
-      </c>
-      <c r="H72" s="121"/>
+        <v>270</v>
+      </c>
+      <c r="H72" s="81"/>
     </row>
     <row r="73" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B73" s="55" t="s">
@@ -5622,16 +5613,16 @@
         <v>172</v>
       </c>
       <c r="G73" s="63" t="s">
-        <v>272</v>
-      </c>
-      <c r="H73" s="121"/>
+        <v>271</v>
+      </c>
+      <c r="H73" s="81"/>
     </row>
     <row r="74" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B74" s="55" t="s">
         <v>49</v>
       </c>
       <c r="C74" s="56" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D74" s="26" t="s">
         <v>7</v>
@@ -5643,9 +5634,9 @@
         <v>172</v>
       </c>
       <c r="G74" s="63" t="s">
-        <v>269</v>
-      </c>
-      <c r="H74" s="121"/>
+        <v>268</v>
+      </c>
+      <c r="H74" s="81"/>
     </row>
     <row r="75" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B75" s="41"/>
@@ -5857,7 +5848,7 @@
   <dimension ref="B1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5871,7 +5862,7 @@
   <sheetData>
     <row r="1" spans="2:7" ht="19" x14ac:dyDescent="0.25">
       <c r="B1" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C1" s="24"/>
       <c r="D1" s="24"/>
@@ -5929,9 +5920,9 @@
         <v>172</v>
       </c>
       <c r="F5" s="62" t="s">
-        <v>274</v>
-      </c>
-      <c r="G5" s="121"/>
+        <v>273</v>
+      </c>
+      <c r="G5" s="81"/>
     </row>
     <row r="6" spans="2:7" ht="30" x14ac:dyDescent="0.2">
       <c r="B6" s="35">
@@ -5947,9 +5938,9 @@
         <v>172</v>
       </c>
       <c r="F6" s="62" t="s">
-        <v>275</v>
-      </c>
-      <c r="G6" s="121"/>
+        <v>274</v>
+      </c>
+      <c r="G6" s="81"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B7" s="35">
@@ -5965,9 +5956,9 @@
         <v>172</v>
       </c>
       <c r="F7" s="62" t="s">
-        <v>276</v>
-      </c>
-      <c r="G7" s="121"/>
+        <v>275</v>
+      </c>
+      <c r="G7" s="81"/>
     </row>
     <row r="8" spans="2:7" ht="32" x14ac:dyDescent="0.2">
       <c r="B8" s="35">
@@ -5983,9 +5974,9 @@
         <v>172</v>
       </c>
       <c r="F8" s="62" t="s">
-        <v>277</v>
-      </c>
-      <c r="G8" s="121"/>
+        <v>276</v>
+      </c>
+      <c r="G8" s="81"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B9" s="35">
@@ -6001,9 +5992,9 @@
         <v>172</v>
       </c>
       <c r="F9" s="62" t="s">
-        <v>278</v>
-      </c>
-      <c r="G9" s="121"/>
+        <v>277</v>
+      </c>
+      <c r="G9" s="81"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B10" s="35">
@@ -6019,9 +6010,9 @@
         <v>172</v>
       </c>
       <c r="F10" s="62" t="s">
-        <v>279</v>
-      </c>
-      <c r="G10" s="121"/>
+        <v>278</v>
+      </c>
+      <c r="G10" s="81"/>
     </row>
     <row r="11" spans="2:7" ht="32" x14ac:dyDescent="0.2">
       <c r="B11" s="35">
@@ -6037,9 +6028,9 @@
         <v>172</v>
       </c>
       <c r="F11" s="62" t="s">
-        <v>280</v>
-      </c>
-      <c r="G11" s="121"/>
+        <v>279</v>
+      </c>
+      <c r="G11" s="81"/>
     </row>
     <row r="12" spans="2:7" ht="30" x14ac:dyDescent="0.2">
       <c r="B12" s="35">
@@ -6055,9 +6046,9 @@
         <v>172</v>
       </c>
       <c r="F12" s="62" t="s">
-        <v>281</v>
-      </c>
-      <c r="G12" s="121"/>
+        <v>280</v>
+      </c>
+      <c r="G12" s="81"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B13" s="35">
@@ -6073,9 +6064,9 @@
         <v>172</v>
       </c>
       <c r="F13" s="62" t="s">
-        <v>282</v>
-      </c>
-      <c r="G13" s="121"/>
+        <v>281</v>
+      </c>
+      <c r="G13" s="81"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B14" s="38"/>
@@ -6088,7 +6079,7 @@
       <c r="G14" s="40"/>
     </row>
     <row r="15" spans="2:7" ht="30" x14ac:dyDescent="0.2">
-      <c r="B15" s="81" t="s">
+      <c r="B15" s="78" t="s">
         <v>164</v>
       </c>
       <c r="C15" s="36" t="s">
@@ -6101,9 +6092,9 @@
         <v>172</v>
       </c>
       <c r="F15" s="62" t="s">
-        <v>283</v>
-      </c>
-      <c r="G15" s="121"/>
+        <v>282</v>
+      </c>
+      <c r="G15" s="81"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B16" s="38"/>
@@ -6129,9 +6120,9 @@
         <v>172</v>
       </c>
       <c r="F17" s="62" t="s">
-        <v>284</v>
-      </c>
-      <c r="G17" s="121"/>
+        <v>283</v>
+      </c>
+      <c r="G17" s="81"/>
     </row>
     <row r="18" spans="2:7" ht="45" x14ac:dyDescent="0.2">
       <c r="B18" s="35">
@@ -6147,9 +6138,9 @@
         <v>172</v>
       </c>
       <c r="F18" s="62" t="s">
-        <v>285</v>
-      </c>
-      <c r="G18" s="121"/>
+        <v>284</v>
+      </c>
+      <c r="G18" s="81"/>
     </row>
     <row r="19" spans="2:7" ht="45" x14ac:dyDescent="0.2">
       <c r="B19" s="35">
@@ -6165,9 +6156,9 @@
         <v>172</v>
       </c>
       <c r="F19" s="62" t="s">
-        <v>285</v>
-      </c>
-      <c r="G19" s="121"/>
+        <v>284</v>
+      </c>
+      <c r="G19" s="81"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B20" s="41"/>
@@ -6306,7 +6297,7 @@
   <dimension ref="B1:H87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6321,7 +6312,7 @@
   <sheetData>
     <row r="1" spans="2:8" ht="19" x14ac:dyDescent="0.25">
       <c r="B1" s="59" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C1" s="50"/>
       <c r="D1" s="50"/>
@@ -6392,7 +6383,7 @@
         <v>172</v>
       </c>
       <c r="G5" s="60"/>
-      <c r="H5" s="121"/>
+      <c r="H5" s="81"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B6" s="35" t="s">
@@ -6411,7 +6402,7 @@
         <v>172</v>
       </c>
       <c r="G6" s="60"/>
-      <c r="H6" s="121"/>
+      <c r="H6" s="81"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B7" s="35" t="s">
@@ -6430,7 +6421,7 @@
         <v>172</v>
       </c>
       <c r="G7" s="60"/>
-      <c r="H7" s="121"/>
+      <c r="H7" s="81"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B8" s="35" t="s">
@@ -6449,7 +6440,7 @@
         <v>172</v>
       </c>
       <c r="G8" s="60"/>
-      <c r="H8" s="121"/>
+      <c r="H8" s="81"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B9" s="35" t="s">
@@ -6468,7 +6459,7 @@
         <v>172</v>
       </c>
       <c r="G9" s="60"/>
-      <c r="H9" s="121"/>
+      <c r="H9" s="81"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B10" s="35" t="s">
@@ -6485,7 +6476,7 @@
         <v>172</v>
       </c>
       <c r="G10" s="60"/>
-      <c r="H10" s="121"/>
+      <c r="H10" s="81"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B11" s="35" t="s">
@@ -6502,7 +6493,7 @@
         <v>172</v>
       </c>
       <c r="G11" s="60"/>
-      <c r="H11" s="121"/>
+      <c r="H11" s="81"/>
     </row>
     <row r="12" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B12" s="35" t="s">
@@ -6519,7 +6510,7 @@
         <v>172</v>
       </c>
       <c r="G12" s="60"/>
-      <c r="H12" s="121"/>
+      <c r="H12" s="81"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B13" s="35" t="s">
@@ -6536,7 +6527,7 @@
         <v>172</v>
       </c>
       <c r="G13" s="60"/>
-      <c r="H13" s="121"/>
+      <c r="H13" s="81"/>
     </row>
     <row r="14" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B14" s="35" t="s">
@@ -6553,7 +6544,7 @@
         <v>172</v>
       </c>
       <c r="G14" s="60"/>
-      <c r="H14" s="121"/>
+      <c r="H14" s="81"/>
     </row>
     <row r="15" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B15" s="35" t="s">
@@ -6570,7 +6561,7 @@
         <v>172</v>
       </c>
       <c r="G15" s="60"/>
-      <c r="H15" s="121"/>
+      <c r="H15" s="81"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B16" s="35" t="s">
@@ -6587,7 +6578,7 @@
         <v>172</v>
       </c>
       <c r="G16" s="60"/>
-      <c r="H16" s="121"/>
+      <c r="H16" s="81"/>
     </row>
     <row r="17" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B17" s="35" t="s">
@@ -6604,7 +6595,7 @@
         <v>172</v>
       </c>
       <c r="G17" s="60"/>
-      <c r="H17" s="121"/>
+      <c r="H17" s="81"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B18" s="38" t="s">
@@ -6636,9 +6627,9 @@
         <v>172</v>
       </c>
       <c r="G19" s="63" t="s">
-        <v>223</v>
-      </c>
-      <c r="H19" s="121"/>
+        <v>222</v>
+      </c>
+      <c r="H19" s="81"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B20" s="55" t="s">
@@ -6657,9 +6648,9 @@
         <v>172</v>
       </c>
       <c r="G20" s="63" t="s">
-        <v>224</v>
-      </c>
-      <c r="H20" s="121"/>
+        <v>223</v>
+      </c>
+      <c r="H20" s="81"/>
     </row>
     <row r="21" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B21" s="55" t="s">
@@ -6678,9 +6669,9 @@
         <v>172</v>
       </c>
       <c r="G21" s="63" t="s">
-        <v>225</v>
-      </c>
-      <c r="H21" s="121"/>
+        <v>224</v>
+      </c>
+      <c r="H21" s="81"/>
     </row>
     <row r="22" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B22" s="55" t="s">
@@ -6699,9 +6690,9 @@
         <v>172</v>
       </c>
       <c r="G22" s="63" t="s">
-        <v>226</v>
-      </c>
-      <c r="H22" s="121"/>
+        <v>225</v>
+      </c>
+      <c r="H22" s="81"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B23" s="55" t="s">
@@ -6720,9 +6711,9 @@
         <v>172</v>
       </c>
       <c r="G23" s="63" t="s">
-        <v>228</v>
-      </c>
-      <c r="H23" s="121"/>
+        <v>227</v>
+      </c>
+      <c r="H23" s="81"/>
     </row>
     <row r="24" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B24" s="55" t="s">
@@ -6741,9 +6732,9 @@
         <v>172</v>
       </c>
       <c r="G24" s="63" t="s">
-        <v>229</v>
-      </c>
-      <c r="H24" s="121"/>
+        <v>228</v>
+      </c>
+      <c r="H24" s="81"/>
     </row>
     <row r="25" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B25" s="55" t="s">
@@ -6762,9 +6753,9 @@
         <v>172</v>
       </c>
       <c r="G25" s="63" t="s">
-        <v>290</v>
-      </c>
-      <c r="H25" s="121"/>
+        <v>289</v>
+      </c>
+      <c r="H25" s="81"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B26" s="55" t="s">
@@ -6781,9 +6772,9 @@
         <v>172</v>
       </c>
       <c r="G26" s="63" t="s">
-        <v>230</v>
-      </c>
-      <c r="H26" s="121"/>
+        <v>229</v>
+      </c>
+      <c r="H26" s="81"/>
     </row>
     <row r="27" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B27" s="55" t="s">
@@ -6800,9 +6791,9 @@
         <v>172</v>
       </c>
       <c r="G27" s="63" t="s">
-        <v>231</v>
-      </c>
-      <c r="H27" s="121"/>
+        <v>230</v>
+      </c>
+      <c r="H27" s="81"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B28" s="55" t="s">
@@ -6819,9 +6810,9 @@
         <v>172</v>
       </c>
       <c r="G28" s="63" t="s">
-        <v>232</v>
-      </c>
-      <c r="H28" s="121"/>
+        <v>231</v>
+      </c>
+      <c r="H28" s="81"/>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B29" s="55" t="s">
@@ -6838,9 +6829,9 @@
         <v>172</v>
       </c>
       <c r="G29" s="63" t="s">
-        <v>233</v>
-      </c>
-      <c r="H29" s="121"/>
+        <v>232</v>
+      </c>
+      <c r="H29" s="81"/>
     </row>
     <row r="30" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B30" s="55" t="s">
@@ -6857,9 +6848,9 @@
         <v>172</v>
       </c>
       <c r="G30" s="63" t="s">
-        <v>234</v>
-      </c>
-      <c r="H30" s="121"/>
+        <v>233</v>
+      </c>
+      <c r="H30" s="81"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B31" s="38" t="s">
@@ -6891,9 +6882,9 @@
         <v>172</v>
       </c>
       <c r="G32" s="63" t="s">
-        <v>235</v>
-      </c>
-      <c r="H32" s="121"/>
+        <v>234</v>
+      </c>
+      <c r="H32" s="81"/>
     </row>
     <row r="33" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B33" s="55" t="s">
@@ -6912,9 +6903,9 @@
         <v>172</v>
       </c>
       <c r="G33" s="63" t="s">
-        <v>236</v>
-      </c>
-      <c r="H33" s="121"/>
+        <v>235</v>
+      </c>
+      <c r="H33" s="81"/>
     </row>
     <row r="34" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B34" s="55" t="s">
@@ -6933,9 +6924,9 @@
         <v>172</v>
       </c>
       <c r="G34" s="63" t="s">
-        <v>237</v>
-      </c>
-      <c r="H34" s="121"/>
+        <v>236</v>
+      </c>
+      <c r="H34" s="81"/>
     </row>
     <row r="35" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B35" s="55" t="s">
@@ -6954,9 +6945,9 @@
         <v>172</v>
       </c>
       <c r="G35" s="63" t="s">
-        <v>238</v>
-      </c>
-      <c r="H35" s="121"/>
+        <v>237</v>
+      </c>
+      <c r="H35" s="81"/>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B36" s="55" t="s">
@@ -6975,9 +6966,9 @@
         <v>172</v>
       </c>
       <c r="G36" s="63" t="s">
-        <v>239</v>
-      </c>
-      <c r="H36" s="121"/>
+        <v>238</v>
+      </c>
+      <c r="H36" s="81"/>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B37" s="55" t="s">
@@ -6996,9 +6987,9 @@
         <v>172</v>
       </c>
       <c r="G37" s="63" t="s">
-        <v>235</v>
-      </c>
-      <c r="H37" s="121"/>
+        <v>234</v>
+      </c>
+      <c r="H37" s="81"/>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B38" s="38" t="s">
@@ -7030,9 +7021,9 @@
         <v>172</v>
       </c>
       <c r="G39" s="63" t="s">
-        <v>240</v>
-      </c>
-      <c r="H39" s="121"/>
+        <v>239</v>
+      </c>
+      <c r="H39" s="81"/>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B40" s="55" t="s">
@@ -7051,9 +7042,9 @@
         <v>172</v>
       </c>
       <c r="G40" s="63" t="s">
-        <v>241</v>
-      </c>
-      <c r="H40" s="121"/>
+        <v>240</v>
+      </c>
+      <c r="H40" s="81"/>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B41" s="55" t="s">
@@ -7072,9 +7063,9 @@
         <v>172</v>
       </c>
       <c r="G41" s="63" t="s">
-        <v>242</v>
-      </c>
-      <c r="H41" s="121"/>
+        <v>241</v>
+      </c>
+      <c r="H41" s="81"/>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B42" s="55" t="s">
@@ -7093,9 +7084,9 @@
         <v>172</v>
       </c>
       <c r="G42" s="63" t="s">
-        <v>243</v>
-      </c>
-      <c r="H42" s="121"/>
+        <v>242</v>
+      </c>
+      <c r="H42" s="81"/>
     </row>
     <row r="43" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B43" s="55" t="s">
@@ -7114,9 +7105,9 @@
         <v>172</v>
       </c>
       <c r="G43" s="63" t="s">
-        <v>244</v>
-      </c>
-      <c r="H43" s="121"/>
+        <v>243</v>
+      </c>
+      <c r="H43" s="81"/>
     </row>
     <row r="44" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B44" s="55" t="s">
@@ -7133,9 +7124,9 @@
         <v>172</v>
       </c>
       <c r="G44" s="63" t="s">
-        <v>245</v>
-      </c>
-      <c r="H44" s="121"/>
+        <v>244</v>
+      </c>
+      <c r="H44" s="81"/>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B45" s="55" t="s">
@@ -7152,9 +7143,9 @@
         <v>172</v>
       </c>
       <c r="G45" s="63" t="s">
-        <v>246</v>
-      </c>
-      <c r="H45" s="121"/>
+        <v>245</v>
+      </c>
+      <c r="H45" s="81"/>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B46" s="55" t="s">
@@ -7171,9 +7162,9 @@
         <v>172</v>
       </c>
       <c r="G46" s="63" t="s">
-        <v>247</v>
-      </c>
-      <c r="H46" s="121"/>
+        <v>246</v>
+      </c>
+      <c r="H46" s="81"/>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B47" s="55" t="s">
@@ -7190,9 +7181,9 @@
         <v>172</v>
       </c>
       <c r="G47" s="63" t="s">
-        <v>248</v>
-      </c>
-      <c r="H47" s="121"/>
+        <v>247</v>
+      </c>
+      <c r="H47" s="81"/>
     </row>
     <row r="48" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B48" s="55" t="s">
@@ -7209,9 +7200,9 @@
         <v>172</v>
       </c>
       <c r="G48" s="63" t="s">
-        <v>249</v>
-      </c>
-      <c r="H48" s="121"/>
+        <v>248</v>
+      </c>
+      <c r="H48" s="81"/>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B49" s="38" t="s">
@@ -7243,9 +7234,9 @@
         <v>172</v>
       </c>
       <c r="G50" s="63" t="s">
-        <v>250</v>
-      </c>
-      <c r="H50" s="121"/>
+        <v>249</v>
+      </c>
+      <c r="H50" s="81"/>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B51" s="55" t="s">
@@ -7264,9 +7255,9 @@
         <v>172</v>
       </c>
       <c r="G51" s="63" t="s">
-        <v>251</v>
-      </c>
-      <c r="H51" s="121"/>
+        <v>250</v>
+      </c>
+      <c r="H51" s="81"/>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B52" s="55" t="s">
@@ -7285,9 +7276,9 @@
         <v>172</v>
       </c>
       <c r="G52" s="63" t="s">
-        <v>252</v>
-      </c>
-      <c r="H52" s="121"/>
+        <v>251</v>
+      </c>
+      <c r="H52" s="81"/>
     </row>
     <row r="53" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B53" s="55" t="s">
@@ -7304,9 +7295,9 @@
         <v>172</v>
       </c>
       <c r="G53" s="63" t="s">
-        <v>253</v>
-      </c>
-      <c r="H53" s="121"/>
+        <v>252</v>
+      </c>
+      <c r="H53" s="81"/>
     </row>
     <row r="54" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B54" s="55" t="s">
@@ -7323,9 +7314,9 @@
         <v>172</v>
       </c>
       <c r="G54" s="63" t="s">
-        <v>254</v>
-      </c>
-      <c r="H54" s="121"/>
+        <v>253</v>
+      </c>
+      <c r="H54" s="81"/>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B55" s="38" t="s">
@@ -7357,9 +7348,9 @@
         <v>172</v>
       </c>
       <c r="G56" s="63" t="s">
-        <v>255</v>
-      </c>
-      <c r="H56" s="121"/>
+        <v>254</v>
+      </c>
+      <c r="H56" s="81"/>
     </row>
     <row r="57" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B57" s="55" t="s">
@@ -7378,9 +7369,9 @@
         <v>172</v>
       </c>
       <c r="G57" s="63" t="s">
-        <v>256</v>
-      </c>
-      <c r="H57" s="121"/>
+        <v>255</v>
+      </c>
+      <c r="H57" s="81"/>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B58" s="55" t="s">
@@ -7399,9 +7390,9 @@
         <v>172</v>
       </c>
       <c r="G58" s="63" t="s">
-        <v>257</v>
-      </c>
-      <c r="H58" s="121"/>
+        <v>256</v>
+      </c>
+      <c r="H58" s="81"/>
     </row>
     <row r="59" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B59" s="55" t="s">
@@ -7420,9 +7411,9 @@
         <v>172</v>
       </c>
       <c r="G59" s="63" t="s">
-        <v>258</v>
-      </c>
-      <c r="H59" s="121"/>
+        <v>257</v>
+      </c>
+      <c r="H59" s="81"/>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B60" s="55" t="s">
@@ -7441,9 +7432,9 @@
         <v>172</v>
       </c>
       <c r="G60" s="63" t="s">
-        <v>259</v>
-      </c>
-      <c r="H60" s="121"/>
+        <v>258</v>
+      </c>
+      <c r="H60" s="81"/>
     </row>
     <row r="61" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B61" s="55" t="s">
@@ -7462,9 +7453,9 @@
         <v>172</v>
       </c>
       <c r="G61" s="63" t="s">
-        <v>260</v>
-      </c>
-      <c r="H61" s="121"/>
+        <v>259</v>
+      </c>
+      <c r="H61" s="81"/>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B62" s="55" t="s">
@@ -7483,9 +7474,9 @@
         <v>172</v>
       </c>
       <c r="G62" s="63" t="s">
-        <v>261</v>
-      </c>
-      <c r="H62" s="121"/>
+        <v>260</v>
+      </c>
+      <c r="H62" s="81"/>
     </row>
     <row r="63" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B63" s="55" t="s">
@@ -7504,9 +7495,9 @@
         <v>172</v>
       </c>
       <c r="G63" s="63" t="s">
-        <v>262</v>
-      </c>
-      <c r="H63" s="121"/>
+        <v>261</v>
+      </c>
+      <c r="H63" s="81"/>
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B64" s="55" t="s">
@@ -7525,9 +7516,9 @@
         <v>172</v>
       </c>
       <c r="G64" s="63" t="s">
-        <v>263</v>
-      </c>
-      <c r="H64" s="121"/>
+        <v>262</v>
+      </c>
+      <c r="H64" s="81"/>
     </row>
     <row r="65" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B65" s="58" t="s">
@@ -7544,9 +7535,9 @@
         <v>172</v>
       </c>
       <c r="G65" s="63" t="s">
-        <v>289</v>
-      </c>
-      <c r="H65" s="121"/>
+        <v>288</v>
+      </c>
+      <c r="H65" s="81"/>
     </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B66" s="38" t="s">
@@ -7578,9 +7569,9 @@
         <v>172</v>
       </c>
       <c r="G67" s="63" t="s">
-        <v>265</v>
-      </c>
-      <c r="H67" s="121"/>
+        <v>264</v>
+      </c>
+      <c r="H67" s="81"/>
     </row>
     <row r="68" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B68" s="55" t="s">
@@ -7599,9 +7590,9 @@
         <v>172</v>
       </c>
       <c r="G68" s="64" t="s">
-        <v>266</v>
-      </c>
-      <c r="H68" s="121"/>
+        <v>265</v>
+      </c>
+      <c r="H68" s="81"/>
     </row>
     <row r="69" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B69" s="55" t="s">
@@ -7620,9 +7611,9 @@
         <v>172</v>
       </c>
       <c r="G69" s="63" t="s">
-        <v>267</v>
-      </c>
-      <c r="H69" s="121"/>
+        <v>266</v>
+      </c>
+      <c r="H69" s="81"/>
     </row>
     <row r="70" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B70" s="55" t="s">
@@ -7641,9 +7632,9 @@
         <v>172</v>
       </c>
       <c r="G70" s="63" t="s">
-        <v>268</v>
-      </c>
-      <c r="H70" s="121"/>
+        <v>267</v>
+      </c>
+      <c r="H70" s="81"/>
     </row>
     <row r="71" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B71" s="55" t="s">
@@ -7662,9 +7653,9 @@
         <v>172</v>
       </c>
       <c r="G71" s="65" t="s">
-        <v>270</v>
-      </c>
-      <c r="H71" s="121"/>
+        <v>269</v>
+      </c>
+      <c r="H71" s="81"/>
     </row>
     <row r="72" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B72" s="55" t="s">
@@ -7683,9 +7674,9 @@
         <v>172</v>
       </c>
       <c r="G72" s="63" t="s">
-        <v>271</v>
-      </c>
-      <c r="H72" s="121"/>
+        <v>270</v>
+      </c>
+      <c r="H72" s="81"/>
     </row>
     <row r="73" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B73" s="55" t="s">
@@ -7704,16 +7695,16 @@
         <v>172</v>
       </c>
       <c r="G73" s="63" t="s">
-        <v>272</v>
-      </c>
-      <c r="H73" s="121"/>
+        <v>271</v>
+      </c>
+      <c r="H73" s="81"/>
     </row>
     <row r="74" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B74" s="55" t="s">
         <v>49</v>
       </c>
       <c r="C74" s="56" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D74" s="26" t="s">
         <v>7</v>
@@ -7725,9 +7716,9 @@
         <v>172</v>
       </c>
       <c r="G74" s="63" t="s">
-        <v>269</v>
-      </c>
-      <c r="H74" s="121"/>
+        <v>268</v>
+      </c>
+      <c r="H74" s="81"/>
     </row>
     <row r="75" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B75" s="41"/>
@@ -7935,8 +7926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7950,7 +7941,7 @@
   <sheetData>
     <row r="1" spans="2:7" ht="19" x14ac:dyDescent="0.25">
       <c r="B1" s="7" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G1" s="24"/>
     </row>
@@ -7999,9 +7990,9 @@
         <v>172</v>
       </c>
       <c r="F5" s="62" t="s">
-        <v>274</v>
-      </c>
-      <c r="G5" s="121"/>
+        <v>273</v>
+      </c>
+      <c r="G5" s="81"/>
     </row>
     <row r="6" spans="2:7" ht="30" x14ac:dyDescent="0.2">
       <c r="B6" s="35">
@@ -8017,9 +8008,9 @@
         <v>172</v>
       </c>
       <c r="F6" s="62" t="s">
-        <v>275</v>
-      </c>
-      <c r="G6" s="121"/>
+        <v>274</v>
+      </c>
+      <c r="G6" s="81"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B7" s="35">
@@ -8035,9 +8026,9 @@
         <v>172</v>
       </c>
       <c r="F7" s="62" t="s">
-        <v>276</v>
-      </c>
-      <c r="G7" s="121"/>
+        <v>275</v>
+      </c>
+      <c r="G7" s="81"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B8" s="35">
@@ -8053,9 +8044,9 @@
         <v>172</v>
       </c>
       <c r="F8" s="62" t="s">
-        <v>277</v>
-      </c>
-      <c r="G8" s="121"/>
+        <v>276</v>
+      </c>
+      <c r="G8" s="81"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B9" s="35">
@@ -8071,9 +8062,9 @@
         <v>172</v>
       </c>
       <c r="F9" s="62" t="s">
-        <v>278</v>
-      </c>
-      <c r="G9" s="121"/>
+        <v>277</v>
+      </c>
+      <c r="G9" s="81"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B10" s="35">
@@ -8089,9 +8080,9 @@
         <v>172</v>
       </c>
       <c r="F10" s="62" t="s">
-        <v>279</v>
-      </c>
-      <c r="G10" s="121"/>
+        <v>278</v>
+      </c>
+      <c r="G10" s="81"/>
     </row>
     <row r="11" spans="2:7" ht="30" x14ac:dyDescent="0.2">
       <c r="B11" s="35">
@@ -8107,9 +8098,9 @@
         <v>172</v>
       </c>
       <c r="F11" s="62" t="s">
-        <v>280</v>
-      </c>
-      <c r="G11" s="121"/>
+        <v>279</v>
+      </c>
+      <c r="G11" s="81"/>
     </row>
     <row r="12" spans="2:7" ht="30" x14ac:dyDescent="0.2">
       <c r="B12" s="35">
@@ -8125,9 +8116,9 @@
         <v>172</v>
       </c>
       <c r="F12" s="62" t="s">
-        <v>281</v>
-      </c>
-      <c r="G12" s="121"/>
+        <v>280</v>
+      </c>
+      <c r="G12" s="81"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B13" s="35">
@@ -8143,9 +8134,9 @@
         <v>172</v>
       </c>
       <c r="F13" s="62" t="s">
-        <v>282</v>
-      </c>
-      <c r="G13" s="121"/>
+        <v>281</v>
+      </c>
+      <c r="G13" s="81"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B14" s="38"/>
@@ -8158,7 +8149,7 @@
       <c r="G14" s="40"/>
     </row>
     <row r="15" spans="2:7" ht="30" x14ac:dyDescent="0.2">
-      <c r="B15" s="81" t="s">
+      <c r="B15" s="78" t="s">
         <v>164</v>
       </c>
       <c r="C15" s="36" t="s">
@@ -8171,9 +8162,9 @@
         <v>172</v>
       </c>
       <c r="F15" s="62" t="s">
-        <v>283</v>
-      </c>
-      <c r="G15" s="121"/>
+        <v>282</v>
+      </c>
+      <c r="G15" s="81"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B16" s="38"/>
@@ -8199,9 +8190,9 @@
         <v>172</v>
       </c>
       <c r="F17" s="62" t="s">
-        <v>284</v>
-      </c>
-      <c r="G17" s="121"/>
+        <v>283</v>
+      </c>
+      <c r="G17" s="81"/>
     </row>
     <row r="18" spans="2:7" ht="45" x14ac:dyDescent="0.2">
       <c r="B18" s="35">
@@ -8217,9 +8208,9 @@
         <v>172</v>
       </c>
       <c r="F18" s="62" t="s">
-        <v>285</v>
-      </c>
-      <c r="G18" s="121"/>
+        <v>284</v>
+      </c>
+      <c r="G18" s="81"/>
     </row>
     <row r="19" spans="2:7" ht="45" x14ac:dyDescent="0.2">
       <c r="B19" s="35">
@@ -8235,9 +8226,9 @@
         <v>172</v>
       </c>
       <c r="F19" s="62" t="s">
-        <v>285</v>
-      </c>
-      <c r="G19" s="121"/>
+        <v>284</v>
+      </c>
+      <c r="G19" s="81"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B20" s="41"/>
@@ -8396,8 +8387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8415,101 +8406,101 @@
       <c r="D1" s="50"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="77" t="s">
+      <c r="A2" s="74" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2" s="74" t="s">
+        <v>191</v>
+      </c>
+      <c r="C2" s="74" t="s">
+        <v>295</v>
+      </c>
+      <c r="D2" s="75" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="72" t="s">
+        <v>166</v>
+      </c>
+      <c r="B3" s="76">
+        <v>0.1</v>
+      </c>
+      <c r="C3" s="73">
+        <v>42765</v>
+      </c>
+      <c r="D3" s="71" t="s">
         <v>296</v>
       </c>
-      <c r="B2" s="77" t="s">
-        <v>191</v>
-      </c>
-      <c r="C2" s="77" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="71" t="s">
+        <v>167</v>
+      </c>
+      <c r="B4" s="76">
+        <v>0.2</v>
+      </c>
+      <c r="C4" s="73">
+        <v>42766</v>
+      </c>
+      <c r="D4" s="71" t="s">
         <v>297</v>
       </c>
-      <c r="D2" s="78" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="75" t="s">
-        <v>166</v>
-      </c>
-      <c r="B3" s="79">
-        <v>0.1</v>
-      </c>
-      <c r="C3" s="76">
-        <v>42765</v>
-      </c>
-      <c r="D3" s="74" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="71" t="s">
+        <v>212</v>
+      </c>
+      <c r="B5" s="76">
+        <v>0.3</v>
+      </c>
+      <c r="C5" s="73">
+        <v>42778</v>
+      </c>
+      <c r="D5" s="71" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="74" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="71" t="s">
+        <v>213</v>
+      </c>
+      <c r="B6" s="76" t="s">
+        <v>290</v>
+      </c>
+      <c r="C6" s="73">
+        <v>42780</v>
+      </c>
+      <c r="D6" s="71" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="71" t="s">
         <v>167</v>
       </c>
-      <c r="B4" s="79">
-        <v>0.2</v>
-      </c>
-      <c r="C4" s="76">
-        <v>42766</v>
-      </c>
-      <c r="D4" s="74" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="74" t="s">
-        <v>212</v>
-      </c>
-      <c r="B5" s="79">
-        <v>0.3</v>
-      </c>
-      <c r="C5" s="76">
-        <v>42778</v>
-      </c>
-      <c r="D5" s="74" t="s">
+      <c r="B7" s="77" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="74" t="s">
+      <c r="C7" s="73">
+        <v>42781</v>
+      </c>
+      <c r="D7" s="71" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="71" t="s">
         <v>213</v>
       </c>
-      <c r="B6" s="79" t="s">
-        <v>291</v>
-      </c>
-      <c r="C6" s="76">
-        <v>42780</v>
-      </c>
-      <c r="D6" s="74" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="74" t="s">
-        <v>167</v>
-      </c>
-      <c r="B7" s="80" t="s">
-        <v>302</v>
-      </c>
-      <c r="C7" s="76">
-        <v>42781</v>
-      </c>
-      <c r="D7" s="74" t="s">
+      <c r="B8" s="77" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="74" t="s">
-        <v>213</v>
-      </c>
-      <c r="B8" s="80" t="s">
-        <v>305</v>
-      </c>
-      <c r="C8" s="76">
+      <c r="C8" s="73">
         <v>42829</v>
       </c>
-      <c r="D8" s="74" t="s">
-        <v>306</v>
+      <c r="D8" s="71" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
changed requirement 2.7, small fixes
</commit_message>
<xml_diff>
--- a/Checklists/Mobile_App_Security_Checklist.xlsx
+++ b/Checklists/Mobile_App_Security_Checklist.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="-5140" windowWidth="38400" windowHeight="21060" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="25600" yWindow="-5140" windowWidth="38400" windowHeight="21060" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="6" r:id="rId1"/>
@@ -302,9 +302,6 @@
     <t xml:space="preserve">Verify that no sensitive data is exposed via IPC mechanisms. </t>
   </si>
   <si>
-    <t>Verify that no sensitive data, such as passwords and credit card numbers, is exposed through the user interface or leaks to screenshots.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Verify that no sensitive data is included in backups. </t>
   </si>
   <si>
@@ -945,6 +942,9 @@
   </si>
   <si>
     <t>V6: Platform Interaction</t>
+  </si>
+  <si>
+    <t>Verify that no sensitive data, such as passwords and credit card numbers, is exposed through the user interface.</t>
   </si>
 </sst>
 </file>
@@ -1895,13 +1895,31 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1936,23 +1954,33 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1963,33 +1991,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2002,7 +2003,6 @@
     <xf numFmtId="0" fontId="11" fillId="12" borderId="22" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2264,11 +2264,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2117684784"/>
-        <c:axId val="-2100459552"/>
+        <c:axId val="-2104214112"/>
+        <c:axId val="-2116939840"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="-2117684784"/>
+        <c:axId val="-2104214112"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2305,7 +2305,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2100459552"/>
+        <c:crossAx val="-2116939840"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -2313,7 +2313,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2100459552"/>
+        <c:axId val="-2116939840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2358,7 +2358,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2117684784"/>
+        <c:crossAx val="-2104214112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2599,11 +2599,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2100834016"/>
-        <c:axId val="-2101963024"/>
+        <c:axId val="-2103965760"/>
+        <c:axId val="-2103670208"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="-2100834016"/>
+        <c:axId val="-2103965760"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2640,7 +2640,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2101963024"/>
+        <c:crossAx val="-2103670208"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -2648,7 +2648,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2101963024"/>
+        <c:axId val="-2103670208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2693,7 +2693,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2100834016"/>
+        <c:crossAx val="-2103965760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3233,307 +3233,305 @@
   <sheetData>
     <row r="1" spans="2:4" ht="8" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B2" s="86" t="s">
-        <v>298</v>
-      </c>
-      <c r="C2" s="87"/>
-      <c r="D2" s="88"/>
+      <c r="B2" s="92" t="s">
+        <v>297</v>
+      </c>
+      <c r="C2" s="93"/>
+      <c r="D2" s="94"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="89"/>
-      <c r="C3" s="90"/>
-      <c r="D3" s="91"/>
+      <c r="B3" s="95"/>
+      <c r="C3" s="96"/>
+      <c r="D3" s="97"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B4" s="89"/>
-      <c r="C4" s="90"/>
-      <c r="D4" s="91"/>
+      <c r="B4" s="95"/>
+      <c r="C4" s="96"/>
+      <c r="D4" s="97"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="89"/>
-      <c r="C5" s="90"/>
-      <c r="D5" s="91"/>
+      <c r="B5" s="95"/>
+      <c r="C5" s="96"/>
+      <c r="D5" s="97"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B6" s="89"/>
-      <c r="C6" s="90"/>
-      <c r="D6" s="91"/>
+      <c r="B6" s="95"/>
+      <c r="C6" s="96"/>
+      <c r="D6" s="97"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B7" s="89"/>
-      <c r="C7" s="90"/>
-      <c r="D7" s="91"/>
+      <c r="B7" s="95"/>
+      <c r="C7" s="96"/>
+      <c r="D7" s="97"/>
     </row>
     <row r="8" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="92"/>
-      <c r="C8" s="93"/>
-      <c r="D8" s="94"/>
+      <c r="B8" s="98"/>
+      <c r="C8" s="99"/>
+      <c r="D8" s="100"/>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B9" s="95" t="s">
-        <v>191</v>
-      </c>
-      <c r="C9" s="96"/>
-      <c r="D9" s="97"/>
+      <c r="B9" s="101" t="s">
+        <v>190</v>
+      </c>
+      <c r="C9" s="89"/>
+      <c r="D9" s="90"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="3"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B11" s="82" t="s">
+      <c r="B11" s="87" t="s">
+        <v>168</v>
+      </c>
+      <c r="C11" s="88"/>
+      <c r="D11" s="13"/>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B12" s="82" t="s">
         <v>169</v>
       </c>
-      <c r="C11" s="83"/>
-      <c r="D11" s="13"/>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B12" s="84" t="s">
+      <c r="C12" s="91"/>
+      <c r="D12" s="13"/>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B13" s="87" t="s">
+        <v>179</v>
+      </c>
+      <c r="C13" s="88"/>
+      <c r="D13" s="13"/>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B14" s="87" t="s">
         <v>170</v>
       </c>
-      <c r="C12" s="85"/>
-      <c r="D12" s="13"/>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B13" s="82" t="s">
-        <v>180</v>
-      </c>
-      <c r="C13" s="83"/>
-      <c r="D13" s="13"/>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B14" s="82" t="s">
-        <v>171</v>
-      </c>
-      <c r="C14" s="83"/>
+      <c r="C14" s="88"/>
       <c r="D14" s="13"/>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B15" s="82" t="s">
+      <c r="B15" s="87" t="s">
+        <v>283</v>
+      </c>
+      <c r="C15" s="88"/>
+      <c r="D15" s="13"/>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B16" s="87" t="s">
+        <v>189</v>
+      </c>
+      <c r="C16" s="88"/>
+      <c r="D16" s="13" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="87" t="s">
+        <v>191</v>
+      </c>
+      <c r="C17" s="88"/>
+      <c r="D17" s="13" t="s">
         <v>284</v>
       </c>
-      <c r="C15" s="83"/>
-      <c r="D15" s="13"/>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B16" s="82" t="s">
-        <v>190</v>
-      </c>
-      <c r="C16" s="83"/>
-      <c r="D16" s="13" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="82" t="s">
-        <v>192</v>
-      </c>
-      <c r="C17" s="83"/>
-      <c r="D17" s="13" t="s">
-        <v>285</v>
-      </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B18" s="96"/>
-      <c r="C18" s="96"/>
-      <c r="D18" s="97"/>
+      <c r="B18" s="89"/>
+      <c r="C18" s="89"/>
+      <c r="D18" s="90"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="3"/>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="13"/>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B21" s="82" t="s">
+      <c r="B21" s="87" t="s">
+        <v>181</v>
+      </c>
+      <c r="C21" s="88"/>
+      <c r="D21" s="13"/>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B22" s="87" t="s">
         <v>182</v>
       </c>
-      <c r="C21" s="83"/>
-      <c r="D21" s="13"/>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B22" s="82" t="s">
+      <c r="C22" s="88"/>
+      <c r="D22" s="13"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B23" s="87" t="s">
         <v>183</v>
       </c>
-      <c r="C22" s="83"/>
-      <c r="D22" s="13"/>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B23" s="82" t="s">
+      <c r="C23" s="88"/>
+      <c r="D23" s="13"/>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B24" s="87" t="s">
         <v>184</v>
       </c>
-      <c r="C23" s="83"/>
-      <c r="D23" s="13"/>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B24" s="82" t="s">
-        <v>185</v>
-      </c>
-      <c r="C24" s="83"/>
+      <c r="C24" s="88"/>
       <c r="D24" s="13"/>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B25" s="96"/>
-      <c r="C25" s="96"/>
-      <c r="D25" s="97"/>
+      <c r="B25" s="89"/>
+      <c r="C25" s="89"/>
+      <c r="D25" s="90"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="3"/>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B27" s="79" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C27" s="80"/>
       <c r="D27" s="13"/>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B28" s="82" t="s">
-        <v>173</v>
-      </c>
-      <c r="C28" s="83"/>
+      <c r="B28" s="87" t="s">
+        <v>172</v>
+      </c>
+      <c r="C28" s="88"/>
       <c r="D28" s="13"/>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B29" s="82" t="s">
+      <c r="B29" s="87" t="s">
+        <v>182</v>
+      </c>
+      <c r="C29" s="88"/>
+      <c r="D29" s="13"/>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B30" s="87" t="s">
         <v>183</v>
       </c>
-      <c r="C29" s="83"/>
-      <c r="D29" s="13"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B30" s="82" t="s">
-        <v>184</v>
-      </c>
-      <c r="C30" s="83"/>
+      <c r="C30" s="88"/>
       <c r="D30" s="13"/>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B31" s="82" t="s">
-        <v>187</v>
-      </c>
-      <c r="C31" s="83"/>
+      <c r="B31" s="87" t="s">
+        <v>186</v>
+      </c>
+      <c r="C31" s="88"/>
       <c r="D31" s="13"/>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B32" s="96"/>
-      <c r="C32" s="96"/>
-      <c r="D32" s="97"/>
+      <c r="B32" s="89"/>
+      <c r="C32" s="89"/>
+      <c r="D32" s="90"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="3"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B34" s="98"/>
-      <c r="C34" s="99"/>
-      <c r="D34" s="100"/>
+      <c r="B34" s="84"/>
+      <c r="C34" s="85"/>
+      <c r="D34" s="86"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B35" s="84" t="s">
+      <c r="B35" s="82" t="s">
+        <v>174</v>
+      </c>
+      <c r="C35" s="83"/>
+      <c r="D35" s="69"/>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B36" s="82" t="s">
         <v>175</v>
       </c>
-      <c r="C35" s="101"/>
-      <c r="D35" s="69"/>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B36" s="84" t="s">
+      <c r="C36" s="83"/>
+      <c r="D36" s="69"/>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B37" s="82" t="s">
         <v>176</v>
       </c>
-      <c r="C36" s="101"/>
-      <c r="D36" s="69"/>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B37" s="84" t="s">
+      <c r="C37" s="83"/>
+      <c r="D37" s="69"/>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B38" s="82" t="s">
         <v>177</v>
       </c>
-      <c r="C37" s="101"/>
-      <c r="D37" s="69"/>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B38" s="84" t="s">
+      <c r="C38" s="83"/>
+      <c r="D38" s="70"/>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B39" s="82" t="s">
         <v>178</v>
       </c>
-      <c r="C38" s="101"/>
-      <c r="D38" s="70"/>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B39" s="84" t="s">
-        <v>179</v>
-      </c>
-      <c r="C39" s="101"/>
+      <c r="C39" s="83"/>
       <c r="D39" s="69"/>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B40" s="98"/>
-      <c r="C40" s="99"/>
-      <c r="D40" s="100"/>
+      <c r="B40" s="84"/>
+      <c r="C40" s="85"/>
+      <c r="D40" s="86"/>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B41" s="84" t="s">
+      <c r="B41" s="82" t="s">
+        <v>174</v>
+      </c>
+      <c r="C41" s="83"/>
+      <c r="D41" s="69"/>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B42" s="82" t="s">
         <v>175</v>
       </c>
-      <c r="C41" s="101"/>
-      <c r="D41" s="69"/>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B42" s="84" t="s">
+      <c r="C42" s="83"/>
+      <c r="D42" s="69"/>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B43" s="82" t="s">
         <v>176</v>
       </c>
-      <c r="C42" s="101"/>
-      <c r="D42" s="69"/>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B43" s="84" t="s">
+      <c r="C43" s="83"/>
+      <c r="D43" s="69"/>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B44" s="82" t="s">
         <v>177</v>
       </c>
-      <c r="C43" s="101"/>
-      <c r="D43" s="69"/>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B44" s="84" t="s">
+      <c r="C44" s="83"/>
+      <c r="D44" s="70"/>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B45" s="82" t="s">
         <v>178</v>
       </c>
-      <c r="C44" s="101"/>
-      <c r="D44" s="70"/>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B45" s="84" t="s">
-        <v>179</v>
-      </c>
-      <c r="C45" s="101"/>
+      <c r="C45" s="83"/>
       <c r="D45" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B2:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B15:C15"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B34:D34"/>
@@ -3548,14 +3546,16 @@
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B2:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="B41:C41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -3587,7 +3587,7 @@
     <row r="2" spans="2:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="8"/>
       <c r="C2" s="23" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
@@ -3601,11 +3601,11 @@
       <c r="F3" s="9"/>
     </row>
     <row r="4" spans="2:24" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="B4" s="118"/>
-      <c r="C4" s="118"/>
-      <c r="D4" s="118"/>
-      <c r="E4" s="118"/>
-      <c r="F4" s="118"/>
+      <c r="B4" s="102"/>
+      <c r="C4" s="102"/>
+      <c r="D4" s="102"/>
+      <c r="E4" s="102"/>
+      <c r="F4" s="102"/>
     </row>
     <row r="5" spans="2:24" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="21"/>
@@ -3620,16 +3620,16 @@
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
       <c r="F6" s="22"/>
-      <c r="G6" s="102" t="s">
-        <v>203</v>
-      </c>
-      <c r="H6" s="103"/>
-      <c r="I6" s="104"/>
-      <c r="V6" s="102" t="s">
-        <v>203</v>
-      </c>
-      <c r="W6" s="103"/>
-      <c r="X6" s="104"/>
+      <c r="G6" s="112" t="s">
+        <v>202</v>
+      </c>
+      <c r="H6" s="113"/>
+      <c r="I6" s="114"/>
+      <c r="V6" s="112" t="s">
+        <v>202</v>
+      </c>
+      <c r="W6" s="113"/>
+      <c r="X6" s="114"/>
     </row>
     <row r="7" spans="2:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="14"/>
@@ -3644,18 +3644,18 @@
       <c r="D8" s="21"/>
       <c r="E8" s="21"/>
       <c r="F8" s="21"/>
-      <c r="G8" s="105" t="e">
+      <c r="G8" s="103" t="e">
         <f>AVERAGE(G43:G50)*5</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H8" s="106"/>
-      <c r="I8" s="107"/>
-      <c r="V8" s="105" t="e">
+      <c r="H8" s="104"/>
+      <c r="I8" s="105"/>
+      <c r="V8" s="103" t="e">
         <f>AVERAGE(K43:K50)*5</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="W8" s="106"/>
-      <c r="X8" s="107"/>
+      <c r="W8" s="104"/>
+      <c r="X8" s="105"/>
     </row>
     <row r="9" spans="2:24" ht="91" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="22"/>
@@ -3663,12 +3663,12 @@
       <c r="D9" s="22"/>
       <c r="E9" s="22"/>
       <c r="F9" s="22"/>
-      <c r="G9" s="108"/>
-      <c r="H9" s="109"/>
-      <c r="I9" s="110"/>
-      <c r="V9" s="108"/>
-      <c r="W9" s="109"/>
-      <c r="X9" s="110"/>
+      <c r="G9" s="106"/>
+      <c r="H9" s="107"/>
+      <c r="I9" s="108"/>
+      <c r="V9" s="106"/>
+      <c r="W9" s="107"/>
+      <c r="X9" s="108"/>
     </row>
     <row r="10" spans="2:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="14"/>
@@ -3676,12 +3676,12 @@
       <c r="D10" s="14"/>
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
-      <c r="G10" s="108"/>
-      <c r="H10" s="109"/>
-      <c r="I10" s="110"/>
-      <c r="V10" s="108"/>
-      <c r="W10" s="109"/>
-      <c r="X10" s="110"/>
+      <c r="G10" s="106"/>
+      <c r="H10" s="107"/>
+      <c r="I10" s="108"/>
+      <c r="V10" s="106"/>
+      <c r="W10" s="107"/>
+      <c r="X10" s="108"/>
     </row>
     <row r="11" spans="2:24" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B11" s="14"/>
@@ -3689,19 +3689,19 @@
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
-      <c r="G11" s="111"/>
-      <c r="H11" s="112"/>
-      <c r="I11" s="113"/>
-      <c r="V11" s="111"/>
-      <c r="W11" s="112"/>
-      <c r="X11" s="113"/>
+      <c r="G11" s="109"/>
+      <c r="H11" s="110"/>
+      <c r="I11" s="111"/>
+      <c r="V11" s="109"/>
+      <c r="W11" s="110"/>
+      <c r="X11" s="111"/>
     </row>
     <row r="12" spans="2:24" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="114"/>
-      <c r="C12" s="114"/>
-      <c r="D12" s="114"/>
-      <c r="E12" s="114"/>
-      <c r="F12" s="114"/>
+      <c r="B12" s="115"/>
+      <c r="C12" s="115"/>
+      <c r="D12" s="115"/>
+      <c r="E12" s="115"/>
+      <c r="F12" s="115"/>
     </row>
     <row r="13" spans="2:24" ht="15" x14ac:dyDescent="0.2">
       <c r="B13" s="15"/>
@@ -3725,11 +3725,11 @@
       <c r="F15" s="14"/>
     </row>
     <row r="16" spans="2:24" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="114"/>
-      <c r="C16" s="114"/>
-      <c r="D16" s="114"/>
-      <c r="E16" s="114"/>
-      <c r="F16" s="114"/>
+      <c r="B16" s="115"/>
+      <c r="C16" s="115"/>
+      <c r="D16" s="115"/>
+      <c r="E16" s="115"/>
+      <c r="F16" s="115"/>
     </row>
     <row r="17" spans="2:6" ht="15" x14ac:dyDescent="0.2">
       <c r="B17" s="15"/>
@@ -3747,7 +3747,7 @@
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B20" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.15">
@@ -3782,48 +3782,48 @@
     </row>
     <row r="35" spans="3:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="41" spans="3:11" x14ac:dyDescent="0.15">
-      <c r="D41" s="115" t="s">
+      <c r="D41" s="116" t="s">
+        <v>200</v>
+      </c>
+      <c r="E41" s="117"/>
+      <c r="F41" s="117"/>
+      <c r="G41" s="118"/>
+      <c r="H41" s="116" t="s">
         <v>201</v>
       </c>
-      <c r="E41" s="116"/>
-      <c r="F41" s="116"/>
-      <c r="G41" s="117"/>
-      <c r="H41" s="115" t="s">
-        <v>202</v>
-      </c>
-      <c r="I41" s="116"/>
-      <c r="J41" s="116"/>
-      <c r="K41" s="117"/>
+      <c r="I41" s="117"/>
+      <c r="J41" s="117"/>
+      <c r="K41" s="118"/>
     </row>
     <row r="42" spans="3:11" x14ac:dyDescent="0.15">
       <c r="D42" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="E42" s="18" t="s">
         <v>197</v>
       </c>
-      <c r="E42" s="18" t="s">
+      <c r="F42" s="18" t="s">
         <v>198</v>
       </c>
-      <c r="F42" s="18" t="s">
+      <c r="G42" s="18" t="s">
         <v>199</v>
       </c>
-      <c r="G42" s="18" t="s">
-        <v>200</v>
-      </c>
       <c r="H42" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="I42" s="18" t="s">
         <v>197</v>
       </c>
-      <c r="I42" s="18" t="s">
+      <c r="J42" s="18" t="s">
         <v>198</v>
       </c>
-      <c r="J42" s="18" t="s">
+      <c r="K42" s="18" t="s">
         <v>199</v>
-      </c>
-      <c r="K42" s="18" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="43" spans="3:11" x14ac:dyDescent="0.15">
       <c r="C43" s="12" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D43" s="10">
         <f>COUNTIFS('Security Requirements - Android'!F5:F15,'Security Requirements - Android'!B79)</f>
@@ -3860,7 +3860,7 @@
     </row>
     <row r="44" spans="3:11" x14ac:dyDescent="0.15">
       <c r="C44" s="12" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D44" s="10">
         <f>COUNTIFS('Security Requirements - Android'!F17:F28,'Security Requirements - Android'!B79)</f>
@@ -3897,7 +3897,7 @@
     </row>
     <row r="45" spans="3:11" x14ac:dyDescent="0.15">
       <c r="C45" s="12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D45" s="10">
         <f>COUNTIFS('Security Requirements - Android'!F30:F35,'Security Requirements - Android'!B79)</f>
@@ -3934,7 +3934,7 @@
     </row>
     <row r="46" spans="3:11" x14ac:dyDescent="0.15">
       <c r="C46" s="12" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D46" s="10">
         <f>COUNTIFS('Security Requirements - Android'!F37:F46,'Security Requirements - Android'!B79)</f>
@@ -3971,7 +3971,7 @@
     </row>
     <row r="47" spans="3:11" x14ac:dyDescent="0.15">
       <c r="C47" s="12" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D47" s="10">
         <f>COUNTIFS('Security Requirements - Android'!F48:F52,'Security Requirements - Android'!B79)</f>
@@ -4008,7 +4008,7 @@
     </row>
     <row r="48" spans="3:11" x14ac:dyDescent="0.15">
       <c r="C48" s="12" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D48" s="10">
         <f>COUNTIFS('Security Requirements - Android'!F54:F63,'Security Requirements - Android'!B79)</f>
@@ -4045,7 +4045,7 @@
     </row>
     <row r="49" spans="3:11" x14ac:dyDescent="0.15">
       <c r="C49" s="12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D49" s="10">
         <f>COUNTIFS('Security Requirements - Android'!F65:F72,'Security Requirements - Android'!B79)</f>
@@ -4082,7 +4082,7 @@
     </row>
     <row r="50" spans="3:11" x14ac:dyDescent="0.15">
       <c r="C50" s="12" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D50" s="10">
         <f>COUNTIFS('Anti-RE - Android'!E4:E19,'Security Requirements - Android'!B79)</f>
@@ -4119,15 +4119,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="D41:G41"/>
+    <mergeCell ref="H41:K41"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="G8:I11"/>
     <mergeCell ref="G6:I6"/>
     <mergeCell ref="V6:X6"/>
     <mergeCell ref="V8:X11"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="D41:G41"/>
-    <mergeCell ref="H41:K41"/>
   </mergeCells>
   <conditionalFormatting sqref="F14">
     <cfRule type="iconSet" priority="3">
@@ -4165,10 +4165,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H85"/>
+  <dimension ref="B1:J85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4183,7 +4183,7 @@
   <sheetData>
     <row r="1" spans="2:8" ht="19" x14ac:dyDescent="0.2">
       <c r="B1" s="119" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C1" s="119"/>
       <c r="D1" s="119"/>
@@ -4215,13 +4215,13 @@
         <v>3</v>
       </c>
       <c r="F3" s="29" t="s">
+        <v>192</v>
+      </c>
+      <c r="G3" s="29" t="s">
+        <v>206</v>
+      </c>
+      <c r="H3" s="30" t="s">
         <v>193</v>
-      </c>
-      <c r="G3" s="29" t="s">
-        <v>207</v>
-      </c>
-      <c r="H3" s="30" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.2">
@@ -4251,10 +4251,10 @@
         <v>7</v>
       </c>
       <c r="F5" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G5" s="52" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H5" s="81"/>
     </row>
@@ -4272,10 +4272,10 @@
         <v>7</v>
       </c>
       <c r="F6" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G6" s="52" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H6" s="81"/>
     </row>
@@ -4293,10 +4293,10 @@
         <v>7</v>
       </c>
       <c r="F7" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G7" s="52" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H7" s="81"/>
     </row>
@@ -4314,10 +4314,10 @@
         <v>7</v>
       </c>
       <c r="F8" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G8" s="52" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H8" s="81"/>
     </row>
@@ -4335,10 +4335,10 @@
         <v>7</v>
       </c>
       <c r="F9" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G9" s="52" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H9" s="81"/>
     </row>
@@ -4354,10 +4354,10 @@
         <v>7</v>
       </c>
       <c r="F10" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G10" s="52" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H10" s="81"/>
     </row>
@@ -4373,10 +4373,10 @@
         <v>7</v>
       </c>
       <c r="F11" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G11" s="52" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H11" s="81"/>
     </row>
@@ -4392,10 +4392,10 @@
         <v>7</v>
       </c>
       <c r="F12" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G12" s="52" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H12" s="81"/>
     </row>
@@ -4411,10 +4411,10 @@
         <v>7</v>
       </c>
       <c r="F13" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G13" s="52" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H13" s="81"/>
     </row>
@@ -4430,10 +4430,10 @@
         <v>7</v>
       </c>
       <c r="F14" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G14" s="52" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H14" s="81"/>
     </row>
@@ -4449,10 +4449,10 @@
         <v>7</v>
       </c>
       <c r="F15" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G15" s="52" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H15" s="81"/>
     </row>
@@ -4483,10 +4483,10 @@
         <v>7</v>
       </c>
       <c r="F17" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G17" s="57" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H17" s="81"/>
     </row>
@@ -4504,10 +4504,10 @@
         <v>7</v>
       </c>
       <c r="F18" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G18" s="57" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H18" s="81"/>
     </row>
@@ -4525,10 +4525,10 @@
         <v>7</v>
       </c>
       <c r="F19" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G19" s="57" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H19" s="81"/>
     </row>
@@ -4546,10 +4546,10 @@
         <v>7</v>
       </c>
       <c r="F20" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G20" s="63" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H20" s="81"/>
     </row>
@@ -4567,10 +4567,10 @@
         <v>7</v>
       </c>
       <c r="F21" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G21" s="63" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H21" s="81"/>
     </row>
@@ -4588,10 +4588,10 @@
         <v>7</v>
       </c>
       <c r="F22" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G22" s="63" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H22" s="81"/>
     </row>
@@ -4600,7 +4600,7 @@
         <v>19</v>
       </c>
       <c r="C23" s="56" t="s">
-        <v>89</v>
+        <v>299</v>
       </c>
       <c r="D23" s="26" t="s">
         <v>7</v>
@@ -4609,10 +4609,10 @@
         <v>7</v>
       </c>
       <c r="F23" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G23" s="63" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H23" s="81"/>
     </row>
@@ -4621,17 +4621,17 @@
         <v>20</v>
       </c>
       <c r="C24" s="56" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D24" s="56"/>
       <c r="E24" s="51" t="s">
         <v>7</v>
       </c>
       <c r="F24" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G24" s="63" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H24" s="81"/>
     </row>
@@ -4640,17 +4640,17 @@
         <v>21</v>
       </c>
       <c r="C25" s="56" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D25" s="56"/>
       <c r="E25" s="51" t="s">
         <v>7</v>
       </c>
       <c r="F25" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G25" s="63" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H25" s="81"/>
     </row>
@@ -4659,17 +4659,17 @@
         <v>81</v>
       </c>
       <c r="C26" s="56" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D26" s="56"/>
       <c r="E26" s="51" t="s">
         <v>7</v>
       </c>
       <c r="F26" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G26" s="63" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H26" s="81"/>
     </row>
@@ -4678,17 +4678,17 @@
         <v>82</v>
       </c>
       <c r="C27" s="56" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D27" s="56"/>
       <c r="E27" s="51" t="s">
         <v>7</v>
       </c>
       <c r="F27" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G27" s="63" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H27" s="81"/>
     </row>
@@ -4697,17 +4697,17 @@
         <v>22</v>
       </c>
       <c r="C28" s="56" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D28" s="56"/>
       <c r="E28" s="51" t="s">
         <v>7</v>
       </c>
       <c r="F28" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G28" s="63" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H28" s="81"/>
     </row>
@@ -4716,7 +4716,7 @@
         <v>23</v>
       </c>
       <c r="C29" s="39" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D29" s="39"/>
       <c r="E29" s="54"/>
@@ -4729,7 +4729,7 @@
         <v>24</v>
       </c>
       <c r="C30" s="56" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D30" s="26" t="s">
         <v>7</v>
@@ -4738,10 +4738,10 @@
         <v>7</v>
       </c>
       <c r="F30" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G30" s="63" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="H30" s="81"/>
     </row>
@@ -4750,7 +4750,7 @@
         <v>25</v>
       </c>
       <c r="C31" s="56" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D31" s="26" t="s">
         <v>7</v>
@@ -4759,10 +4759,10 @@
         <v>7</v>
       </c>
       <c r="F31" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G31" s="63" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H31" s="81"/>
     </row>
@@ -4771,7 +4771,7 @@
         <v>26</v>
       </c>
       <c r="C32" s="56" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D32" s="26" t="s">
         <v>7</v>
@@ -4780,19 +4780,19 @@
         <v>7</v>
       </c>
       <c r="F32" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G32" s="63" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H32" s="81"/>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B33" s="55" t="s">
         <v>27</v>
       </c>
       <c r="C33" s="56" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D33" s="26" t="s">
         <v>7</v>
@@ -4801,19 +4801,19 @@
         <v>7</v>
       </c>
       <c r="F33" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G33" s="63" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H33" s="81"/>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B34" s="55" t="s">
         <v>28</v>
       </c>
       <c r="C34" s="56" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D34" s="26" t="s">
         <v>7</v>
@@ -4822,19 +4822,19 @@
         <v>7</v>
       </c>
       <c r="F34" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G34" s="63" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H34" s="81"/>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B35" s="55" t="s">
         <v>29</v>
       </c>
       <c r="C35" s="56" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D35" s="26" t="s">
         <v>7</v>
@@ -4843,19 +4843,19 @@
         <v>7</v>
       </c>
       <c r="F35" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G35" s="63" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="H35" s="81"/>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B36" s="38" t="s">
         <v>30</v>
       </c>
       <c r="C36" s="39" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D36" s="39"/>
       <c r="E36" s="54"/>
@@ -4863,55 +4863,55 @@
       <c r="G36" s="39"/>
       <c r="H36" s="40"/>
     </row>
-    <row r="37" spans="2:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:10" ht="30" x14ac:dyDescent="0.2">
       <c r="B37" s="55" t="s">
         <v>31</v>
       </c>
       <c r="C37" s="56" t="s">
+        <v>104</v>
+      </c>
+      <c r="D37" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F37" s="37" t="s">
+        <v>164</v>
+      </c>
+      <c r="G37" s="63" t="s">
+        <v>231</v>
+      </c>
+      <c r="H37" s="81"/>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B38" s="55" t="s">
+        <v>100</v>
+      </c>
+      <c r="C38" s="56" t="s">
         <v>105</v>
       </c>
-      <c r="D37" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E37" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F37" s="37" t="s">
-        <v>165</v>
-      </c>
-      <c r="G37" s="63" t="s">
+      <c r="D38" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F38" s="37" t="s">
+        <v>164</v>
+      </c>
+      <c r="G38" s="63" t="s">
         <v>232</v>
       </c>
-      <c r="H37" s="81"/>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B38" s="55" t="s">
+      <c r="H38" s="81"/>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B39" s="55" t="s">
         <v>101</v>
       </c>
-      <c r="C38" s="56" t="s">
+      <c r="C39" s="56" t="s">
         <v>106</v>
       </c>
-      <c r="D38" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E38" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F38" s="37" t="s">
-        <v>165</v>
-      </c>
-      <c r="G38" s="63" t="s">
-        <v>233</v>
-      </c>
-      <c r="H38" s="81"/>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B39" s="55" t="s">
-        <v>102</v>
-      </c>
-      <c r="C39" s="56" t="s">
-        <v>107</v>
-      </c>
       <c r="D39" s="26" t="s">
         <v>7</v>
       </c>
@@ -4919,19 +4919,20 @@
         <v>7</v>
       </c>
       <c r="F39" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G39" s="63" t="s">
         <v>234</v>
       </c>
       <c r="H39" s="81"/>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J39" s="63"/>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B40" s="55" t="s">
         <v>32</v>
       </c>
       <c r="C40" s="56" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D40" s="26" t="s">
         <v>7</v>
@@ -4940,135 +4941,135 @@
         <v>7</v>
       </c>
       <c r="F40" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G40" s="63" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="H40" s="81"/>
     </row>
-    <row r="41" spans="2:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:10" ht="30" x14ac:dyDescent="0.2">
       <c r="B41" s="55" t="s">
         <v>33</v>
       </c>
       <c r="C41" s="56" t="s">
+        <v>108</v>
+      </c>
+      <c r="D41" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F41" s="37" t="s">
+        <v>164</v>
+      </c>
+      <c r="G41" s="63" t="s">
+        <v>235</v>
+      </c>
+      <c r="H41" s="81"/>
+    </row>
+    <row r="42" spans="2:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="B42" s="55" t="s">
+        <v>102</v>
+      </c>
+      <c r="C42" s="56" t="s">
         <v>109</v>
-      </c>
-      <c r="D41" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E41" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F41" s="37" t="s">
-        <v>165</v>
-      </c>
-      <c r="G41" s="63" t="s">
-        <v>236</v>
-      </c>
-      <c r="H41" s="81"/>
-    </row>
-    <row r="42" spans="2:8" ht="30" x14ac:dyDescent="0.2">
-      <c r="B42" s="55" t="s">
-        <v>103</v>
-      </c>
-      <c r="C42" s="56" t="s">
-        <v>110</v>
       </c>
       <c r="D42" s="56"/>
       <c r="E42" s="51" t="s">
         <v>7</v>
       </c>
       <c r="F42" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G42" s="63" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H42" s="81"/>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B43" s="55" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C43" s="56" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D43" s="56"/>
       <c r="E43" s="51" t="s">
         <v>7</v>
       </c>
       <c r="F43" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G43" s="63" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H43" s="81"/>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B44" s="55" t="s">
         <v>34</v>
       </c>
       <c r="C44" s="56" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D44" s="56"/>
       <c r="E44" s="51" t="s">
         <v>7</v>
       </c>
       <c r="F44" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G44" s="63" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H44" s="81"/>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B45" s="55" t="s">
         <v>35</v>
       </c>
       <c r="C45" s="56" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D45" s="56"/>
       <c r="E45" s="51" t="s">
         <v>7</v>
       </c>
       <c r="F45" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G45" s="63" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H45" s="81"/>
     </row>
-    <row r="46" spans="2:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:10" ht="30" x14ac:dyDescent="0.2">
       <c r="B46" s="55" t="s">
         <v>36</v>
       </c>
       <c r="C46" s="56" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D46" s="56"/>
       <c r="E46" s="51" t="s">
         <v>7</v>
       </c>
       <c r="F46" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G46" s="63" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H46" s="81"/>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B47" s="38" t="s">
         <v>37</v>
       </c>
       <c r="C47" s="39" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D47" s="39"/>
       <c r="E47" s="54"/>
@@ -5076,12 +5077,12 @@
       <c r="G47" s="39"/>
       <c r="H47" s="40"/>
     </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B48" s="55" t="s">
         <v>38</v>
       </c>
       <c r="C48" s="56" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D48" s="26" t="s">
         <v>7</v>
@@ -5090,19 +5091,19 @@
         <v>7</v>
       </c>
       <c r="F48" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G48" s="63" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H48" s="81"/>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B49" s="55" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C49" s="56" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D49" s="26" t="s">
         <v>7</v>
@@ -5111,10 +5112,10 @@
         <v>7</v>
       </c>
       <c r="F49" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G49" s="63" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H49" s="81"/>
     </row>
@@ -5123,7 +5124,7 @@
         <v>39</v>
       </c>
       <c r="C50" s="56" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D50" s="26" t="s">
         <v>7</v>
@@ -5132,29 +5133,29 @@
         <v>7</v>
       </c>
       <c r="F50" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G50" s="63" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H50" s="81"/>
     </row>
     <row r="51" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B51" s="55" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C51" s="56" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D51" s="56"/>
       <c r="E51" s="51" t="s">
         <v>7</v>
       </c>
       <c r="F51" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G51" s="63" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="H51" s="81"/>
     </row>
@@ -5163,17 +5164,17 @@
         <v>40</v>
       </c>
       <c r="C52" s="56" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D52" s="56"/>
       <c r="E52" s="51" t="s">
         <v>7</v>
       </c>
       <c r="F52" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G52" s="63" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H52" s="81"/>
     </row>
@@ -5182,7 +5183,7 @@
         <v>41</v>
       </c>
       <c r="C53" s="39" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D53" s="39"/>
       <c r="E53" s="54"/>
@@ -5192,10 +5193,10 @@
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B54" s="55" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C54" s="56" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D54" s="26" t="s">
         <v>7</v>
@@ -5204,19 +5205,19 @@
         <v>7</v>
       </c>
       <c r="F54" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G54" s="63" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H54" s="81"/>
     </row>
     <row r="55" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B55" s="55" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C55" s="56" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D55" s="26" t="s">
         <v>7</v>
@@ -5225,19 +5226,19 @@
         <v>7</v>
       </c>
       <c r="F55" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G55" s="63" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H55" s="81"/>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B56" s="55" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C56" s="56" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D56" s="26" t="s">
         <v>7</v>
@@ -5246,19 +5247,19 @@
         <v>7</v>
       </c>
       <c r="F56" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G56" s="63" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H56" s="81"/>
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B57" s="55" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C57" s="56" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D57" s="26" t="s">
         <v>7</v>
@@ -5267,19 +5268,19 @@
         <v>7</v>
       </c>
       <c r="F57" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G57" s="63" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H57" s="81"/>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B58" s="55" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C58" s="56" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D58" s="26" t="s">
         <v>7</v>
@@ -5288,19 +5289,19 @@
         <v>7</v>
       </c>
       <c r="F58" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G58" s="63" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H58" s="81"/>
     </row>
     <row r="59" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B59" s="55" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C59" s="56" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D59" s="26" t="s">
         <v>7</v>
@@ -5309,19 +5310,19 @@
         <v>7</v>
       </c>
       <c r="F59" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G59" s="63" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H59" s="81"/>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B60" s="55" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C60" s="56" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D60" s="26" t="s">
         <v>7</v>
@@ -5330,19 +5331,19 @@
         <v>7</v>
       </c>
       <c r="F60" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G60" s="63" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H60" s="81"/>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B61" s="55" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C61" s="56" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D61" s="26" t="s">
         <v>7</v>
@@ -5351,19 +5352,19 @@
         <v>7</v>
       </c>
       <c r="F61" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G61" s="63" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="H61" s="81"/>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B62" s="55" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C62" s="56" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D62" s="26" t="s">
         <v>7</v>
@@ -5372,29 +5373,29 @@
         <v>7</v>
       </c>
       <c r="F62" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G62" s="63" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H62" s="81"/>
     </row>
     <row r="63" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B63" s="58" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C63" s="56" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D63" s="56"/>
       <c r="E63" s="51" t="s">
         <v>7</v>
       </c>
       <c r="F63" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G63" s="63" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H63" s="81"/>
     </row>
@@ -5403,7 +5404,7 @@
         <v>42</v>
       </c>
       <c r="C64" s="39" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D64" s="39"/>
       <c r="E64" s="54"/>
@@ -5413,10 +5414,10 @@
     </row>
     <row r="65" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B65" s="55" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C65" s="56" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D65" s="26" t="s">
         <v>7</v>
@@ -5425,10 +5426,10 @@
         <v>7</v>
       </c>
       <c r="F65" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G65" s="63" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H65" s="81"/>
     </row>
@@ -5437,7 +5438,7 @@
         <v>43</v>
       </c>
       <c r="C66" s="56" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D66" s="26" t="s">
         <v>7</v>
@@ -5446,19 +5447,19 @@
         <v>7</v>
       </c>
       <c r="F66" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G66" s="64" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H66" s="81"/>
     </row>
     <row r="67" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B67" s="55" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C67" s="56" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D67" s="26" t="s">
         <v>7</v>
@@ -5467,19 +5468,19 @@
         <v>7</v>
       </c>
       <c r="F67" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G67" s="63" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H67" s="81"/>
     </row>
     <row r="68" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B68" s="55" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C68" s="56" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D68" s="26" t="s">
         <v>7</v>
@@ -5488,19 +5489,19 @@
         <v>7</v>
       </c>
       <c r="F68" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G68" s="63" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H68" s="81"/>
     </row>
     <row r="69" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B69" s="55" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C69" s="56" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D69" s="26" t="s">
         <v>7</v>
@@ -5509,10 +5510,10 @@
         <v>7</v>
       </c>
       <c r="F69" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G69" s="65" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H69" s="81"/>
     </row>
@@ -5530,10 +5531,10 @@
         <v>7</v>
       </c>
       <c r="F70" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G70" s="63" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H70" s="81"/>
     </row>
@@ -5542,7 +5543,7 @@
         <v>45</v>
       </c>
       <c r="C71" s="56" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D71" s="26" t="s">
         <v>7</v>
@@ -5551,10 +5552,10 @@
         <v>7</v>
       </c>
       <c r="F71" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G71" s="63" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="H71" s="81"/>
     </row>
@@ -5563,7 +5564,7 @@
         <v>46</v>
       </c>
       <c r="C72" s="56" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D72" s="26" t="s">
         <v>7</v>
@@ -5572,10 +5573,10 @@
         <v>7</v>
       </c>
       <c r="F72" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G72" s="63" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H72" s="81"/>
     </row>
@@ -5617,7 +5618,7 @@
     </row>
     <row r="77" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B77" s="46" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C77" s="47"/>
       <c r="D77" s="45"/>
@@ -5628,10 +5629,10 @@
     </row>
     <row r="78" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B78" s="48" t="s">
+        <v>161</v>
+      </c>
+      <c r="C78" s="48" t="s">
         <v>162</v>
-      </c>
-      <c r="C78" s="48" t="s">
-        <v>163</v>
       </c>
       <c r="D78" s="45"/>
       <c r="E78" s="45"/>
@@ -5641,10 +5642,10 @@
     </row>
     <row r="79" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B79" s="49" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C79" s="49" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D79" s="45"/>
       <c r="E79" s="45"/>
@@ -5654,10 +5655,10 @@
     </row>
     <row r="80" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B80" s="49" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C80" s="49" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D80" s="45"/>
       <c r="E80" s="45"/>
@@ -5667,10 +5668,10 @@
     </row>
     <row r="81" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B81" s="49" t="s">
+        <v>164</v>
+      </c>
+      <c r="C81" s="49" t="s">
         <v>165</v>
-      </c>
-      <c r="C81" s="49" t="s">
-        <v>166</v>
       </c>
       <c r="D81" s="45"/>
       <c r="E81" s="45"/>
@@ -5744,40 +5745,40 @@
     <hyperlink ref="G33" r:id="rId15" location="testing-for-insecure-andor-deprecated-cryptographic-algorithms"/>
     <hyperlink ref="G34" r:id="rId16" location="testing-random-number-generation"/>
     <hyperlink ref="G35" r:id="rId17" location="verifying-key-management"/>
-    <hyperlink ref="G40" r:id="rId18" location="testing-the-logout-functionality"/>
-    <hyperlink ref="G41" r:id="rId19" location="testing-excessive-login-attempts"/>
-    <hyperlink ref="G42" r:id="rId20" location="testing-biometric-authentication"/>
-    <hyperlink ref="G43" r:id="rId21" location="testing-the-session-timeout"/>
-    <hyperlink ref="G44" r:id="rId22" location="testing-2-factor-authentication"/>
-    <hyperlink ref="G45" r:id="rId23" location="testing-step-up-authentication"/>
-    <hyperlink ref="G46" r:id="rId24" location="testing-user-device-management"/>
-    <hyperlink ref="G48" r:id="rId25" location="testing-for-unencrypted-sensitive-data-on-the-network"/>
-    <hyperlink ref="G49" r:id="rId26" location="verifying-the-tls-settings"/>
-    <hyperlink ref="G50" r:id="rId27" location="testing-endpoint-identify-verification"/>
-    <hyperlink ref="G51" r:id="rId28" location="testing-custom-certificate-stores-and-ssl-pinning"/>
-    <hyperlink ref="G52" r:id="rId29" location="verifying-that-critical-operations-use-secure-communication-channels"/>
-    <hyperlink ref="G54" r:id="rId30" location="testing-app-permissions"/>
-    <hyperlink ref="G55" r:id="rId31" location="testing-input-validation-and-sanitization"/>
-    <hyperlink ref="G56" r:id="rId32" location="testing-custom-url-schemes"/>
-    <hyperlink ref="G57" r:id="rId33" location="testing-for-sensitive-functionality-exposure-through-ipc"/>
-    <hyperlink ref="G58" r:id="rId34" location="testing-javascript-execution-in-webviews"/>
-    <hyperlink ref="G59" r:id="rId35" location="testing-webview-protocol-handlers"/>
-    <hyperlink ref="G60" r:id="rId36" location="testing-for-local-file-inclusion-in-webviews"/>
-    <hyperlink ref="G61" r:id="rId37" location="testing-whether-java-objects-are-exposed-through-webviews"/>
-    <hyperlink ref="G62" r:id="rId38" location="testing-object-de-serialization"/>
-    <hyperlink ref="G63" r:id="rId39" location="testing-root-detection"/>
-    <hyperlink ref="G65" r:id="rId40" location="verifying-that-the-app-is-properly-signed"/>
-    <hyperlink ref="G66" r:id="rId41" location="testing-if-the-app-is-debuggable"/>
-    <hyperlink ref="G67" r:id="rId42" location="testing-for-debugging-symbols"/>
-    <hyperlink ref="G68" r:id="rId43" location="testing-for-debugging-code-and-verbose-error-logging"/>
-    <hyperlink ref="G69" r:id="rId44" location="testing-exception-handling"/>
-    <hyperlink ref="G70" r:id="rId45" location="testing-exception-handling"/>
-    <hyperlink ref="G71" r:id="rId46" location="testing-for-memory-management-bugs"/>
-    <hyperlink ref="G72" r:id="rId47" location="verifying-compiler-settings"/>
-    <hyperlink ref="G37" r:id="rId48" location="verifying-that-users-are-properly-authenticated"/>
-    <hyperlink ref="G39" r:id="rId49" location="testing-the-password-policy"/>
-    <hyperlink ref="G38" r:id="rId50" location="testing-session-management"/>
-    <hyperlink ref="G23" r:id="rId51"/>
+    <hyperlink ref="G41" r:id="rId18" location="testing-excessive-login-attempts"/>
+    <hyperlink ref="G42" r:id="rId19" location="testing-biometric-authentication"/>
+    <hyperlink ref="G43" r:id="rId20" location="testing-the-session-timeout"/>
+    <hyperlink ref="G44" r:id="rId21" location="testing-2-factor-authentication"/>
+    <hyperlink ref="G45" r:id="rId22" location="testing-step-up-authentication"/>
+    <hyperlink ref="G46" r:id="rId23" location="testing-user-device-management"/>
+    <hyperlink ref="G48" r:id="rId24" location="testing-for-unencrypted-sensitive-data-on-the-network"/>
+    <hyperlink ref="G49" r:id="rId25" location="verifying-the-tls-settings"/>
+    <hyperlink ref="G50" r:id="rId26" location="testing-endpoint-identify-verification"/>
+    <hyperlink ref="G51" r:id="rId27" location="testing-custom-certificate-stores-and-ssl-pinning"/>
+    <hyperlink ref="G52" r:id="rId28" location="verifying-that-critical-operations-use-secure-communication-channels"/>
+    <hyperlink ref="G54" r:id="rId29" location="testing-app-permissions"/>
+    <hyperlink ref="G55" r:id="rId30" location="testing-input-validation-and-sanitization"/>
+    <hyperlink ref="G56" r:id="rId31" location="testing-custom-url-schemes"/>
+    <hyperlink ref="G57" r:id="rId32" location="testing-for-sensitive-functionality-exposure-through-ipc"/>
+    <hyperlink ref="G58" r:id="rId33" location="testing-javascript-execution-in-webviews"/>
+    <hyperlink ref="G59" r:id="rId34" location="testing-webview-protocol-handlers"/>
+    <hyperlink ref="G60" r:id="rId35" location="testing-for-local-file-inclusion-in-webviews"/>
+    <hyperlink ref="G61" r:id="rId36" location="testing-whether-java-objects-are-exposed-through-webviews"/>
+    <hyperlink ref="G62" r:id="rId37" location="testing-object-de-serialization"/>
+    <hyperlink ref="G63" r:id="rId38" location="testing-root-detection"/>
+    <hyperlink ref="G65" r:id="rId39" location="verifying-that-the-app-is-properly-signed"/>
+    <hyperlink ref="G66" r:id="rId40" location="testing-if-the-app-is-debuggable"/>
+    <hyperlink ref="G67" r:id="rId41" location="testing-for-debugging-symbols"/>
+    <hyperlink ref="G68" r:id="rId42" location="testing-for-debugging-code-and-verbose-error-logging"/>
+    <hyperlink ref="G69" r:id="rId43" location="testing-exception-handling"/>
+    <hyperlink ref="G70" r:id="rId44" location="testing-exception-handling"/>
+    <hyperlink ref="G71" r:id="rId45" location="testing-for-memory-management-bugs"/>
+    <hyperlink ref="G72" r:id="rId46" location="verifying-compiler-settings"/>
+    <hyperlink ref="G37" r:id="rId47" location="verifying-that-users-are-properly-authenticated"/>
+    <hyperlink ref="G38" r:id="rId48" location="testing-session-management"/>
+    <hyperlink ref="G23" r:id="rId49"/>
+    <hyperlink ref="G39" r:id="rId50" location="testing-the-logout-functionality"/>
+    <hyperlink ref="G40" r:id="rId51" location="testing-the-password-policy"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -5803,7 +5804,7 @@
   <sheetData>
     <row r="1" spans="2:7" ht="19" x14ac:dyDescent="0.25">
       <c r="B1" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C1" s="24"/>
       <c r="D1" s="24"/>
@@ -5828,13 +5829,13 @@
         <v>61</v>
       </c>
       <c r="E3" s="29" t="s">
+        <v>192</v>
+      </c>
+      <c r="F3" s="29" t="s">
+        <v>206</v>
+      </c>
+      <c r="G3" s="30" t="s">
         <v>193</v>
-      </c>
-      <c r="F3" s="29" t="s">
-        <v>207</v>
-      </c>
-      <c r="G3" s="30" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.2">
@@ -5858,10 +5859,10 @@
         <v>7</v>
       </c>
       <c r="E5" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F5" s="62" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G5" s="81"/>
     </row>
@@ -5876,10 +5877,10 @@
         <v>7</v>
       </c>
       <c r="E6" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F6" s="62" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G6" s="81"/>
     </row>
@@ -5894,10 +5895,10 @@
         <v>7</v>
       </c>
       <c r="E7" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F7" s="62" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G7" s="81"/>
     </row>
@@ -5912,10 +5913,10 @@
         <v>7</v>
       </c>
       <c r="E8" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F8" s="62" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G8" s="81"/>
     </row>
@@ -5930,10 +5931,10 @@
         <v>7</v>
       </c>
       <c r="E9" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F9" s="62" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G9" s="81"/>
     </row>
@@ -5948,10 +5949,10 @@
         <v>7</v>
       </c>
       <c r="E10" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F10" s="62" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G10" s="81"/>
     </row>
@@ -5966,10 +5967,10 @@
         <v>7</v>
       </c>
       <c r="E11" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F11" s="62" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G11" s="81"/>
     </row>
@@ -5984,10 +5985,10 @@
         <v>7</v>
       </c>
       <c r="E12" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F12" s="62" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G12" s="81"/>
     </row>
@@ -6002,10 +6003,10 @@
         <v>7</v>
       </c>
       <c r="E13" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F13" s="62" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G13" s="81"/>
     </row>
@@ -6021,7 +6022,7 @@
     </row>
     <row r="15" spans="2:7" ht="30" x14ac:dyDescent="0.2">
       <c r="B15" s="78" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C15" s="36" t="s">
         <v>74</v>
@@ -6030,10 +6031,10 @@
         <v>7</v>
       </c>
       <c r="E15" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F15" s="62" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G15" s="81"/>
     </row>
@@ -6058,10 +6059,10 @@
         <v>7</v>
       </c>
       <c r="E17" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F17" s="62" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G17" s="81"/>
     </row>
@@ -6076,10 +6077,10 @@
         <v>7</v>
       </c>
       <c r="E18" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F18" s="62" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G18" s="81"/>
     </row>
@@ -6094,10 +6095,10 @@
         <v>7</v>
       </c>
       <c r="E19" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F19" s="62" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G19" s="81"/>
     </row>
@@ -6127,7 +6128,7 @@
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B23" s="46" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C23" s="47"/>
       <c r="D23" s="45"/>
@@ -6137,10 +6138,10 @@
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B24" s="48" t="s">
+        <v>161</v>
+      </c>
+      <c r="C24" s="48" t="s">
         <v>162</v>
-      </c>
-      <c r="C24" s="48" t="s">
-        <v>163</v>
       </c>
       <c r="D24" s="45"/>
       <c r="E24" s="45"/>
@@ -6149,10 +6150,10 @@
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B25" s="49" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C25" s="49" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D25" s="45"/>
       <c r="E25" s="45"/>
@@ -6161,10 +6162,10 @@
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B26" s="49" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C26" s="49" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D26" s="45"/>
       <c r="E26" s="45"/>
@@ -6173,10 +6174,10 @@
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B27" s="49" t="s">
+        <v>164</v>
+      </c>
+      <c r="C27" s="49" t="s">
         <v>165</v>
-      </c>
-      <c r="C27" s="49" t="s">
-        <v>166</v>
       </c>
       <c r="D27" s="45"/>
       <c r="E27" s="45"/>
@@ -6235,10 +6236,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H85"/>
+  <dimension ref="B1:J85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6246,14 +6247,14 @@
     <col min="1" max="1" width="1.83203125" customWidth="1"/>
     <col min="2" max="2" width="8" customWidth="1"/>
     <col min="3" max="3" width="122.83203125" customWidth="1"/>
-    <col min="7" max="7" width="34.83203125" customWidth="1"/>
+    <col min="7" max="7" width="60" customWidth="1"/>
     <col min="8" max="8" width="30.83203125" customWidth="1"/>
     <col min="10" max="11" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="19" x14ac:dyDescent="0.25">
       <c r="B1" s="59" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C1" s="50"/>
       <c r="D1" s="50"/>
@@ -6285,13 +6286,13 @@
         <v>3</v>
       </c>
       <c r="F3" s="29" t="s">
+        <v>192</v>
+      </c>
+      <c r="G3" s="29" t="s">
+        <v>206</v>
+      </c>
+      <c r="H3" s="30" t="s">
         <v>193</v>
-      </c>
-      <c r="G3" s="29" t="s">
-        <v>207</v>
-      </c>
-      <c r="H3" s="30" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.2">
@@ -6321,7 +6322,7 @@
         <v>7</v>
       </c>
       <c r="F5" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G5" s="60"/>
       <c r="H5" s="81"/>
@@ -6340,7 +6341,7 @@
         <v>7</v>
       </c>
       <c r="F6" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G6" s="60"/>
       <c r="H6" s="81"/>
@@ -6359,7 +6360,7 @@
         <v>7</v>
       </c>
       <c r="F7" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G7" s="60"/>
       <c r="H7" s="81"/>
@@ -6378,7 +6379,7 @@
         <v>7</v>
       </c>
       <c r="F8" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G8" s="60"/>
       <c r="H8" s="81"/>
@@ -6397,7 +6398,7 @@
         <v>7</v>
       </c>
       <c r="F9" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G9" s="60"/>
       <c r="H9" s="81"/>
@@ -6414,7 +6415,7 @@
         <v>7</v>
       </c>
       <c r="F10" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G10" s="60"/>
       <c r="H10" s="81"/>
@@ -6431,7 +6432,7 @@
         <v>7</v>
       </c>
       <c r="F11" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G11" s="60"/>
       <c r="H11" s="81"/>
@@ -6448,7 +6449,7 @@
         <v>7</v>
       </c>
       <c r="F12" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G12" s="60"/>
       <c r="H12" s="81"/>
@@ -6465,7 +6466,7 @@
         <v>7</v>
       </c>
       <c r="F13" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G13" s="60"/>
       <c r="H13" s="81"/>
@@ -6482,7 +6483,7 @@
         <v>7</v>
       </c>
       <c r="F14" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G14" s="60"/>
       <c r="H14" s="81"/>
@@ -6499,7 +6500,7 @@
         <v>7</v>
       </c>
       <c r="F15" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G15" s="60"/>
       <c r="H15" s="81"/>
@@ -6531,10 +6532,10 @@
         <v>7</v>
       </c>
       <c r="F17" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G17" s="63" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H17" s="81"/>
     </row>
@@ -6552,14 +6553,14 @@
         <v>7</v>
       </c>
       <c r="F18" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G18" s="63" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H18" s="81"/>
     </row>
-    <row r="19" spans="2:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B19" s="55" t="s">
         <v>79</v>
       </c>
@@ -6573,14 +6574,14 @@
         <v>7</v>
       </c>
       <c r="F19" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G19" s="63" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H19" s="81"/>
     </row>
-    <row r="20" spans="2:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B20" s="55" t="s">
         <v>17</v>
       </c>
@@ -6594,10 +6595,10 @@
         <v>7</v>
       </c>
       <c r="F20" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G20" s="63" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H20" s="81"/>
     </row>
@@ -6615,14 +6616,14 @@
         <v>7</v>
       </c>
       <c r="F21" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G21" s="63" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H21" s="81"/>
     </row>
-    <row r="22" spans="2:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B22" s="55" t="s">
         <v>18</v>
       </c>
@@ -6636,19 +6637,19 @@
         <v>7</v>
       </c>
       <c r="F22" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G22" s="63" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H22" s="81"/>
     </row>
-    <row r="23" spans="2:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B23" s="55" t="s">
         <v>19</v>
       </c>
       <c r="C23" s="56" t="s">
-        <v>89</v>
+        <v>299</v>
       </c>
       <c r="D23" s="26" t="s">
         <v>7</v>
@@ -6657,10 +6658,10 @@
         <v>7</v>
       </c>
       <c r="F23" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G23" s="63" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H23" s="81"/>
     </row>
@@ -6669,36 +6670,36 @@
         <v>20</v>
       </c>
       <c r="C24" s="56" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D24" s="56"/>
       <c r="E24" s="51" t="s">
         <v>7</v>
       </c>
       <c r="F24" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G24" s="63" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H24" s="81"/>
     </row>
-    <row r="25" spans="2:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B25" s="55" t="s">
         <v>21</v>
       </c>
       <c r="C25" s="56" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D25" s="56"/>
       <c r="E25" s="51" t="s">
         <v>7</v>
       </c>
       <c r="F25" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G25" s="63" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H25" s="81"/>
     </row>
@@ -6707,17 +6708,17 @@
         <v>81</v>
       </c>
       <c r="C26" s="56" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D26" s="56"/>
       <c r="E26" s="51" t="s">
         <v>7</v>
       </c>
       <c r="F26" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G26" s="63" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H26" s="81"/>
     </row>
@@ -6726,17 +6727,17 @@
         <v>82</v>
       </c>
       <c r="C27" s="56" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D27" s="56"/>
       <c r="E27" s="51" t="s">
         <v>7</v>
       </c>
       <c r="F27" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G27" s="63" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H27" s="81"/>
     </row>
@@ -6745,17 +6746,17 @@
         <v>22</v>
       </c>
       <c r="C28" s="56" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D28" s="56"/>
       <c r="E28" s="51" t="s">
         <v>7</v>
       </c>
       <c r="F28" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G28" s="63" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H28" s="81"/>
     </row>
@@ -6764,7 +6765,7 @@
         <v>23</v>
       </c>
       <c r="C29" s="39" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D29" s="39"/>
       <c r="E29" s="54"/>
@@ -6777,7 +6778,7 @@
         <v>24</v>
       </c>
       <c r="C30" s="56" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D30" s="26" t="s">
         <v>7</v>
@@ -6786,19 +6787,19 @@
         <v>7</v>
       </c>
       <c r="F30" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G30" s="63" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="H30" s="81"/>
     </row>
-    <row r="31" spans="2:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B31" s="55" t="s">
         <v>25</v>
       </c>
       <c r="C31" s="56" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D31" s="26" t="s">
         <v>7</v>
@@ -6807,10 +6808,10 @@
         <v>7</v>
       </c>
       <c r="F31" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G31" s="63" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H31" s="81"/>
     </row>
@@ -6819,7 +6820,7 @@
         <v>26</v>
       </c>
       <c r="C32" s="56" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D32" s="26" t="s">
         <v>7</v>
@@ -6828,19 +6829,19 @@
         <v>7</v>
       </c>
       <c r="F32" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G32" s="63" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H32" s="81"/>
     </row>
-    <row r="33" spans="2:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B33" s="55" t="s">
         <v>27</v>
       </c>
       <c r="C33" s="56" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D33" s="26" t="s">
         <v>7</v>
@@ -6849,19 +6850,19 @@
         <v>7</v>
       </c>
       <c r="F33" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G33" s="63" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H33" s="81"/>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B34" s="55" t="s">
         <v>28</v>
       </c>
       <c r="C34" s="56" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D34" s="26" t="s">
         <v>7</v>
@@ -6870,19 +6871,19 @@
         <v>7</v>
       </c>
       <c r="F34" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G34" s="63" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H34" s="81"/>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B35" s="55" t="s">
         <v>29</v>
       </c>
       <c r="C35" s="56" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D35" s="26" t="s">
         <v>7</v>
@@ -6891,19 +6892,19 @@
         <v>7</v>
       </c>
       <c r="F35" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G35" s="63" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="H35" s="81"/>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B36" s="38" t="s">
         <v>30</v>
       </c>
       <c r="C36" s="39" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D36" s="39"/>
       <c r="E36" s="54"/>
@@ -6911,55 +6912,55 @@
       <c r="G36" s="39"/>
       <c r="H36" s="40"/>
     </row>
-    <row r="37" spans="2:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:10" ht="30" x14ac:dyDescent="0.2">
       <c r="B37" s="55" t="s">
         <v>31</v>
       </c>
       <c r="C37" s="56" t="s">
+        <v>104</v>
+      </c>
+      <c r="D37" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F37" s="37" t="s">
+        <v>164</v>
+      </c>
+      <c r="G37" s="63" t="s">
+        <v>231</v>
+      </c>
+      <c r="H37" s="81"/>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B38" s="55" t="s">
+        <v>100</v>
+      </c>
+      <c r="C38" s="56" t="s">
         <v>105</v>
       </c>
-      <c r="D37" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E37" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F37" s="37" t="s">
-        <v>165</v>
-      </c>
-      <c r="G37" s="63" t="s">
+      <c r="D38" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F38" s="37" t="s">
+        <v>164</v>
+      </c>
+      <c r="G38" s="63" t="s">
         <v>232</v>
       </c>
-      <c r="H37" s="81"/>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B38" s="55" t="s">
+      <c r="H38" s="81"/>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B39" s="55" t="s">
         <v>101</v>
       </c>
-      <c r="C38" s="56" t="s">
+      <c r="C39" s="56" t="s">
         <v>106</v>
       </c>
-      <c r="D38" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E38" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F38" s="37" t="s">
-        <v>165</v>
-      </c>
-      <c r="G38" s="63" t="s">
-        <v>233</v>
-      </c>
-      <c r="H38" s="81"/>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B39" s="55" t="s">
-        <v>102</v>
-      </c>
-      <c r="C39" s="56" t="s">
-        <v>107</v>
-      </c>
       <c r="D39" s="26" t="s">
         <v>7</v>
       </c>
@@ -6967,19 +6968,19 @@
         <v>7</v>
       </c>
       <c r="F39" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G39" s="63" t="s">
         <v>234</v>
       </c>
       <c r="H39" s="81"/>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B40" s="55" t="s">
         <v>32</v>
       </c>
       <c r="C40" s="56" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D40" s="26" t="s">
         <v>7</v>
@@ -6988,135 +6989,136 @@
         <v>7</v>
       </c>
       <c r="F40" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G40" s="63" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="H40" s="81"/>
-    </row>
-    <row r="41" spans="2:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="J40" s="63"/>
+    </row>
+    <row r="41" spans="2:10" ht="30" x14ac:dyDescent="0.2">
       <c r="B41" s="55" t="s">
         <v>33</v>
       </c>
       <c r="C41" s="56" t="s">
+        <v>108</v>
+      </c>
+      <c r="D41" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F41" s="37" t="s">
+        <v>164</v>
+      </c>
+      <c r="G41" s="63" t="s">
+        <v>235</v>
+      </c>
+      <c r="H41" s="81"/>
+    </row>
+    <row r="42" spans="2:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="B42" s="55" t="s">
+        <v>102</v>
+      </c>
+      <c r="C42" s="56" t="s">
         <v>109</v>
-      </c>
-      <c r="D41" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E41" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F41" s="37" t="s">
-        <v>165</v>
-      </c>
-      <c r="G41" s="63" t="s">
-        <v>236</v>
-      </c>
-      <c r="H41" s="81"/>
-    </row>
-    <row r="42" spans="2:8" ht="30" x14ac:dyDescent="0.2">
-      <c r="B42" s="55" t="s">
-        <v>103</v>
-      </c>
-      <c r="C42" s="56" t="s">
-        <v>110</v>
       </c>
       <c r="D42" s="56"/>
       <c r="E42" s="51" t="s">
         <v>7</v>
       </c>
       <c r="F42" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G42" s="63" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H42" s="81"/>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B43" s="55" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C43" s="56" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D43" s="56"/>
       <c r="E43" s="51" t="s">
         <v>7</v>
       </c>
       <c r="F43" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G43" s="63" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H43" s="81"/>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B44" s="55" t="s">
         <v>34</v>
       </c>
       <c r="C44" s="56" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D44" s="56"/>
       <c r="E44" s="51" t="s">
         <v>7</v>
       </c>
       <c r="F44" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G44" s="63" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H44" s="81"/>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B45" s="55" t="s">
         <v>35</v>
       </c>
       <c r="C45" s="56" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D45" s="56"/>
       <c r="E45" s="51" t="s">
         <v>7</v>
       </c>
       <c r="F45" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G45" s="63" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H45" s="81"/>
     </row>
-    <row r="46" spans="2:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:10" ht="30" x14ac:dyDescent="0.2">
       <c r="B46" s="55" t="s">
         <v>36</v>
       </c>
       <c r="C46" s="56" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D46" s="56"/>
       <c r="E46" s="51" t="s">
         <v>7</v>
       </c>
       <c r="F46" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G46" s="63" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H46" s="81"/>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B47" s="38" t="s">
         <v>37</v>
       </c>
       <c r="C47" s="39" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D47" s="39"/>
       <c r="E47" s="54"/>
@@ -7124,12 +7126,12 @@
       <c r="G47" s="39"/>
       <c r="H47" s="40"/>
     </row>
-    <row r="48" spans="2:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:10" ht="30" x14ac:dyDescent="0.2">
       <c r="B48" s="55" t="s">
         <v>38</v>
       </c>
       <c r="C48" s="56" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D48" s="26" t="s">
         <v>7</v>
@@ -7138,19 +7140,19 @@
         <v>7</v>
       </c>
       <c r="F48" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G48" s="63" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H48" s="81"/>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B49" s="55" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C49" s="56" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D49" s="26" t="s">
         <v>7</v>
@@ -7159,10 +7161,10 @@
         <v>7</v>
       </c>
       <c r="F49" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G49" s="63" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H49" s="81"/>
     </row>
@@ -7171,7 +7173,7 @@
         <v>39</v>
       </c>
       <c r="C50" s="56" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D50" s="26" t="s">
         <v>7</v>
@@ -7180,29 +7182,29 @@
         <v>7</v>
       </c>
       <c r="F50" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G50" s="63" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H50" s="81"/>
     </row>
     <row r="51" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B51" s="55" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C51" s="56" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D51" s="56"/>
       <c r="E51" s="51" t="s">
         <v>7</v>
       </c>
       <c r="F51" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G51" s="63" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="H51" s="81"/>
     </row>
@@ -7211,17 +7213,17 @@
         <v>40</v>
       </c>
       <c r="C52" s="56" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D52" s="56"/>
       <c r="E52" s="51" t="s">
         <v>7</v>
       </c>
       <c r="F52" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G52" s="63" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H52" s="81"/>
     </row>
@@ -7230,7 +7232,7 @@
         <v>41</v>
       </c>
       <c r="C53" s="39" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D53" s="39"/>
       <c r="E53" s="54"/>
@@ -7240,10 +7242,10 @@
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B54" s="55" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C54" s="56" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D54" s="26" t="s">
         <v>7</v>
@@ -7252,19 +7254,19 @@
         <v>7</v>
       </c>
       <c r="F54" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G54" s="63" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H54" s="81"/>
     </row>
     <row r="55" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B55" s="55" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C55" s="56" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D55" s="26" t="s">
         <v>7</v>
@@ -7273,19 +7275,19 @@
         <v>7</v>
       </c>
       <c r="F55" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G55" s="63" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H55" s="81"/>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B56" s="55" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C56" s="56" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D56" s="26" t="s">
         <v>7</v>
@@ -7294,19 +7296,19 @@
         <v>7</v>
       </c>
       <c r="F56" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G56" s="63" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H56" s="81"/>
     </row>
     <row r="57" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B57" s="55" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C57" s="56" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D57" s="26" t="s">
         <v>7</v>
@@ -7315,19 +7317,19 @@
         <v>7</v>
       </c>
       <c r="F57" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G57" s="63" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H57" s="81"/>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B58" s="55" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C58" s="56" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D58" s="26" t="s">
         <v>7</v>
@@ -7336,19 +7338,19 @@
         <v>7</v>
       </c>
       <c r="F58" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G58" s="63" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H58" s="81"/>
     </row>
     <row r="59" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B59" s="55" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C59" s="56" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D59" s="26" t="s">
         <v>7</v>
@@ -7357,19 +7359,19 @@
         <v>7</v>
       </c>
       <c r="F59" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G59" s="63" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H59" s="81"/>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B60" s="55" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C60" s="56" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D60" s="26" t="s">
         <v>7</v>
@@ -7378,19 +7380,19 @@
         <v>7</v>
       </c>
       <c r="F60" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G60" s="63" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H60" s="81"/>
     </row>
     <row r="61" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B61" s="55" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C61" s="56" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D61" s="26" t="s">
         <v>7</v>
@@ -7399,19 +7401,19 @@
         <v>7</v>
       </c>
       <c r="F61" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G61" s="63" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="H61" s="81"/>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B62" s="55" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C62" s="56" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D62" s="26" t="s">
         <v>7</v>
@@ -7420,29 +7422,29 @@
         <v>7</v>
       </c>
       <c r="F62" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G62" s="63" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H62" s="81"/>
     </row>
     <row r="63" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B63" s="58" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C63" s="56" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D63" s="56"/>
       <c r="E63" s="51" t="s">
         <v>7</v>
       </c>
       <c r="F63" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G63" s="63" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="H63" s="81"/>
     </row>
@@ -7451,7 +7453,7 @@
         <v>42</v>
       </c>
       <c r="C64" s="39" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D64" s="39"/>
       <c r="E64" s="54"/>
@@ -7461,10 +7463,10 @@
     </row>
     <row r="65" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B65" s="55" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C65" s="56" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D65" s="26" t="s">
         <v>7</v>
@@ -7473,10 +7475,10 @@
         <v>7</v>
       </c>
       <c r="F65" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G65" s="63" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H65" s="81"/>
     </row>
@@ -7485,7 +7487,7 @@
         <v>43</v>
       </c>
       <c r="C66" s="56" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D66" s="26" t="s">
         <v>7</v>
@@ -7494,61 +7496,61 @@
         <v>7</v>
       </c>
       <c r="F66" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G66" s="64" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H66" s="81"/>
     </row>
     <row r="67" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B67" s="55" t="s">
+        <v>142</v>
+      </c>
+      <c r="C67" s="56" t="s">
+        <v>148</v>
+      </c>
+      <c r="D67" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E67" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F67" s="37" t="s">
+        <v>164</v>
+      </c>
+      <c r="G67" s="63" t="s">
+        <v>258</v>
+      </c>
+      <c r="H67" s="81"/>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B68" s="55" t="s">
         <v>143</v>
       </c>
-      <c r="C67" s="56" t="s">
+      <c r="C68" s="56" t="s">
         <v>149</v>
       </c>
-      <c r="D67" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E67" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F67" s="37" t="s">
-        <v>165</v>
-      </c>
-      <c r="G67" s="63" t="s">
+      <c r="D68" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E68" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F68" s="37" t="s">
+        <v>164</v>
+      </c>
+      <c r="G68" s="63" t="s">
         <v>259</v>
-      </c>
-      <c r="H67" s="81"/>
-    </row>
-    <row r="68" spans="2:8" ht="30" x14ac:dyDescent="0.2">
-      <c r="B68" s="55" t="s">
-        <v>144</v>
-      </c>
-      <c r="C68" s="56" t="s">
-        <v>150</v>
-      </c>
-      <c r="D68" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E68" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F68" s="37" t="s">
-        <v>165</v>
-      </c>
-      <c r="G68" s="63" t="s">
-        <v>260</v>
       </c>
       <c r="H68" s="81"/>
     </row>
     <row r="69" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B69" s="55" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C69" s="56" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D69" s="26" t="s">
         <v>7</v>
@@ -7557,10 +7559,10 @@
         <v>7</v>
       </c>
       <c r="F69" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G69" s="65" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H69" s="81"/>
     </row>
@@ -7578,10 +7580,10 @@
         <v>7</v>
       </c>
       <c r="F70" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G70" s="63" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H70" s="81"/>
     </row>
@@ -7590,7 +7592,7 @@
         <v>45</v>
       </c>
       <c r="C71" s="56" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D71" s="26" t="s">
         <v>7</v>
@@ -7599,10 +7601,10 @@
         <v>7</v>
       </c>
       <c r="F71" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G71" s="63" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="H71" s="81"/>
     </row>
@@ -7611,7 +7613,7 @@
         <v>46</v>
       </c>
       <c r="C72" s="56" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D72" s="26" t="s">
         <v>7</v>
@@ -7620,10 +7622,10 @@
         <v>7</v>
       </c>
       <c r="F72" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G72" s="63" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H72" s="81"/>
     </row>
@@ -7665,7 +7667,7 @@
     </row>
     <row r="77" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B77" s="46" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C77" s="47"/>
       <c r="D77" s="45"/>
@@ -7676,10 +7678,10 @@
     </row>
     <row r="78" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B78" s="48" t="s">
+        <v>161</v>
+      </c>
+      <c r="C78" s="48" t="s">
         <v>162</v>
-      </c>
-      <c r="C78" s="48" t="s">
-        <v>163</v>
       </c>
       <c r="D78" s="45"/>
       <c r="E78" s="45"/>
@@ -7689,10 +7691,10 @@
     </row>
     <row r="79" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B79" s="49" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C79" s="49" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D79" s="45"/>
       <c r="E79" s="45"/>
@@ -7702,10 +7704,10 @@
     </row>
     <row r="80" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B80" s="49" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C80" s="49" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D80" s="45"/>
       <c r="E80" s="45"/>
@@ -7715,10 +7717,10 @@
     </row>
     <row r="81" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B81" s="49" t="s">
+        <v>164</v>
+      </c>
+      <c r="C81" s="49" t="s">
         <v>165</v>
-      </c>
-      <c r="C81" s="49" t="s">
-        <v>166</v>
       </c>
       <c r="D81" s="45"/>
       <c r="E81" s="45"/>
@@ -7788,41 +7790,41 @@
     <hyperlink ref="G35" r:id="rId14" location="verifying-cryptographic-key-management"/>
     <hyperlink ref="G37" r:id="rId15" location="verifying-that-users-are-authenticated-properly https://b-mueller.gitbooks.io/owasp-mobile-security-testing-guide/content/"/>
     <hyperlink ref="G38" r:id="rId16" location="testing-session-management https://b-mueller.gitbooks.io/owasp-mobile-security-testing-guide/content/"/>
-    <hyperlink ref="G40" r:id="rId17" location="testing-the-logout-functionality"/>
-    <hyperlink ref="G39" r:id="rId18" location="testing-the-password-policy"/>
-    <hyperlink ref="G41" r:id="rId19" location="testing-excessive-login-attempts"/>
-    <hyperlink ref="G42" r:id="rId20" location="testing-biometric-authentication"/>
-    <hyperlink ref="G43" r:id="rId21" location="testing-the-session-timeout"/>
-    <hyperlink ref="G44" r:id="rId22" location="testing-2-factor-authentication"/>
-    <hyperlink ref="G45" r:id="rId23" location="testing-step-up-authentication"/>
-    <hyperlink ref="G46" r:id="rId24" location="testing-user-device-management"/>
-    <hyperlink ref="G48" r:id="rId25" location="testing-for-unencrypted-sensitive-data-on-the-network"/>
-    <hyperlink ref="G49" r:id="rId26" location="verifying-the-tls-settings"/>
-    <hyperlink ref="G50" r:id="rId27" location="testing-endpoint-identity-verification"/>
-    <hyperlink ref="G51" r:id="rId28" location="testing-custom-certificate-stores-and-ssl-pinning"/>
-    <hyperlink ref="G52" r:id="rId29" location="verifying-that-critical-operations-use-secure-communication-channels"/>
-    <hyperlink ref="G54" r:id="rId30" location="testing-app-permissions"/>
-    <hyperlink ref="G55" r:id="rId31" location="testing-input-validation-and-sanitization"/>
-    <hyperlink ref="G56" r:id="rId32" location="testing-custom-url-schemes"/>
-    <hyperlink ref="G57" r:id="rId33" location="testing-for-sensitive-functionality-exposed-through-ipc"/>
-    <hyperlink ref="G58" r:id="rId34" location="testing-javascript-execution-in-webviews"/>
-    <hyperlink ref="G59" r:id="rId35" location="testing-webview-protocol-handlers"/>
-    <hyperlink ref="G60" r:id="rId36" location="testing-for-local-file-inclusion-in-webviews"/>
-    <hyperlink ref="G61" r:id="rId37" location="testing-whether-java-objects-are-exposed-through-webviews"/>
-    <hyperlink ref="G62" r:id="rId38" location="testing-object-serialization"/>
-    <hyperlink ref="G63" r:id="rId39" location="testing-jailbreak-detection" display="Testing Root Detection"/>
-    <hyperlink ref="G65" r:id="rId40" location="verifying-that-the-app-is-properly-signed"/>
-    <hyperlink ref="G66" r:id="rId41" location="testing-whether-the-app-is-debuggable"/>
-    <hyperlink ref="G67" r:id="rId42" location="verifying-that-debugging-symbols-have-been-removed"/>
-    <hyperlink ref="G68" r:id="rId43" location="testing-for-debugging-code-and-verbose-error-logging"/>
-    <hyperlink ref="G69" r:id="rId44" location="testing-exception-handling"/>
-    <hyperlink ref="G70" r:id="rId45" location="verifying-that-the-app-fails-securely"/>
-    <hyperlink ref="G72" r:id="rId46" location="testing-compiler-settings"/>
-    <hyperlink ref="G25" r:id="rId47" location="testing-for-sensitive-information-in-auto-generated-screenshots"/>
-    <hyperlink ref="G26" r:id="rId48"/>
-    <hyperlink ref="G27" r:id="rId49" location="testing-the-device-access-security-policy"/>
-    <hyperlink ref="G28" r:id="rId50" location="verifying-user-education-controls"/>
-    <hyperlink ref="G71" r:id="rId51" location="testing-for-memory-management-bugs"/>
+    <hyperlink ref="G41" r:id="rId17" location="testing-excessive-login-attempts"/>
+    <hyperlink ref="G42" r:id="rId18" location="testing-biometric-authentication"/>
+    <hyperlink ref="G43" r:id="rId19" location="testing-the-session-timeout"/>
+    <hyperlink ref="G44" r:id="rId20" location="testing-2-factor-authentication"/>
+    <hyperlink ref="G45" r:id="rId21" location="testing-step-up-authentication"/>
+    <hyperlink ref="G46" r:id="rId22" location="testing-user-device-management"/>
+    <hyperlink ref="G48" r:id="rId23" location="testing-for-unencrypted-sensitive-data-on-the-network"/>
+    <hyperlink ref="G49" r:id="rId24" location="verifying-the-tls-settings"/>
+    <hyperlink ref="G50" r:id="rId25" location="testing-endpoint-identity-verification"/>
+    <hyperlink ref="G51" r:id="rId26" location="testing-custom-certificate-stores-and-ssl-pinning"/>
+    <hyperlink ref="G52" r:id="rId27" location="verifying-that-critical-operations-use-secure-communication-channels"/>
+    <hyperlink ref="G54" r:id="rId28" location="testing-app-permissions"/>
+    <hyperlink ref="G55" r:id="rId29" location="testing-input-validation-and-sanitization"/>
+    <hyperlink ref="G56" r:id="rId30" location="testing-custom-url-schemes"/>
+    <hyperlink ref="G57" r:id="rId31" location="testing-for-sensitive-functionality-exposed-through-ipc"/>
+    <hyperlink ref="G58" r:id="rId32" location="testing-javascript-execution-in-webviews"/>
+    <hyperlink ref="G59" r:id="rId33" location="testing-webview-protocol-handlers"/>
+    <hyperlink ref="G60" r:id="rId34" location="testing-for-local-file-inclusion-in-webviews"/>
+    <hyperlink ref="G61" r:id="rId35" location="testing-whether-java-objects-are-exposed-through-webviews"/>
+    <hyperlink ref="G62" r:id="rId36" location="testing-object-serialization"/>
+    <hyperlink ref="G63" r:id="rId37" location="testing-jailbreak-detection" display="Testing Root Detection"/>
+    <hyperlink ref="G65" r:id="rId38" location="verifying-that-the-app-is-properly-signed"/>
+    <hyperlink ref="G66" r:id="rId39" location="testing-whether-the-app-is-debuggable"/>
+    <hyperlink ref="G67" r:id="rId40" location="verifying-that-debugging-symbols-have-been-removed"/>
+    <hyperlink ref="G68" r:id="rId41" location="testing-for-debugging-code-and-verbose-error-logging"/>
+    <hyperlink ref="G69" r:id="rId42" location="testing-exception-handling"/>
+    <hyperlink ref="G70" r:id="rId43" location="verifying-that-the-app-fails-securely"/>
+    <hyperlink ref="G72" r:id="rId44" location="testing-compiler-settings"/>
+    <hyperlink ref="G25" r:id="rId45" location="testing-for-sensitive-information-in-auto-generated-screenshots"/>
+    <hyperlink ref="G26" r:id="rId46"/>
+    <hyperlink ref="G27" r:id="rId47" location="testing-the-device-access-security-policy"/>
+    <hyperlink ref="G28" r:id="rId48" location="verifying-user-education-controls"/>
+    <hyperlink ref="G71" r:id="rId49" location="testing-for-memory-management-bugs"/>
+    <hyperlink ref="G39" r:id="rId50" location="testing-the-logout-functionality"/>
+    <hyperlink ref="G40" r:id="rId51" location="testing-the-password-policy"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -7848,7 +7850,7 @@
   <sheetData>
     <row r="1" spans="2:7" ht="19" x14ac:dyDescent="0.25">
       <c r="B1" s="7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G1" s="24"/>
     </row>
@@ -7864,13 +7866,13 @@
         <v>61</v>
       </c>
       <c r="E3" s="29" t="s">
+        <v>192</v>
+      </c>
+      <c r="F3" s="30" t="s">
+        <v>206</v>
+      </c>
+      <c r="G3" s="30" t="s">
         <v>193</v>
-      </c>
-      <c r="F3" s="30" t="s">
-        <v>207</v>
-      </c>
-      <c r="G3" s="30" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.2">
@@ -7894,10 +7896,10 @@
         <v>7</v>
       </c>
       <c r="E5" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F5" s="62" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G5" s="81"/>
     </row>
@@ -7912,10 +7914,10 @@
         <v>7</v>
       </c>
       <c r="E6" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F6" s="62" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G6" s="81"/>
     </row>
@@ -7930,10 +7932,10 @@
         <v>7</v>
       </c>
       <c r="E7" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F7" s="62" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G7" s="81"/>
     </row>
@@ -7948,10 +7950,10 @@
         <v>7</v>
       </c>
       <c r="E8" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F8" s="62" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G8" s="81"/>
     </row>
@@ -7966,10 +7968,10 @@
         <v>7</v>
       </c>
       <c r="E9" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F9" s="62" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G9" s="81"/>
     </row>
@@ -7984,10 +7986,10 @@
         <v>7</v>
       </c>
       <c r="E10" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F10" s="62" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G10" s="81"/>
     </row>
@@ -8002,10 +8004,10 @@
         <v>7</v>
       </c>
       <c r="E11" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F11" s="62" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G11" s="81"/>
     </row>
@@ -8020,10 +8022,10 @@
         <v>7</v>
       </c>
       <c r="E12" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F12" s="62" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G12" s="81"/>
     </row>
@@ -8038,10 +8040,10 @@
         <v>7</v>
       </c>
       <c r="E13" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F13" s="62" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G13" s="81"/>
     </row>
@@ -8057,7 +8059,7 @@
     </row>
     <row r="15" spans="2:7" ht="30" x14ac:dyDescent="0.2">
       <c r="B15" s="78" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C15" s="36" t="s">
         <v>74</v>
@@ -8066,10 +8068,10 @@
         <v>7</v>
       </c>
       <c r="E15" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F15" s="62" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G15" s="81"/>
     </row>
@@ -8094,10 +8096,10 @@
         <v>7</v>
       </c>
       <c r="E17" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F17" s="62" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G17" s="81"/>
     </row>
@@ -8112,10 +8114,10 @@
         <v>7</v>
       </c>
       <c r="E18" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F18" s="62" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G18" s="81"/>
     </row>
@@ -8130,10 +8132,10 @@
         <v>7</v>
       </c>
       <c r="E19" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F19" s="62" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G19" s="81"/>
     </row>
@@ -8163,7 +8165,7 @@
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B23" s="46" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C23" s="47"/>
       <c r="D23" s="45"/>
@@ -8173,10 +8175,10 @@
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B24" s="48" t="s">
+        <v>161</v>
+      </c>
+      <c r="C24" s="48" t="s">
         <v>162</v>
-      </c>
-      <c r="C24" s="48" t="s">
-        <v>163</v>
       </c>
       <c r="D24" s="45"/>
       <c r="E24" s="45"/>
@@ -8185,10 +8187,10 @@
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B25" s="49" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C25" s="49" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D25" s="45"/>
       <c r="E25" s="45"/>
@@ -8197,10 +8199,10 @@
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B26" s="49" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C26" s="49" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D26" s="45"/>
       <c r="E26" s="45"/>
@@ -8209,10 +8211,10 @@
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B27" s="49" t="s">
+        <v>164</v>
+      </c>
+      <c r="C27" s="49" t="s">
         <v>165</v>
-      </c>
-      <c r="C27" s="49" t="s">
-        <v>166</v>
       </c>
       <c r="D27" s="45"/>
       <c r="E27" s="45"/>
@@ -8306,7 +8308,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="120" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B1" s="120"/>
       <c r="C1" s="50"/>
@@ -8314,21 +8316,21 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="74" t="s">
+        <v>286</v>
+      </c>
+      <c r="B2" s="74" t="s">
+        <v>183</v>
+      </c>
+      <c r="C2" s="74" t="s">
         <v>287</v>
       </c>
-      <c r="B2" s="74" t="s">
-        <v>184</v>
-      </c>
-      <c r="C2" s="74" t="s">
-        <v>288</v>
-      </c>
       <c r="D2" s="75" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="72" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B3" s="76">
         <v>0.1</v>
@@ -8337,12 +8339,12 @@
         <v>42765</v>
       </c>
       <c r="D3" s="71" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="71" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B4" s="76">
         <v>0.2</v>
@@ -8351,12 +8353,12 @@
         <v>42766</v>
       </c>
       <c r="D4" s="71" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="71" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B5" s="76">
         <v>0.3</v>
@@ -8365,49 +8367,49 @@
         <v>42778</v>
       </c>
       <c r="D5" s="71" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="71" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B6" s="76" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C6" s="73">
         <v>42780</v>
       </c>
       <c r="D6" s="71" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="71" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B7" s="77" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C7" s="73">
         <v>42781</v>
       </c>
       <c r="D7" s="71" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="71" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B8" s="77" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C8" s="73">
         <v>42829</v>
       </c>
       <c r="D8" s="71" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
update checklist to version 1.0
</commit_message>
<xml_diff>
--- a/Checklists/Mobile_App_Security_Checklist.xlsx
+++ b/Checklists/Mobile_App_Security_Checklist.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27106"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="29005"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="29340" yWindow="-2400" windowWidth="25860" windowHeight="21140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="6" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="300">
   <si>
     <t>ID</t>
   </si>
@@ -912,6 +912,15 @@
   </si>
   <si>
     <t>Sync with MASVS (update requirements of domain 1, 4 and 6)</t>
+  </si>
+  <si>
+    <t>Verify that the remote endpoint implements a mechanism to protect against the submission of credentials an excessive number of times.</t>
+  </si>
+  <si>
+    <t>Verify that obfuscation is applied to programmatic defenses, which in turn impede de-obfuscation via dynamic analysis.</t>
+  </si>
+  <si>
+    <t>8.9</t>
   </si>
   <si>
     <r>
@@ -925,17 +934,17 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">
-Based on the OWASP Mobile Application Security Verification Standard 0.9.4</t>
+Based on the OWASP Mobile Application Security Verification Standard 1.0</t>
     </r>
   </si>
   <si>
-    <t>Verify that the remote endpoint implements a mechanism to protect against the submission of credentials an excessive number of times.</t>
-  </si>
-  <si>
-    <t>Verify that obfuscation is applied to programmatic defenses, which in turn impede de-obfuscation via dynamic analysis.</t>
-  </si>
-  <si>
-    <t>8.9</t>
+    <t>0.9.4</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>Sync with MASVS (update requirements of domain 3 and 8)</t>
   </si>
 </sst>
 </file>
@@ -1673,7 +1682,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -1865,64 +1874,100 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1937,47 +1982,14 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="62">
@@ -2075,7 +2087,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-SG"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2234,11 +2246,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2079049120"/>
-        <c:axId val="-2080404784"/>
+        <c:axId val="987869328"/>
+        <c:axId val="905755360"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="-2079049120"/>
+        <c:axId val="987869328"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2275,7 +2287,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2080404784"/>
+        <c:crossAx val="905755360"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -2283,7 +2295,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2080404784"/>
+        <c:axId val="905755360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2328,7 +2340,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2079049120"/>
+        <c:crossAx val="987869328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2416,7 +2428,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-SG"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2569,11 +2581,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2079132336"/>
-        <c:axId val="-2079135632"/>
+        <c:axId val="985158976"/>
+        <c:axId val="904745696"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="-2079132336"/>
+        <c:axId val="985158976"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2610,7 +2622,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2079135632"/>
+        <c:crossAx val="904745696"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -2618,7 +2630,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2079135632"/>
+        <c:axId val="904745696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2663,7 +2675,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2079132336"/>
+        <c:crossAx val="985158976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3190,8 +3202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D45"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:D18"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3203,48 +3215,48 @@
   <sheetData>
     <row r="1" spans="2:4" ht="8" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B2" s="85" t="s">
-        <v>293</v>
-      </c>
-      <c r="C2" s="86"/>
-      <c r="D2" s="87"/>
+      <c r="B2" s="79" t="s">
+        <v>296</v>
+      </c>
+      <c r="C2" s="80"/>
+      <c r="D2" s="81"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="88"/>
-      <c r="C3" s="89"/>
-      <c r="D3" s="90"/>
+      <c r="B3" s="82"/>
+      <c r="C3" s="83"/>
+      <c r="D3" s="84"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B4" s="88"/>
-      <c r="C4" s="89"/>
-      <c r="D4" s="90"/>
+      <c r="B4" s="82"/>
+      <c r="C4" s="83"/>
+      <c r="D4" s="84"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="88"/>
-      <c r="C5" s="89"/>
-      <c r="D5" s="90"/>
+      <c r="B5" s="82"/>
+      <c r="C5" s="83"/>
+      <c r="D5" s="84"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B6" s="88"/>
-      <c r="C6" s="89"/>
-      <c r="D6" s="90"/>
+      <c r="B6" s="82"/>
+      <c r="C6" s="83"/>
+      <c r="D6" s="84"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B7" s="88"/>
-      <c r="C7" s="89"/>
-      <c r="D7" s="90"/>
+      <c r="B7" s="82"/>
+      <c r="C7" s="83"/>
+      <c r="D7" s="84"/>
     </row>
     <row r="8" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="91"/>
-      <c r="C8" s="92"/>
-      <c r="D8" s="93"/>
+      <c r="B8" s="85"/>
+      <c r="C8" s="86"/>
+      <c r="D8" s="87"/>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B9" s="94" t="s">
+      <c r="B9" s="88" t="s">
         <v>164</v>
       </c>
-      <c r="C9" s="82"/>
-      <c r="D9" s="83"/>
+      <c r="C9" s="89"/>
+      <c r="D9" s="90"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
@@ -3254,62 +3266,62 @@
       <c r="D10" s="3"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B11" s="80" t="s">
+      <c r="B11" s="75" t="s">
         <v>142</v>
       </c>
-      <c r="C11" s="81"/>
+      <c r="C11" s="76"/>
       <c r="D11" s="13"/>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B12" s="75" t="s">
+      <c r="B12" s="77" t="s">
         <v>143</v>
       </c>
-      <c r="C12" s="84"/>
+      <c r="C12" s="78"/>
       <c r="D12" s="13"/>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B13" s="80" t="s">
+      <c r="B13" s="75" t="s">
         <v>153</v>
       </c>
-      <c r="C13" s="81"/>
+      <c r="C13" s="76"/>
       <c r="D13" s="13"/>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B14" s="80" t="s">
+      <c r="B14" s="75" t="s">
         <v>144</v>
       </c>
-      <c r="C14" s="81"/>
+      <c r="C14" s="76"/>
       <c r="D14" s="13"/>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B15" s="80" t="s">
+      <c r="B15" s="75" t="s">
         <v>253</v>
       </c>
-      <c r="C15" s="81"/>
+      <c r="C15" s="76"/>
       <c r="D15" s="13"/>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B16" s="80" t="s">
+      <c r="B16" s="75" t="s">
         <v>163</v>
       </c>
-      <c r="C16" s="81"/>
+      <c r="C16" s="76"/>
       <c r="D16" s="13" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="80" t="s">
+      <c r="B17" s="75" t="s">
         <v>165</v>
       </c>
-      <c r="C17" s="81"/>
+      <c r="C17" s="76"/>
       <c r="D17" s="13" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B18" s="82"/>
-      <c r="C18" s="82"/>
-      <c r="D18" s="83"/>
+      <c r="B18" s="89"/>
+      <c r="C18" s="89"/>
+      <c r="D18" s="90"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
@@ -3326,37 +3338,37 @@
       <c r="D20" s="13"/>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B21" s="80" t="s">
+      <c r="B21" s="75" t="s">
         <v>155</v>
       </c>
-      <c r="C21" s="81"/>
+      <c r="C21" s="76"/>
       <c r="D21" s="13"/>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B22" s="80" t="s">
+      <c r="B22" s="75" t="s">
         <v>156</v>
       </c>
-      <c r="C22" s="81"/>
+      <c r="C22" s="76"/>
       <c r="D22" s="13"/>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B23" s="80" t="s">
+      <c r="B23" s="75" t="s">
         <v>157</v>
       </c>
-      <c r="C23" s="81"/>
+      <c r="C23" s="76"/>
       <c r="D23" s="13"/>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B24" s="80" t="s">
+      <c r="B24" s="75" t="s">
         <v>158</v>
       </c>
-      <c r="C24" s="81"/>
+      <c r="C24" s="76"/>
       <c r="D24" s="13"/>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B25" s="82"/>
-      <c r="C25" s="82"/>
-      <c r="D25" s="83"/>
+      <c r="B25" s="89"/>
+      <c r="C25" s="89"/>
+      <c r="D25" s="90"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
@@ -3373,37 +3385,37 @@
       <c r="D27" s="13"/>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B28" s="80" t="s">
+      <c r="B28" s="75" t="s">
         <v>146</v>
       </c>
-      <c r="C28" s="81"/>
+      <c r="C28" s="76"/>
       <c r="D28" s="13"/>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B29" s="80" t="s">
+      <c r="B29" s="75" t="s">
         <v>156</v>
       </c>
-      <c r="C29" s="81"/>
+      <c r="C29" s="76"/>
       <c r="D29" s="13"/>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B30" s="80" t="s">
+      <c r="B30" s="75" t="s">
         <v>157</v>
       </c>
-      <c r="C30" s="81"/>
+      <c r="C30" s="76"/>
       <c r="D30" s="13"/>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B31" s="80" t="s">
+      <c r="B31" s="75" t="s">
         <v>160</v>
       </c>
-      <c r="C31" s="81"/>
+      <c r="C31" s="76"/>
       <c r="D31" s="13"/>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B32" s="82"/>
-      <c r="C32" s="82"/>
-      <c r="D32" s="83"/>
+      <c r="B32" s="89"/>
+      <c r="C32" s="89"/>
+      <c r="D32" s="90"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
@@ -3413,95 +3425,97 @@
       <c r="D33" s="3"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B34" s="77"/>
-      <c r="C34" s="78"/>
-      <c r="D34" s="79"/>
+      <c r="B34" s="91"/>
+      <c r="C34" s="92"/>
+      <c r="D34" s="93"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B35" s="75" t="s">
+      <c r="B35" s="77" t="s">
         <v>148</v>
       </c>
-      <c r="C35" s="76"/>
+      <c r="C35" s="94"/>
       <c r="D35" s="62"/>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B36" s="75" t="s">
+      <c r="B36" s="77" t="s">
         <v>149</v>
       </c>
-      <c r="C36" s="76"/>
+      <c r="C36" s="94"/>
       <c r="D36" s="62"/>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B37" s="75" t="s">
+      <c r="B37" s="77" t="s">
         <v>150</v>
       </c>
-      <c r="C37" s="76"/>
+      <c r="C37" s="94"/>
       <c r="D37" s="62"/>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B38" s="75" t="s">
+      <c r="B38" s="77" t="s">
         <v>151</v>
       </c>
-      <c r="C38" s="76"/>
+      <c r="C38" s="94"/>
       <c r="D38" s="63"/>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B39" s="75" t="s">
+      <c r="B39" s="77" t="s">
         <v>152</v>
       </c>
-      <c r="C39" s="76"/>
+      <c r="C39" s="94"/>
       <c r="D39" s="62"/>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B40" s="77"/>
-      <c r="C40" s="78"/>
-      <c r="D40" s="79"/>
+      <c r="B40" s="91"/>
+      <c r="C40" s="92"/>
+      <c r="D40" s="93"/>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B41" s="75" t="s">
+      <c r="B41" s="77" t="s">
         <v>148</v>
       </c>
-      <c r="C41" s="76"/>
+      <c r="C41" s="94"/>
       <c r="D41" s="62"/>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B42" s="75" t="s">
+      <c r="B42" s="77" t="s">
         <v>149</v>
       </c>
-      <c r="C42" s="76"/>
+      <c r="C42" s="94"/>
       <c r="D42" s="62"/>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B43" s="75" t="s">
+      <c r="B43" s="77" t="s">
         <v>150</v>
       </c>
-      <c r="C43" s="76"/>
+      <c r="C43" s="94"/>
       <c r="D43" s="62"/>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B44" s="75" t="s">
+      <c r="B44" s="77" t="s">
         <v>151</v>
       </c>
-      <c r="C44" s="76"/>
+      <c r="C44" s="94"/>
       <c r="D44" s="63"/>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B45" s="75" t="s">
+      <c r="B45" s="77" t="s">
         <v>152</v>
       </c>
-      <c r="C45" s="76"/>
+      <c r="C45" s="94"/>
       <c r="D45" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B2:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="B41:C41"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B34:D34"/>
@@ -3516,16 +3530,14 @@
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B2:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B15:C15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -3571,11 +3583,11 @@
       <c r="F3" s="9"/>
     </row>
     <row r="4" spans="2:24" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="B4" s="99"/>
-      <c r="C4" s="99"/>
-      <c r="D4" s="99"/>
-      <c r="E4" s="99"/>
-      <c r="F4" s="99"/>
+      <c r="B4" s="111"/>
+      <c r="C4" s="111"/>
+      <c r="D4" s="111"/>
+      <c r="E4" s="111"/>
+      <c r="F4" s="111"/>
     </row>
     <row r="5" spans="2:24" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="21"/>
@@ -3590,16 +3602,16 @@
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
       <c r="F6" s="22"/>
-      <c r="G6" s="109" t="s">
+      <c r="G6" s="95" t="s">
         <v>176</v>
       </c>
-      <c r="H6" s="110"/>
-      <c r="I6" s="111"/>
-      <c r="V6" s="109" t="s">
+      <c r="H6" s="96"/>
+      <c r="I6" s="97"/>
+      <c r="V6" s="95" t="s">
         <v>176</v>
       </c>
-      <c r="W6" s="110"/>
-      <c r="X6" s="111"/>
+      <c r="W6" s="96"/>
+      <c r="X6" s="97"/>
     </row>
     <row r="7" spans="2:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="14"/>
@@ -3614,18 +3626,18 @@
       <c r="D8" s="21"/>
       <c r="E8" s="21"/>
       <c r="F8" s="21"/>
-      <c r="G8" s="100" t="e">
+      <c r="G8" s="98" t="e">
         <f>AVERAGE(G43:G50)*5</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H8" s="101"/>
-      <c r="I8" s="102"/>
-      <c r="V8" s="100" t="e">
+      <c r="H8" s="99"/>
+      <c r="I8" s="100"/>
+      <c r="V8" s="98" t="e">
         <f>AVERAGE(K43:K50)*5</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="W8" s="101"/>
-      <c r="X8" s="102"/>
+      <c r="W8" s="99"/>
+      <c r="X8" s="100"/>
     </row>
     <row r="9" spans="2:24" ht="91" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="22"/>
@@ -3633,12 +3645,12 @@
       <c r="D9" s="22"/>
       <c r="E9" s="22"/>
       <c r="F9" s="22"/>
-      <c r="G9" s="103"/>
-      <c r="H9" s="104"/>
-      <c r="I9" s="105"/>
-      <c r="V9" s="103"/>
-      <c r="W9" s="104"/>
-      <c r="X9" s="105"/>
+      <c r="G9" s="101"/>
+      <c r="H9" s="102"/>
+      <c r="I9" s="103"/>
+      <c r="V9" s="101"/>
+      <c r="W9" s="102"/>
+      <c r="X9" s="103"/>
     </row>
     <row r="10" spans="2:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="14"/>
@@ -3646,12 +3658,12 @@
       <c r="D10" s="14"/>
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
-      <c r="G10" s="103"/>
-      <c r="H10" s="104"/>
-      <c r="I10" s="105"/>
-      <c r="V10" s="103"/>
-      <c r="W10" s="104"/>
-      <c r="X10" s="105"/>
+      <c r="G10" s="101"/>
+      <c r="H10" s="102"/>
+      <c r="I10" s="103"/>
+      <c r="V10" s="101"/>
+      <c r="W10" s="102"/>
+      <c r="X10" s="103"/>
     </row>
     <row r="11" spans="2:24" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B11" s="14"/>
@@ -3659,19 +3671,19 @@
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
-      <c r="G11" s="106"/>
-      <c r="H11" s="107"/>
-      <c r="I11" s="108"/>
-      <c r="V11" s="106"/>
-      <c r="W11" s="107"/>
-      <c r="X11" s="108"/>
+      <c r="G11" s="104"/>
+      <c r="H11" s="105"/>
+      <c r="I11" s="106"/>
+      <c r="V11" s="104"/>
+      <c r="W11" s="105"/>
+      <c r="X11" s="106"/>
     </row>
     <row r="12" spans="2:24" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="95"/>
-      <c r="C12" s="95"/>
-      <c r="D12" s="95"/>
-      <c r="E12" s="95"/>
-      <c r="F12" s="95"/>
+      <c r="B12" s="107"/>
+      <c r="C12" s="107"/>
+      <c r="D12" s="107"/>
+      <c r="E12" s="107"/>
+      <c r="F12" s="107"/>
     </row>
     <row r="13" spans="2:24" ht="15" x14ac:dyDescent="0.2">
       <c r="B13" s="15"/>
@@ -3695,11 +3707,11 @@
       <c r="F15" s="14"/>
     </row>
     <row r="16" spans="2:24" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="95"/>
-      <c r="C16" s="95"/>
-      <c r="D16" s="95"/>
-      <c r="E16" s="95"/>
-      <c r="F16" s="95"/>
+      <c r="B16" s="107"/>
+      <c r="C16" s="107"/>
+      <c r="D16" s="107"/>
+      <c r="E16" s="107"/>
+      <c r="F16" s="107"/>
     </row>
     <row r="17" spans="2:6" ht="15" x14ac:dyDescent="0.2">
       <c r="B17" s="15"/>
@@ -3752,18 +3764,18 @@
     </row>
     <row r="35" spans="3:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="41" spans="3:11" x14ac:dyDescent="0.15">
-      <c r="D41" s="96" t="s">
+      <c r="D41" s="108" t="s">
         <v>174</v>
       </c>
-      <c r="E41" s="97"/>
-      <c r="F41" s="97"/>
-      <c r="G41" s="98"/>
-      <c r="H41" s="96" t="s">
+      <c r="E41" s="109"/>
+      <c r="F41" s="109"/>
+      <c r="G41" s="110"/>
+      <c r="H41" s="108" t="s">
         <v>175</v>
       </c>
-      <c r="I41" s="97"/>
-      <c r="J41" s="97"/>
-      <c r="K41" s="98"/>
+      <c r="I41" s="109"/>
+      <c r="J41" s="109"/>
+      <c r="K41" s="110"/>
     </row>
     <row r="42" spans="3:11" x14ac:dyDescent="0.15">
       <c r="D42" s="18" t="s">
@@ -4089,15 +4101,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="G8:I11"/>
+    <mergeCell ref="G6:I6"/>
     <mergeCell ref="V6:X6"/>
     <mergeCell ref="V8:X11"/>
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="B16:F16"/>
     <mergeCell ref="D41:G41"/>
     <mergeCell ref="H41:K41"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="G8:I11"/>
-    <mergeCell ref="G6:I6"/>
   </mergeCells>
   <conditionalFormatting sqref="F14">
     <cfRule type="iconSet" priority="3">
@@ -4137,7 +4149,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J85"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
@@ -4876,7 +4888,7 @@
         <v>88</v>
       </c>
       <c r="C41" s="56" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D41" s="26" t="s">
         <v>7</v>
@@ -5878,7 +5890,7 @@
         <v>8.9</v>
       </c>
       <c r="C13" s="36" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D13" s="25" t="s">
         <v>7</v>
@@ -6100,7 +6112,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J85"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
@@ -6839,7 +6851,7 @@
         <v>88</v>
       </c>
       <c r="C41" s="56" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D41" s="26" t="s">
         <v>7</v>
@@ -7826,7 +7838,7 @@
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B13" s="71" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C13" s="36" t="s">
         <v>63</v>
@@ -8073,7 +8085,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8207,7 +8219,7 @@
         <v>133</v>
       </c>
       <c r="B10" s="70" t="s">
-        <v>265</v>
+        <v>297</v>
       </c>
       <c r="C10" s="66">
         <v>42963</v>
@@ -8217,10 +8229,18 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="50"/>
-      <c r="B11" s="50"/>
-      <c r="C11" s="50"/>
-      <c r="D11" s="50"/>
+      <c r="A11" s="64" t="s">
+        <v>133</v>
+      </c>
+      <c r="B11" s="114" t="s">
+        <v>298</v>
+      </c>
+      <c r="C11" s="66">
+        <v>43113</v>
+      </c>
+      <c r="D11" s="64" t="s">
+        <v>299</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
fixed on excel checklist
</commit_message>
<xml_diff>
--- a/Checklists/Mobile_App_Security_Checklist.xlsx
+++ b/Checklists/Mobile_App_Security_Checklist.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="29005"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10116"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,18 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="6" r:id="rId1"/>
     <sheet name="Management Summary" sheetId="7" r:id="rId2"/>
-    <sheet name="Security Requirements - Android" sheetId="10" r:id="rId3"/>
-    <sheet name="Anti-RE - Android" sheetId="11" r:id="rId4"/>
+    <sheet name="Anti-RE - Android" sheetId="11" r:id="rId3"/>
+    <sheet name="Security Requirements - Android" sheetId="10" r:id="rId4"/>
     <sheet name="Security Requirements - iOS" sheetId="1" r:id="rId5"/>
     <sheet name="Anti-RE - iOS" sheetId="3" r:id="rId6"/>
     <sheet name="Version history" sheetId="2" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Security Requirements - Android'!$B$3:$H$72</definedName>
+  </definedNames>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -950,7 +953,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
   </numFmts>
@@ -1877,64 +1880,76 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="21" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="20" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="22" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="13" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1972,18 +1987,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="21" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="20" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="22" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -2085,7 +2088,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2128,7 +2131,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.619807766243752"/>
-          <c:y val="0.0246058769467697"/>
+          <c:y val="2.46058769467697E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -2146,10 +2149,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.221460287279808"/>
-          <c:y val="0.112618692933654"/>
-          <c:w val="0.502513690978939"/>
-          <c:h val="0.841079865016873"/>
+          <c:x val="0.22146028727980799"/>
+          <c:y val="0.11261869293365399"/>
+          <c:w val="0.50251369097893905"/>
+          <c:h val="0.84107986501687304"/>
         </c:manualLayout>
       </c:layout>
       <c:radarChart>
@@ -2211,32 +2214,37 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DEA7-C349-8A34-4369353CE077}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2288,7 +2296,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="918959216"/>
-        <c:crossesAt val="0.0"/>
+        <c:crossesAt val="0"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -2357,10 +2365,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.823556052033288"/>
-          <c:y val="0.0867538179349203"/>
-          <c:w val="0.152253978633294"/>
-          <c:h val="0.0463334650736225"/>
+          <c:x val="0.82355605203328797"/>
+          <c:y val="8.6753817934920305E-2"/>
+          <c:w val="0.15225397863329401"/>
+          <c:h val="4.6333465073622501E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -2419,14 +2427,14 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.984251969" l="0.787401575" r="0.787401575" t="0.984251969" header="0.511805555555556" footer="0.511805555555556"/>
+    <c:pageMargins b="0.984251969" l="0.78740157499999996" r="0.78740157499999996" t="0.984251969" header="0.51180555555555596" footer="0.51180555555555596"/>
     <c:pageSetup firstPageNumber="0"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2468,8 +2476,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.64902100128693"/>
-          <c:y val="0.0246058605184029"/>
+          <c:x val="0.64902100128692997"/>
+          <c:y val="2.4605860518402901E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -2487,10 +2495,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.221460287279808"/>
-          <c:y val="0.112618692933654"/>
-          <c:w val="0.502513690978939"/>
-          <c:h val="0.841079865016873"/>
+          <c:x val="0.22146028727980799"/>
+          <c:y val="0.11261869293365399"/>
+          <c:w val="0.50251369097893905"/>
+          <c:h val="0.84107986501687304"/>
         </c:manualLayout>
       </c:layout>
       <c:radarChart>
@@ -2546,32 +2554,37 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-44E8-7142-8A6C-612DBEEBB445}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2623,7 +2636,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="920829984"/>
-        <c:crossesAt val="0.0"/>
+        <c:crossesAt val="0"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -2692,10 +2705,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.823556052033288"/>
-          <c:y val="0.0867538179349203"/>
-          <c:w val="0.044674738528106"/>
-          <c:h val="0.0390752020396546"/>
+          <c:x val="0.82355605203328797"/>
+          <c:y val="8.6753817934920305E-2"/>
+          <c:w val="4.4674738528106002E-2"/>
+          <c:h val="3.9075202039654602E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -2754,7 +2767,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.984251969" l="0.787401575" r="0.787401575" t="0.984251969" header="0.511805555555556" footer="0.511805555555556"/>
+    <c:pageMargins b="0.984251969" l="0.78740157499999996" r="0.78740157499999996" t="0.984251969" header="0.51180555555555596" footer="0.51180555555555596"/>
     <c:pageSetup firstPageNumber="0"/>
   </c:printSettings>
 </c:chartSpace>
@@ -2777,7 +2790,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2820,13 +2839,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>361952</xdr:colOff>
+      <xdr:colOff>246498</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>67913</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Graphique 1"/>
+        <xdr:cNvPr id="2" name="Graphique 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -2846,19 +2871,25 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>290996</xdr:colOff>
+      <xdr:colOff>175541</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>65373</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>434010</xdr:colOff>
+      <xdr:colOff>318556</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>97123</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Graphique 1"/>
+        <xdr:cNvPr id="3" name="Graphique 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -3199,10 +3230,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:D45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -3215,48 +3246,48 @@
   <sheetData>
     <row r="1" spans="2:4" ht="8" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B2" s="86" t="s">
+      <c r="B2" s="80" t="s">
         <v>296</v>
       </c>
-      <c r="C2" s="87"/>
-      <c r="D2" s="88"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="82"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="89"/>
-      <c r="C3" s="90"/>
-      <c r="D3" s="91"/>
+      <c r="B3" s="83"/>
+      <c r="C3" s="84"/>
+      <c r="D3" s="85"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B4" s="89"/>
-      <c r="C4" s="90"/>
-      <c r="D4" s="91"/>
+      <c r="B4" s="83"/>
+      <c r="C4" s="84"/>
+      <c r="D4" s="85"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="89"/>
-      <c r="C5" s="90"/>
-      <c r="D5" s="91"/>
+      <c r="B5" s="83"/>
+      <c r="C5" s="84"/>
+      <c r="D5" s="85"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B6" s="89"/>
-      <c r="C6" s="90"/>
-      <c r="D6" s="91"/>
+      <c r="B6" s="83"/>
+      <c r="C6" s="84"/>
+      <c r="D6" s="85"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B7" s="89"/>
-      <c r="C7" s="90"/>
-      <c r="D7" s="91"/>
+      <c r="B7" s="83"/>
+      <c r="C7" s="84"/>
+      <c r="D7" s="85"/>
     </row>
     <row r="8" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="92"/>
-      <c r="C8" s="93"/>
-      <c r="D8" s="94"/>
+      <c r="B8" s="86"/>
+      <c r="C8" s="87"/>
+      <c r="D8" s="88"/>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B9" s="95" t="s">
+      <c r="B9" s="89" t="s">
         <v>164</v>
       </c>
-      <c r="C9" s="83"/>
-      <c r="D9" s="84"/>
+      <c r="C9" s="90"/>
+      <c r="D9" s="91"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
@@ -3266,62 +3297,62 @@
       <c r="D10" s="3"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B11" s="81" t="s">
+      <c r="B11" s="76" t="s">
         <v>142</v>
       </c>
-      <c r="C11" s="82"/>
+      <c r="C11" s="77"/>
       <c r="D11" s="13"/>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B12" s="76" t="s">
+      <c r="B12" s="78" t="s">
         <v>143</v>
       </c>
-      <c r="C12" s="85"/>
+      <c r="C12" s="79"/>
       <c r="D12" s="13"/>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B13" s="81" t="s">
+      <c r="B13" s="76" t="s">
         <v>153</v>
       </c>
-      <c r="C13" s="82"/>
+      <c r="C13" s="77"/>
       <c r="D13" s="13"/>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B14" s="81" t="s">
+      <c r="B14" s="76" t="s">
         <v>144</v>
       </c>
-      <c r="C14" s="82"/>
+      <c r="C14" s="77"/>
       <c r="D14" s="13"/>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B15" s="81" t="s">
+      <c r="B15" s="76" t="s">
         <v>253</v>
       </c>
-      <c r="C15" s="82"/>
+      <c r="C15" s="77"/>
       <c r="D15" s="13"/>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B16" s="81" t="s">
+      <c r="B16" s="76" t="s">
         <v>163</v>
       </c>
-      <c r="C16" s="82"/>
+      <c r="C16" s="77"/>
       <c r="D16" s="13" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="81" t="s">
+      <c r="B17" s="76" t="s">
         <v>165</v>
       </c>
-      <c r="C17" s="82"/>
+      <c r="C17" s="77"/>
       <c r="D17" s="13" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B18" s="83"/>
-      <c r="C18" s="83"/>
-      <c r="D18" s="84"/>
+      <c r="B18" s="90"/>
+      <c r="C18" s="90"/>
+      <c r="D18" s="91"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
@@ -3338,37 +3369,37 @@
       <c r="D20" s="13"/>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B21" s="81" t="s">
+      <c r="B21" s="76" t="s">
         <v>155</v>
       </c>
-      <c r="C21" s="82"/>
+      <c r="C21" s="77"/>
       <c r="D21" s="13"/>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B22" s="81" t="s">
+      <c r="B22" s="76" t="s">
         <v>156</v>
       </c>
-      <c r="C22" s="82"/>
+      <c r="C22" s="77"/>
       <c r="D22" s="13"/>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B23" s="81" t="s">
+      <c r="B23" s="76" t="s">
         <v>157</v>
       </c>
-      <c r="C23" s="82"/>
+      <c r="C23" s="77"/>
       <c r="D23" s="13"/>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B24" s="81" t="s">
+      <c r="B24" s="76" t="s">
         <v>158</v>
       </c>
-      <c r="C24" s="82"/>
+      <c r="C24" s="77"/>
       <c r="D24" s="13"/>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B25" s="83"/>
-      <c r="C25" s="83"/>
-      <c r="D25" s="84"/>
+      <c r="B25" s="90"/>
+      <c r="C25" s="90"/>
+      <c r="D25" s="91"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
@@ -3385,37 +3416,37 @@
       <c r="D27" s="13"/>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B28" s="81" t="s">
+      <c r="B28" s="76" t="s">
         <v>146</v>
       </c>
-      <c r="C28" s="82"/>
+      <c r="C28" s="77"/>
       <c r="D28" s="13"/>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B29" s="81" t="s">
+      <c r="B29" s="76" t="s">
         <v>156</v>
       </c>
-      <c r="C29" s="82"/>
+      <c r="C29" s="77"/>
       <c r="D29" s="13"/>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B30" s="81" t="s">
+      <c r="B30" s="76" t="s">
         <v>157</v>
       </c>
-      <c r="C30" s="82"/>
+      <c r="C30" s="77"/>
       <c r="D30" s="13"/>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B31" s="81" t="s">
+      <c r="B31" s="76" t="s">
         <v>160</v>
       </c>
-      <c r="C31" s="82"/>
+      <c r="C31" s="77"/>
       <c r="D31" s="13"/>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B32" s="83"/>
-      <c r="C32" s="83"/>
-      <c r="D32" s="84"/>
+      <c r="B32" s="90"/>
+      <c r="C32" s="90"/>
+      <c r="D32" s="91"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
@@ -3425,95 +3456,97 @@
       <c r="D33" s="3"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B34" s="78"/>
-      <c r="C34" s="79"/>
-      <c r="D34" s="80"/>
+      <c r="B34" s="92"/>
+      <c r="C34" s="93"/>
+      <c r="D34" s="94"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B35" s="76" t="s">
+      <c r="B35" s="78" t="s">
         <v>148</v>
       </c>
-      <c r="C35" s="77"/>
+      <c r="C35" s="95"/>
       <c r="D35" s="62"/>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B36" s="76" t="s">
+      <c r="B36" s="78" t="s">
         <v>149</v>
       </c>
-      <c r="C36" s="77"/>
+      <c r="C36" s="95"/>
       <c r="D36" s="62"/>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B37" s="76" t="s">
+      <c r="B37" s="78" t="s">
         <v>150</v>
       </c>
-      <c r="C37" s="77"/>
+      <c r="C37" s="95"/>
       <c r="D37" s="62"/>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B38" s="76" t="s">
+      <c r="B38" s="78" t="s">
         <v>151</v>
       </c>
-      <c r="C38" s="77"/>
+      <c r="C38" s="95"/>
       <c r="D38" s="63"/>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B39" s="76" t="s">
+      <c r="B39" s="78" t="s">
         <v>152</v>
       </c>
-      <c r="C39" s="77"/>
+      <c r="C39" s="95"/>
       <c r="D39" s="62"/>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B40" s="78"/>
-      <c r="C40" s="79"/>
-      <c r="D40" s="80"/>
+      <c r="B40" s="92"/>
+      <c r="C40" s="93"/>
+      <c r="D40" s="94"/>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B41" s="76" t="s">
+      <c r="B41" s="78" t="s">
         <v>148</v>
       </c>
-      <c r="C41" s="77"/>
+      <c r="C41" s="95"/>
       <c r="D41" s="62"/>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B42" s="76" t="s">
+      <c r="B42" s="78" t="s">
         <v>149</v>
       </c>
-      <c r="C42" s="77"/>
+      <c r="C42" s="95"/>
       <c r="D42" s="62"/>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B43" s="76" t="s">
+      <c r="B43" s="78" t="s">
         <v>150</v>
       </c>
-      <c r="C43" s="77"/>
+      <c r="C43" s="95"/>
       <c r="D43" s="62"/>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B44" s="76" t="s">
+      <c r="B44" s="78" t="s">
         <v>151</v>
       </c>
-      <c r="C44" s="77"/>
+      <c r="C44" s="95"/>
       <c r="D44" s="63"/>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B45" s="76" t="s">
+      <c r="B45" s="78" t="s">
         <v>152</v>
       </c>
-      <c r="C45" s="77"/>
+      <c r="C45" s="95"/>
       <c r="D45" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B2:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="B41:C41"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B34:D34"/>
@@ -3528,16 +3561,14 @@
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B2:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B15:C15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -3546,11 +3577,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:X50"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A9" zoomScale="88" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="88" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="L43" sqref="L43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -3561,12 +3592,12 @@
     <col min="4" max="4" width="6" style="6" customWidth="1"/>
     <col min="5" max="5" width="4.6640625" style="6" customWidth="1"/>
     <col min="6" max="6" width="5.83203125" style="6" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="10.1640625" style="6" customWidth="1"/>
     <col min="8" max="16384" width="8.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B2" s="8"/>
       <c r="C2" s="23" t="s">
         <v>162</v>
@@ -3575,45 +3606,45 @@
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
     </row>
-    <row r="3" spans="2:24" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
     </row>
-    <row r="4" spans="2:24" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="B4" s="96"/>
-      <c r="C4" s="96"/>
-      <c r="D4" s="96"/>
-      <c r="E4" s="96"/>
-      <c r="F4" s="96"/>
-    </row>
-    <row r="5" spans="2:24" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:24" x14ac:dyDescent="0.15">
+      <c r="B4" s="100"/>
+      <c r="C4" s="100"/>
+      <c r="D4" s="100"/>
+      <c r="E4" s="100"/>
+      <c r="F4" s="100"/>
+    </row>
+    <row r="5" spans="2:24" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B5" s="21"/>
       <c r="C5" s="21"/>
       <c r="D5" s="21"/>
       <c r="E5" s="21"/>
       <c r="F5" s="21"/>
     </row>
-    <row r="6" spans="2:24" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:24" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B6" s="22"/>
       <c r="C6" s="22"/>
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
       <c r="F6" s="22"/>
-      <c r="G6" s="106" t="s">
+      <c r="G6" s="110" t="s">
         <v>176</v>
       </c>
-      <c r="H6" s="107"/>
-      <c r="I6" s="108"/>
-      <c r="V6" s="106" t="s">
+      <c r="H6" s="111"/>
+      <c r="I6" s="112"/>
+      <c r="V6" s="110" t="s">
         <v>176</v>
       </c>
-      <c r="W6" s="107"/>
-      <c r="X6" s="108"/>
-    </row>
-    <row r="7" spans="2:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="W6" s="111"/>
+      <c r="X6" s="112"/>
+    </row>
+    <row r="7" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -3626,18 +3657,18 @@
       <c r="D8" s="21"/>
       <c r="E8" s="21"/>
       <c r="F8" s="21"/>
-      <c r="G8" s="97" t="e">
+      <c r="G8" s="101">
         <f>AVERAGE(G43:G50)*5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H8" s="98"/>
-      <c r="I8" s="99"/>
-      <c r="V8" s="97" t="e">
+        <v>0.625</v>
+      </c>
+      <c r="H8" s="102"/>
+      <c r="I8" s="103"/>
+      <c r="V8" s="101">
         <f>AVERAGE(K43:K50)*5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W8" s="98"/>
-      <c r="X8" s="99"/>
+        <v>0</v>
+      </c>
+      <c r="W8" s="102"/>
+      <c r="X8" s="103"/>
     </row>
     <row r="9" spans="2:24" ht="91" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="22"/>
@@ -3645,12 +3676,12 @@
       <c r="D9" s="22"/>
       <c r="E9" s="22"/>
       <c r="F9" s="22"/>
-      <c r="G9" s="100"/>
-      <c r="H9" s="101"/>
-      <c r="I9" s="102"/>
-      <c r="V9" s="100"/>
-      <c r="W9" s="101"/>
-      <c r="X9" s="102"/>
+      <c r="G9" s="104"/>
+      <c r="H9" s="105"/>
+      <c r="I9" s="106"/>
+      <c r="V9" s="104"/>
+      <c r="W9" s="105"/>
+      <c r="X9" s="106"/>
     </row>
     <row r="10" spans="2:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="14"/>
@@ -3658,12 +3689,12 @@
       <c r="D10" s="14"/>
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
-      <c r="G10" s="100"/>
-      <c r="H10" s="101"/>
-      <c r="I10" s="102"/>
-      <c r="V10" s="100"/>
-      <c r="W10" s="101"/>
-      <c r="X10" s="102"/>
+      <c r="G10" s="104"/>
+      <c r="H10" s="105"/>
+      <c r="I10" s="106"/>
+      <c r="V10" s="104"/>
+      <c r="W10" s="105"/>
+      <c r="X10" s="106"/>
     </row>
     <row r="11" spans="2:24" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B11" s="14"/>
@@ -3671,56 +3702,56 @@
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
-      <c r="G11" s="103"/>
-      <c r="H11" s="104"/>
-      <c r="I11" s="105"/>
-      <c r="V11" s="103"/>
-      <c r="W11" s="104"/>
-      <c r="X11" s="105"/>
-    </row>
-    <row r="12" spans="2:24" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="109"/>
-      <c r="C12" s="109"/>
-      <c r="D12" s="109"/>
-      <c r="E12" s="109"/>
-      <c r="F12" s="109"/>
-    </row>
-    <row r="13" spans="2:24" ht="15" x14ac:dyDescent="0.2">
+      <c r="G11" s="107"/>
+      <c r="H11" s="108"/>
+      <c r="I11" s="109"/>
+      <c r="V11" s="107"/>
+      <c r="W11" s="108"/>
+      <c r="X11" s="109"/>
+    </row>
+    <row r="12" spans="2:24" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B12" s="96"/>
+      <c r="C12" s="96"/>
+      <c r="D12" s="96"/>
+      <c r="E12" s="96"/>
+      <c r="F12" s="96"/>
+    </row>
+    <row r="13" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B13" s="15"/>
       <c r="C13" s="15"/>
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
     </row>
-    <row r="14" spans="2:24" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B14" s="16"/>
       <c r="C14" s="16"/>
       <c r="D14" s="16"/>
       <c r="E14" s="16"/>
       <c r="F14" s="17"/>
     </row>
-    <row r="15" spans="2:24" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
       <c r="E15" s="14"/>
       <c r="F15" s="14"/>
     </row>
-    <row r="16" spans="2:24" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="109"/>
-      <c r="C16" s="109"/>
-      <c r="D16" s="109"/>
-      <c r="E16" s="109"/>
-      <c r="F16" s="109"/>
-    </row>
-    <row r="17" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:24" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B16" s="96"/>
+      <c r="C16" s="96"/>
+      <c r="D16" s="96"/>
+      <c r="E16" s="96"/>
+      <c r="F16" s="96"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
     </row>
-    <row r="18" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B18" s="16"/>
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
@@ -3764,18 +3795,18 @@
     </row>
     <row r="35" spans="3:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="41" spans="3:11" x14ac:dyDescent="0.15">
-      <c r="D41" s="110" t="s">
+      <c r="D41" s="97" t="s">
         <v>174</v>
       </c>
-      <c r="E41" s="111"/>
-      <c r="F41" s="111"/>
-      <c r="G41" s="112"/>
-      <c r="H41" s="110" t="s">
+      <c r="E41" s="98"/>
+      <c r="F41" s="98"/>
+      <c r="G41" s="99"/>
+      <c r="H41" s="97" t="s">
         <v>175</v>
       </c>
-      <c r="I41" s="111"/>
-      <c r="J41" s="111"/>
-      <c r="K41" s="112"/>
+      <c r="I41" s="98"/>
+      <c r="J41" s="98"/>
+      <c r="K41" s="99"/>
     </row>
     <row r="42" spans="3:11" x14ac:dyDescent="0.15">
       <c r="D42" s="18" t="s">
@@ -3820,7 +3851,7 @@
         <v>6</v>
       </c>
       <c r="G43" s="20">
-        <f>D43/(E43+D43)</f>
+        <f t="shared" ref="G43:G49" si="0">IF(D43+E43=0, 0, D43/(E43+D43))</f>
         <v>1</v>
       </c>
       <c r="H43" s="10">
@@ -3835,9 +3866,9 @@
         <f>COUNTIFS('Security Requirements - iOS'!F5:F14,'Security Requirements - Android'!B81)</f>
         <v>6</v>
       </c>
-      <c r="K43" s="20" t="e">
-        <f>H43/(H43+I43)</f>
-        <v>#DIV/0!</v>
+      <c r="K43" s="20">
+        <f t="shared" ref="K43:K49" si="1">IF(H43+I43=0, 0, H43/(H43+I43))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="3:11" x14ac:dyDescent="0.15">
@@ -3856,25 +3887,25 @@
         <f>COUNTIFS('Security Requirements - Android'!F16:F27,'Security Requirements - Android'!B81)</f>
         <v>5</v>
       </c>
-      <c r="G44" s="20" t="e">
-        <f t="shared" ref="G44:G50" si="0">D44/(E44+D44)</f>
-        <v>#DIV/0!</v>
+      <c r="G44" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="H44" s="10">
-        <f>COUNTIFS('Security Requirements - iOS'!F17:F27,'Security Requirements - Android'!B79)</f>
+        <f>COUNTIFS('Security Requirements - iOS'!F16:F27,'Security Requirements - Android'!B79)</f>
         <v>0</v>
       </c>
       <c r="I44" s="10">
-        <f>COUNTIFS('Security Requirements - iOS'!F17:F27,'Security Requirements - Android'!B80)</f>
+        <f>COUNTIFS('Security Requirements - iOS'!F16:F27,'Security Requirements - Android'!B80)</f>
         <v>0</v>
       </c>
       <c r="J44" s="10">
-        <f>COUNTIFS('Security Requirements - iOS'!F17:F27,'Security Requirements - Android'!B81)</f>
+        <f>COUNTIFS('Security Requirements - iOS'!F16:F27,'Security Requirements - Android'!B81)</f>
         <v>5</v>
       </c>
-      <c r="K44" s="20" t="e">
-        <f t="shared" ref="K44:K50" si="1">H44/(H44+I44)</f>
-        <v>#DIV/0!</v>
+      <c r="K44" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="3:11" x14ac:dyDescent="0.15">
@@ -3893,9 +3924,9 @@
         <f>COUNTIFS('Security Requirements - Android'!F29:F34,'Security Requirements - Android'!B81)</f>
         <v>0</v>
       </c>
-      <c r="G45" s="20" t="e">
+      <c r="G45" s="20">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="H45" s="10">
         <f>COUNTIFS('Security Requirements - iOS'!F29:F34,'Security Requirements - Android'!B79)</f>
@@ -3909,9 +3940,9 @@
         <f>COUNTIFS('Security Requirements - iOS'!F29:F34,'Security Requirements - Android'!B81)</f>
         <v>0</v>
       </c>
-      <c r="K45" s="20" t="e">
+      <c r="K45" s="20">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="3:11" x14ac:dyDescent="0.15">
@@ -3930,9 +3961,9 @@
         <f>COUNTIFS('Security Requirements - Android'!F36:F46,'Security Requirements - Android'!B81)</f>
         <v>5</v>
       </c>
-      <c r="G46" s="20" t="e">
+      <c r="G46" s="20">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="H46" s="10">
         <f>COUNTIFS('Security Requirements - iOS'!F36:F46,'Security Requirements - Android'!B79)</f>
@@ -3946,9 +3977,9 @@
         <f>COUNTIFS('Security Requirements - iOS'!F36:F46,'Security Requirements - Android'!B81)</f>
         <v>5</v>
       </c>
-      <c r="K46" s="20" t="e">
+      <c r="K46" s="20">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="3:11" x14ac:dyDescent="0.15">
@@ -3967,9 +3998,9 @@
         <f>COUNTIFS('Security Requirements - Android'!F48:F53,'Security Requirements - Android'!B81)</f>
         <v>3</v>
       </c>
-      <c r="G47" s="20" t="e">
+      <c r="G47" s="20">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="H47" s="10">
         <f>COUNTIFS('Security Requirements - iOS'!F48:F53,'Security Requirements - Android'!B79)</f>
@@ -3983,9 +4014,9 @@
         <f>COUNTIFS('Security Requirements - iOS'!F48:F53,'Security Requirements - Android'!B81)</f>
         <v>3</v>
       </c>
-      <c r="K47" s="20" t="e">
+      <c r="K47" s="20">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="3:11" x14ac:dyDescent="0.15">
@@ -4004,9 +4035,9 @@
         <f>COUNTIFS('Security Requirements - Android'!F55:F62,'Security Requirements - Android'!B81)</f>
         <v>0</v>
       </c>
-      <c r="G48" s="20" t="e">
+      <c r="G48" s="20">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="H48" s="10">
         <f>COUNTIFS('Security Requirements - iOS'!F55:F62,'Security Requirements - Android'!B79)</f>
@@ -4020,9 +4051,9 @@
         <f>COUNTIFS('Security Requirements - iOS'!F55:F62,'Security Requirements - Android'!B81)</f>
         <v>0</v>
       </c>
-      <c r="K48" s="20" t="e">
+      <c r="K48" s="20">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="3:11" x14ac:dyDescent="0.15">
@@ -4041,9 +4072,9 @@
         <f>COUNTIFS('Security Requirements - Android'!F64:F72,'Security Requirements - Android'!B81)</f>
         <v>0</v>
       </c>
-      <c r="G49" s="20" t="e">
+      <c r="G49" s="20">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="H49" s="10">
         <f>COUNTIFS('Security Requirements - iOS'!F64:F72,'Security Requirements - Android'!B79)</f>
@@ -4057,9 +4088,9 @@
         <f>COUNTIFS('Security Requirements - iOS'!F64:F72,'Security Requirements - Android'!B81)</f>
         <v>0</v>
       </c>
-      <c r="K49" s="20" t="e">
+      <c r="K49" s="20">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="3:11" x14ac:dyDescent="0.15">
@@ -4078,9 +4109,9 @@
         <f>COUNTIFS('Anti-RE - Android'!E4:E18,'Security Requirements - Android'!B81)</f>
         <v>12</v>
       </c>
-      <c r="G50" s="20" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="G50" s="20">
+        <f>IF(D50+E50=0, 0, D50/(E50+D50))</f>
+        <v>0</v>
       </c>
       <c r="H50" s="10">
         <f>COUNTIFS('Anti-RE - iOS'!E4:E18,'Security Requirements - Android'!B79)</f>
@@ -4094,13 +4125,15 @@
         <f>COUNTIFS('Anti-RE - iOS'!E4:E18,'Security Requirements - Android'!B81)</f>
         <v>12</v>
       </c>
-      <c r="K50" s="20" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="K50" s="20">
+        <f>IF(H50+I50=0, 0, H50/(H50+I50))</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="V6:X6"/>
+    <mergeCell ref="V8:X11"/>
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="B16:F16"/>
     <mergeCell ref="D41:G41"/>
@@ -4108,8 +4141,6 @@
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="G8:I11"/>
     <mergeCell ref="G6:I6"/>
-    <mergeCell ref="V6:X6"/>
-    <mergeCell ref="V8:X11"/>
   </mergeCells>
   <conditionalFormatting sqref="F14">
     <cfRule type="iconSet" priority="3">
@@ -4146,1542 +4177,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J85"/>
-  <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="1.83203125" customWidth="1"/>
-    <col min="2" max="2" width="8" customWidth="1"/>
-    <col min="3" max="3" width="96.6640625" style="61" customWidth="1"/>
-    <col min="7" max="7" width="53.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.83203125" customWidth="1"/>
-    <col min="10" max="11" width="10.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:8" ht="19" x14ac:dyDescent="0.2">
-      <c r="B1" s="113" t="s">
-        <v>177</v>
-      </c>
-      <c r="C1" s="113"/>
-      <c r="D1" s="113"/>
-      <c r="E1" s="113"/>
-      <c r="F1" s="113"/>
-      <c r="G1" s="113"/>
-      <c r="H1" s="113"/>
-    </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B2" s="50"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B3" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="29" t="s">
-        <v>166</v>
-      </c>
-      <c r="G3" s="29" t="s">
-        <v>180</v>
-      </c>
-      <c r="H3" s="30" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B4" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="34"/>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B5" s="35" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="36" t="s">
-        <v>48</v>
-      </c>
-      <c r="D5" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="37" t="s">
-        <v>168</v>
-      </c>
-      <c r="G5" s="52" t="s">
-        <v>192</v>
-      </c>
-      <c r="H5" s="74"/>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B6" s="35">
-        <v>1.2</v>
-      </c>
-      <c r="C6" s="36" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="37"/>
-      <c r="G6" s="52" t="s">
-        <v>192</v>
-      </c>
-      <c r="H6" s="74"/>
-    </row>
-    <row r="7" spans="2:8" ht="30" x14ac:dyDescent="0.2">
-      <c r="B7" s="35">
-        <v>1.3</v>
-      </c>
-      <c r="C7" s="36" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="37"/>
-      <c r="G7" s="52" t="s">
-        <v>192</v>
-      </c>
-      <c r="H7" s="74"/>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B8" s="35">
-        <v>1.4</v>
-      </c>
-      <c r="C8" s="36" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="37"/>
-      <c r="G8" s="52" t="s">
-        <v>192</v>
-      </c>
-      <c r="H8" s="74"/>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B9" s="35">
-        <v>1.5</v>
-      </c>
-      <c r="C9" s="36" t="s">
-        <v>47</v>
-      </c>
-      <c r="D9" s="36"/>
-      <c r="E9" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="37" t="s">
-        <v>138</v>
-      </c>
-      <c r="G9" s="52" t="s">
-        <v>192</v>
-      </c>
-      <c r="H9" s="74"/>
-    </row>
-    <row r="10" spans="2:8" ht="30" x14ac:dyDescent="0.2">
-      <c r="B10" s="35">
-        <v>1.6</v>
-      </c>
-      <c r="C10" s="36" t="s">
-        <v>46</v>
-      </c>
-      <c r="D10" s="36"/>
-      <c r="E10" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="37" t="s">
-        <v>138</v>
-      </c>
-      <c r="G10" s="52" t="s">
-        <v>192</v>
-      </c>
-      <c r="H10" s="74"/>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B11" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="D11" s="53"/>
-      <c r="E11" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11" s="37" t="s">
-        <v>138</v>
-      </c>
-      <c r="G11" s="52" t="s">
-        <v>192</v>
-      </c>
-      <c r="H11" s="74"/>
-    </row>
-    <row r="12" spans="2:8" ht="30" x14ac:dyDescent="0.2">
-      <c r="B12" s="35">
-        <v>1.8</v>
-      </c>
-      <c r="C12" s="36" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12" s="36"/>
-      <c r="E12" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F12" s="37" t="s">
-        <v>138</v>
-      </c>
-      <c r="G12" s="52" t="s">
-        <v>192</v>
-      </c>
-      <c r="H12" s="74"/>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B13" s="35">
-        <v>1.9</v>
-      </c>
-      <c r="C13" s="36" t="s">
-        <v>285</v>
-      </c>
-      <c r="D13" s="36"/>
-      <c r="E13" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13" s="37" t="s">
-        <v>138</v>
-      </c>
-      <c r="G13" s="52" t="s">
-        <v>192</v>
-      </c>
-      <c r="H13" s="74"/>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B14" s="71" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="36" t="s">
-        <v>286</v>
-      </c>
-      <c r="D14" s="36"/>
-      <c r="E14" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F14" s="37" t="s">
-        <v>138</v>
-      </c>
-      <c r="G14" s="52" t="s">
-        <v>192</v>
-      </c>
-      <c r="H14" s="74"/>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B15" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="39" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" s="39"/>
-      <c r="E15" s="54"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="40"/>
-    </row>
-    <row r="16" spans="2:8" ht="30" x14ac:dyDescent="0.2">
-      <c r="B16" s="55" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="56" t="s">
-        <v>70</v>
-      </c>
-      <c r="D16" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F16" s="37"/>
-      <c r="G16" s="58" t="s">
-        <v>188</v>
-      </c>
-      <c r="H16" s="74"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B17" s="55" t="s">
-        <v>65</v>
-      </c>
-      <c r="C17" s="56" t="s">
-        <v>71</v>
-      </c>
-      <c r="D17" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F17" s="37"/>
-      <c r="G17" s="58" t="s">
-        <v>189</v>
-      </c>
-      <c r="H17" s="74"/>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B18" s="55" t="s">
-        <v>66</v>
-      </c>
-      <c r="C18" s="56" t="s">
-        <v>72</v>
-      </c>
-      <c r="D18" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F18" s="37"/>
-      <c r="G18" s="58" t="s">
-        <v>190</v>
-      </c>
-      <c r="H18" s="74"/>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B19" s="55" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19" s="56" t="s">
-        <v>73</v>
-      </c>
-      <c r="D19" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F19" s="37"/>
-      <c r="G19" s="58" t="s">
-        <v>191</v>
-      </c>
-      <c r="H19" s="74"/>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B20" s="55" t="s">
-        <v>67</v>
-      </c>
-      <c r="C20" s="56" t="s">
-        <v>74</v>
-      </c>
-      <c r="D20" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F20" s="37"/>
-      <c r="G20" s="58" t="s">
-        <v>193</v>
-      </c>
-      <c r="H20" s="74"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B21" s="55" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" s="56" t="s">
-        <v>75</v>
-      </c>
-      <c r="D21" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F21" s="37"/>
-      <c r="G21" s="58" t="s">
-        <v>194</v>
-      </c>
-      <c r="H21" s="74"/>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B22" s="55" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" s="56" t="s">
-        <v>287</v>
-      </c>
-      <c r="D22" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F22" s="37"/>
-      <c r="G22" s="58" t="s">
-        <v>251</v>
-      </c>
-      <c r="H22" s="74"/>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B23" s="55" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" s="56" t="s">
-        <v>288</v>
-      </c>
-      <c r="D23" s="56"/>
-      <c r="E23" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F23" s="37" t="s">
-        <v>138</v>
-      </c>
-      <c r="G23" s="58" t="s">
-        <v>195</v>
-      </c>
-      <c r="H23" s="74"/>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B24" s="55" t="s">
-        <v>16</v>
-      </c>
-      <c r="C24" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="D24" s="56"/>
-      <c r="E24" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F24" s="37" t="s">
-        <v>138</v>
-      </c>
-      <c r="G24" s="58" t="s">
-        <v>196</v>
-      </c>
-      <c r="H24" s="74"/>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B25" s="55" t="s">
-        <v>68</v>
-      </c>
-      <c r="C25" s="56" t="s">
-        <v>77</v>
-      </c>
-      <c r="D25" s="56"/>
-      <c r="E25" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F25" s="37" t="s">
-        <v>138</v>
-      </c>
-      <c r="G25" s="58" t="s">
-        <v>197</v>
-      </c>
-      <c r="H25" s="74"/>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B26" s="55" t="s">
-        <v>69</v>
-      </c>
-      <c r="C26" s="56" t="s">
-        <v>78</v>
-      </c>
-      <c r="D26" s="56"/>
-      <c r="E26" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F26" s="37" t="s">
-        <v>138</v>
-      </c>
-      <c r="G26" s="58" t="s">
-        <v>198</v>
-      </c>
-      <c r="H26" s="74"/>
-    </row>
-    <row r="27" spans="2:8" ht="30" x14ac:dyDescent="0.2">
-      <c r="B27" s="55" t="s">
-        <v>17</v>
-      </c>
-      <c r="C27" s="56" t="s">
-        <v>127</v>
-      </c>
-      <c r="D27" s="56"/>
-      <c r="E27" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F27" s="37" t="s">
-        <v>138</v>
-      </c>
-      <c r="G27" s="58" t="s">
-        <v>199</v>
-      </c>
-      <c r="H27" s="74"/>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B28" s="38" t="s">
-        <v>18</v>
-      </c>
-      <c r="C28" s="39" t="s">
-        <v>79</v>
-      </c>
-      <c r="D28" s="39"/>
-      <c r="E28" s="54"/>
-      <c r="F28" s="39"/>
-      <c r="G28" s="39"/>
-      <c r="H28" s="40"/>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B29" s="55" t="s">
-        <v>19</v>
-      </c>
-      <c r="C29" s="56" t="s">
-        <v>80</v>
-      </c>
-      <c r="D29" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E29" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F29" s="37"/>
-      <c r="G29" s="58" t="s">
-        <v>200</v>
-      </c>
-      <c r="H29" s="74"/>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B30" s="55" t="s">
-        <v>20</v>
-      </c>
-      <c r="C30" s="56" t="s">
-        <v>81</v>
-      </c>
-      <c r="D30" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E30" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F30" s="37"/>
-      <c r="G30" s="58" t="s">
-        <v>201</v>
-      </c>
-      <c r="H30" s="74"/>
-    </row>
-    <row r="31" spans="2:8" ht="30" x14ac:dyDescent="0.2">
-      <c r="B31" s="55" t="s">
-        <v>21</v>
-      </c>
-      <c r="C31" s="56" t="s">
-        <v>82</v>
-      </c>
-      <c r="D31" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E31" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F31" s="37"/>
-      <c r="G31" s="58" t="s">
-        <v>202</v>
-      </c>
-      <c r="H31" s="74"/>
-    </row>
-    <row r="32" spans="2:8" ht="30" x14ac:dyDescent="0.2">
-      <c r="B32" s="55" t="s">
-        <v>22</v>
-      </c>
-      <c r="C32" s="56" t="s">
-        <v>128</v>
-      </c>
-      <c r="D32" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E32" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F32" s="37"/>
-      <c r="G32" s="58" t="s">
-        <v>203</v>
-      </c>
-      <c r="H32" s="74"/>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B33" s="55" t="s">
-        <v>23</v>
-      </c>
-      <c r="C33" s="56" t="s">
-        <v>83</v>
-      </c>
-      <c r="D33" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E33" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F33" s="37"/>
-      <c r="G33" s="58" t="s">
-        <v>204</v>
-      </c>
-      <c r="H33" s="74"/>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B34" s="55" t="s">
-        <v>24</v>
-      </c>
-      <c r="C34" s="56" t="s">
-        <v>84</v>
-      </c>
-      <c r="D34" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E34" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F34" s="37"/>
-      <c r="G34" s="58" t="s">
-        <v>200</v>
-      </c>
-      <c r="H34" s="74"/>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B35" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="C35" s="39" t="s">
-        <v>85</v>
-      </c>
-      <c r="D35" s="39"/>
-      <c r="E35" s="54"/>
-      <c r="F35" s="39"/>
-      <c r="G35" s="39"/>
-      <c r="H35" s="40"/>
-    </row>
-    <row r="36" spans="2:10" ht="30" x14ac:dyDescent="0.2">
-      <c r="B36" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="C36" s="56" t="s">
-        <v>90</v>
-      </c>
-      <c r="D36" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E36" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F36" s="37"/>
-      <c r="G36" s="58" t="s">
-        <v>205</v>
-      </c>
-      <c r="H36" s="74"/>
-    </row>
-    <row r="37" spans="2:10" ht="30" x14ac:dyDescent="0.2">
-      <c r="B37" s="55" t="s">
-        <v>86</v>
-      </c>
-      <c r="C37" s="56" t="s">
-        <v>274</v>
-      </c>
-      <c r="D37" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E37" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F37" s="37"/>
-      <c r="G37" s="58" t="s">
-        <v>206</v>
-      </c>
-      <c r="H37" s="74"/>
-    </row>
-    <row r="38" spans="2:10" ht="30" x14ac:dyDescent="0.2">
-      <c r="B38" s="55" t="s">
-        <v>87</v>
-      </c>
-      <c r="C38" s="56" t="s">
-        <v>272</v>
-      </c>
-      <c r="D38" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E38" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F38" s="37"/>
-      <c r="G38" s="58" t="s">
-        <v>206</v>
-      </c>
-      <c r="H38" s="74"/>
-      <c r="J38" s="58"/>
-    </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B39" s="55" t="s">
-        <v>27</v>
-      </c>
-      <c r="C39" s="56" t="s">
-        <v>289</v>
-      </c>
-      <c r="D39" s="26"/>
-      <c r="E39" s="51"/>
-      <c r="F39" s="37"/>
-      <c r="G39" s="58" t="s">
-        <v>208</v>
-      </c>
-      <c r="H39" s="74"/>
-      <c r="J39" s="58"/>
-    </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B40" s="55" t="s">
-        <v>28</v>
-      </c>
-      <c r="C40" s="56" t="s">
-        <v>91</v>
-      </c>
-      <c r="D40" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E40" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F40" s="37"/>
-      <c r="G40" s="58" t="s">
-        <v>207</v>
-      </c>
-      <c r="H40" s="74"/>
-    </row>
-    <row r="41" spans="2:10" ht="30" x14ac:dyDescent="0.2">
-      <c r="B41" s="55" t="s">
-        <v>88</v>
-      </c>
-      <c r="C41" s="56" t="s">
-        <v>293</v>
-      </c>
-      <c r="D41" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E41" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F41" s="37"/>
-      <c r="G41" s="58" t="s">
-        <v>209</v>
-      </c>
-      <c r="H41" s="74"/>
-    </row>
-    <row r="42" spans="2:10" ht="30" x14ac:dyDescent="0.2">
-      <c r="B42" s="55" t="s">
-        <v>89</v>
-      </c>
-      <c r="C42" s="56" t="s">
-        <v>92</v>
-      </c>
-      <c r="D42" s="56"/>
-      <c r="E42" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F42" s="37" t="s">
-        <v>138</v>
-      </c>
-      <c r="G42" s="58" t="s">
-        <v>210</v>
-      </c>
-      <c r="H42" s="74"/>
-    </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B43" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="C43" s="56" t="s">
-        <v>290</v>
-      </c>
-      <c r="D43" s="56"/>
-      <c r="E43" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F43" s="37" t="s">
-        <v>138</v>
-      </c>
-      <c r="G43" s="58" t="s">
-        <v>211</v>
-      </c>
-      <c r="H43" s="74"/>
-    </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B44" s="55" t="s">
-        <v>30</v>
-      </c>
-      <c r="C44" s="56" t="s">
-        <v>93</v>
-      </c>
-      <c r="D44" s="56"/>
-      <c r="E44" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F44" s="37" t="s">
-        <v>138</v>
-      </c>
-      <c r="G44" s="58" t="s">
-        <v>212</v>
-      </c>
-      <c r="H44" s="74"/>
-    </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B45" s="55" t="s">
-        <v>31</v>
-      </c>
-      <c r="C45" s="56" t="s">
-        <v>94</v>
-      </c>
-      <c r="D45" s="56"/>
-      <c r="E45" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F45" s="37" t="s">
-        <v>138</v>
-      </c>
-      <c r="G45" s="58" t="s">
-        <v>213</v>
-      </c>
-      <c r="H45" s="74"/>
-    </row>
-    <row r="46" spans="2:10" ht="30" x14ac:dyDescent="0.2">
-      <c r="B46" s="55" t="s">
-        <v>273</v>
-      </c>
-      <c r="C46" s="56" t="s">
-        <v>95</v>
-      </c>
-      <c r="D46" s="56"/>
-      <c r="E46" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F46" s="37" t="s">
-        <v>138</v>
-      </c>
-      <c r="G46" s="58" t="s">
-        <v>214</v>
-      </c>
-      <c r="H46" s="74"/>
-    </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B47" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="C47" s="39" t="s">
-        <v>96</v>
-      </c>
-      <c r="D47" s="39"/>
-      <c r="E47" s="54"/>
-      <c r="F47" s="39"/>
-      <c r="G47" s="39"/>
-      <c r="H47" s="40"/>
-    </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B48" s="55" t="s">
-        <v>33</v>
-      </c>
-      <c r="C48" s="56" t="s">
-        <v>99</v>
-      </c>
-      <c r="D48" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E48" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F48" s="37"/>
-      <c r="G48" s="58" t="s">
-        <v>215</v>
-      </c>
-      <c r="H48" s="74"/>
-    </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B49" s="55" t="s">
-        <v>97</v>
-      </c>
-      <c r="C49" s="56" t="s">
-        <v>129</v>
-      </c>
-      <c r="D49" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E49" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F49" s="37"/>
-      <c r="G49" s="58" t="s">
-        <v>216</v>
-      </c>
-      <c r="H49" s="74"/>
-    </row>
-    <row r="50" spans="2:8" ht="30" x14ac:dyDescent="0.2">
-      <c r="B50" s="55" t="s">
-        <v>34</v>
-      </c>
-      <c r="C50" s="56" t="s">
-        <v>100</v>
-      </c>
-      <c r="D50" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E50" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F50" s="37"/>
-      <c r="G50" s="58" t="s">
-        <v>217</v>
-      </c>
-      <c r="H50" s="74"/>
-    </row>
-    <row r="51" spans="2:8" ht="30" x14ac:dyDescent="0.2">
-      <c r="B51" s="55" t="s">
-        <v>98</v>
-      </c>
-      <c r="C51" s="56" t="s">
-        <v>101</v>
-      </c>
-      <c r="D51" s="56"/>
-      <c r="E51" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F51" s="37" t="s">
-        <v>138</v>
-      </c>
-      <c r="G51" s="58" t="s">
-        <v>218</v>
-      </c>
-      <c r="H51" s="74"/>
-    </row>
-    <row r="52" spans="2:8" ht="30" x14ac:dyDescent="0.2">
-      <c r="B52" s="55" t="s">
-        <v>35</v>
-      </c>
-      <c r="C52" s="56" t="s">
-        <v>102</v>
-      </c>
-      <c r="D52" s="56"/>
-      <c r="E52" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F52" s="37" t="s">
-        <v>138</v>
-      </c>
-      <c r="G52" s="58" t="s">
-        <v>219</v>
-      </c>
-      <c r="H52" s="74"/>
-    </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B53" s="55">
-        <v>5.6</v>
-      </c>
-      <c r="C53" s="56" t="s">
-        <v>269</v>
-      </c>
-      <c r="D53" s="56"/>
-      <c r="E53" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F53" s="37" t="s">
-        <v>138</v>
-      </c>
-      <c r="G53" s="58" t="s">
-        <v>270</v>
-      </c>
-      <c r="H53" s="74"/>
-    </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B54" s="38" t="s">
-        <v>36</v>
-      </c>
-      <c r="C54" s="39" t="s">
-        <v>236</v>
-      </c>
-      <c r="D54" s="39"/>
-      <c r="E54" s="54"/>
-      <c r="F54" s="39"/>
-      <c r="G54" s="39"/>
-      <c r="H54" s="40"/>
-    </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B55" s="55" t="s">
-        <v>103</v>
-      </c>
-      <c r="C55" s="56" t="s">
-        <v>109</v>
-      </c>
-      <c r="D55" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E55" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F55" s="37"/>
-      <c r="G55" s="58" t="s">
-        <v>220</v>
-      </c>
-      <c r="H55" s="74"/>
-    </row>
-    <row r="56" spans="2:8" ht="30" x14ac:dyDescent="0.2">
-      <c r="B56" s="55" t="s">
-        <v>104</v>
-      </c>
-      <c r="C56" s="56" t="s">
-        <v>110</v>
-      </c>
-      <c r="D56" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E56" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F56" s="37"/>
-      <c r="G56" s="58" t="s">
-        <v>221</v>
-      </c>
-      <c r="H56" s="74"/>
-    </row>
-    <row r="57" spans="2:8" ht="30" x14ac:dyDescent="0.2">
-      <c r="B57" s="55" t="s">
-        <v>105</v>
-      </c>
-      <c r="C57" s="56" t="s">
-        <v>111</v>
-      </c>
-      <c r="D57" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E57" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F57" s="37"/>
-      <c r="G57" s="58" t="s">
-        <v>222</v>
-      </c>
-      <c r="H57" s="74"/>
-    </row>
-    <row r="58" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B58" s="55" t="s">
-        <v>106</v>
-      </c>
-      <c r="C58" s="56" t="s">
-        <v>112</v>
-      </c>
-      <c r="D58" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E58" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F58" s="37"/>
-      <c r="G58" s="58" t="s">
-        <v>223</v>
-      </c>
-      <c r="H58" s="74"/>
-    </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B59" s="55" t="s">
-        <v>107</v>
-      </c>
-      <c r="C59" s="56" t="s">
-        <v>113</v>
-      </c>
-      <c r="D59" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E59" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F59" s="37"/>
-      <c r="G59" s="58" t="s">
-        <v>224</v>
-      </c>
-      <c r="H59" s="74"/>
-    </row>
-    <row r="60" spans="2:8" ht="30" x14ac:dyDescent="0.2">
-      <c r="B60" s="55" t="s">
-        <v>108</v>
-      </c>
-      <c r="C60" s="56" t="s">
-        <v>114</v>
-      </c>
-      <c r="D60" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E60" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F60" s="37"/>
-      <c r="G60" s="58" t="s">
-        <v>225</v>
-      </c>
-      <c r="H60" s="74"/>
-    </row>
-    <row r="61" spans="2:8" ht="30" x14ac:dyDescent="0.2">
-      <c r="B61" s="55" t="s">
-        <v>291</v>
-      </c>
-      <c r="C61" s="56" t="s">
-        <v>268</v>
-      </c>
-      <c r="D61" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E61" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F61" s="37"/>
-      <c r="G61" s="58" t="s">
-        <v>226</v>
-      </c>
-      <c r="H61" s="74"/>
-    </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B62" s="55">
-        <v>6.8</v>
-      </c>
-      <c r="C62" s="56" t="s">
-        <v>115</v>
-      </c>
-      <c r="D62" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E62" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F62" s="37"/>
-      <c r="G62" s="58" t="s">
-        <v>227</v>
-      </c>
-      <c r="H62" s="74"/>
-    </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B63" s="38" t="s">
-        <v>37</v>
-      </c>
-      <c r="C63" s="39" t="s">
-        <v>120</v>
-      </c>
-      <c r="D63" s="39"/>
-      <c r="E63" s="54"/>
-      <c r="F63" s="39"/>
-      <c r="G63" s="39"/>
-      <c r="H63" s="40"/>
-    </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B64" s="55" t="s">
-        <v>116</v>
-      </c>
-      <c r="C64" s="56" t="s">
-        <v>121</v>
-      </c>
-      <c r="D64" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E64" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F64" s="37"/>
-      <c r="G64" s="58" t="s">
-        <v>228</v>
-      </c>
-      <c r="H64" s="74"/>
-    </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B65" s="55" t="s">
-        <v>38</v>
-      </c>
-      <c r="C65" s="56" t="s">
-        <v>122</v>
-      </c>
-      <c r="D65" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E65" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F65" s="37"/>
-      <c r="G65" s="58" t="s">
-        <v>229</v>
-      </c>
-      <c r="H65" s="74"/>
-    </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B66" s="55" t="s">
-        <v>117</v>
-      </c>
-      <c r="C66" s="56" t="s">
-        <v>123</v>
-      </c>
-      <c r="D66" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E66" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F66" s="37"/>
-      <c r="G66" s="58" t="s">
-        <v>230</v>
-      </c>
-      <c r="H66" s="74"/>
-    </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B67" s="55" t="s">
-        <v>118</v>
-      </c>
-      <c r="C67" s="56" t="s">
-        <v>124</v>
-      </c>
-      <c r="D67" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E67" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F67" s="37"/>
-      <c r="G67" s="58" t="s">
-        <v>231</v>
-      </c>
-      <c r="H67" s="74"/>
-    </row>
-    <row r="68" spans="2:8" ht="30" x14ac:dyDescent="0.2">
-      <c r="B68" s="55" t="s">
-        <v>119</v>
-      </c>
-      <c r="C68" s="56" t="s">
-        <v>283</v>
-      </c>
-      <c r="D68" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E68" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F68" s="37"/>
-      <c r="G68" s="58" t="s">
-        <v>284</v>
-      </c>
-      <c r="H68" s="74"/>
-    </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B69" s="55" t="s">
-        <v>39</v>
-      </c>
-      <c r="C69" s="56" t="s">
-        <v>125</v>
-      </c>
-      <c r="D69" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E69" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F69" s="37"/>
-      <c r="G69" s="58" t="s">
-        <v>233</v>
-      </c>
-      <c r="H69" s="74"/>
-    </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B70" s="55" t="s">
-        <v>40</v>
-      </c>
-      <c r="C70" s="56" t="s">
-        <v>42</v>
-      </c>
-      <c r="D70" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E70" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F70" s="37"/>
-      <c r="G70" s="58" t="s">
-        <v>234</v>
-      </c>
-      <c r="H70" s="74"/>
-    </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B71" s="55" t="s">
-        <v>41</v>
-      </c>
-      <c r="C71" s="56" t="s">
-        <v>126</v>
-      </c>
-      <c r="D71" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E71" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F71" s="37"/>
-      <c r="G71" s="58" t="s">
-        <v>235</v>
-      </c>
-      <c r="H71" s="74"/>
-    </row>
-    <row r="72" spans="2:8" ht="30" x14ac:dyDescent="0.2">
-      <c r="B72" s="55" t="s">
-        <v>282</v>
-      </c>
-      <c r="C72" s="56" t="s">
-        <v>264</v>
-      </c>
-      <c r="D72" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E72" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F72" s="37"/>
-      <c r="G72" s="58" t="s">
-        <v>271</v>
-      </c>
-      <c r="H72" s="74"/>
-    </row>
-    <row r="73" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B73" s="41"/>
-      <c r="C73" s="42"/>
-      <c r="D73" s="43"/>
-      <c r="E73" s="43"/>
-      <c r="F73" s="43"/>
-      <c r="G73" s="43"/>
-      <c r="H73" s="44"/>
-    </row>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B74" s="45"/>
-      <c r="C74" s="47"/>
-      <c r="D74" s="45"/>
-      <c r="E74" s="45"/>
-      <c r="F74" s="45"/>
-      <c r="G74" s="45"/>
-      <c r="H74" s="45"/>
-    </row>
-    <row r="75" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B75" s="45"/>
-      <c r="C75" s="56"/>
-      <c r="D75" s="45"/>
-      <c r="E75" s="45"/>
-      <c r="F75" s="45"/>
-      <c r="G75" s="45"/>
-      <c r="H75" s="45"/>
-    </row>
-    <row r="76" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B76" s="45"/>
-      <c r="C76" s="47"/>
-      <c r="D76" s="45"/>
-      <c r="E76" s="45"/>
-      <c r="F76" s="45"/>
-      <c r="G76" s="45"/>
-      <c r="H76" s="45"/>
-    </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B77" s="46" t="s">
-        <v>134</v>
-      </c>
-      <c r="C77" s="47"/>
-      <c r="D77" s="45"/>
-      <c r="E77" s="45"/>
-      <c r="F77" s="45"/>
-      <c r="G77" s="45"/>
-      <c r="H77" s="45"/>
-    </row>
-    <row r="78" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B78" s="48" t="s">
-        <v>135</v>
-      </c>
-      <c r="C78" s="48" t="s">
-        <v>136</v>
-      </c>
-      <c r="D78" s="45"/>
-      <c r="E78" s="45"/>
-      <c r="F78" s="45"/>
-      <c r="G78" s="45"/>
-      <c r="H78" s="45"/>
-    </row>
-    <row r="79" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B79" s="49" t="s">
-        <v>168</v>
-      </c>
-      <c r="C79" s="49" t="s">
-        <v>137</v>
-      </c>
-      <c r="D79" s="45"/>
-      <c r="E79" s="45"/>
-      <c r="F79" s="45"/>
-      <c r="G79" s="45"/>
-      <c r="H79" s="45"/>
-    </row>
-    <row r="80" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B80" s="49" t="s">
-        <v>169</v>
-      </c>
-      <c r="C80" s="49" t="s">
-        <v>140</v>
-      </c>
-      <c r="D80" s="45"/>
-      <c r="E80" s="45"/>
-      <c r="F80" s="45"/>
-      <c r="G80" s="45"/>
-      <c r="H80" s="45"/>
-    </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B81" s="49" t="s">
-        <v>138</v>
-      </c>
-      <c r="C81" s="49" t="s">
-        <v>139</v>
-      </c>
-      <c r="D81" s="45"/>
-      <c r="E81" s="45"/>
-      <c r="F81" s="45"/>
-      <c r="G81" s="45"/>
-      <c r="H81" s="45"/>
-    </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B82" s="45"/>
-      <c r="C82" s="47"/>
-      <c r="D82" s="45"/>
-      <c r="E82" s="45"/>
-      <c r="F82" s="45"/>
-      <c r="G82" s="45"/>
-      <c r="H82" s="24"/>
-    </row>
-    <row r="83" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B83" s="45"/>
-      <c r="C83" s="47"/>
-      <c r="D83" s="45"/>
-      <c r="E83" s="45"/>
-      <c r="F83" s="45"/>
-      <c r="G83" s="45"/>
-      <c r="H83" s="24"/>
-    </row>
-    <row r="84" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B84" s="45"/>
-      <c r="C84" s="47"/>
-      <c r="D84" s="45"/>
-      <c r="E84" s="45"/>
-      <c r="F84" s="45"/>
-      <c r="G84" s="45"/>
-      <c r="H84" s="24"/>
-    </row>
-    <row r="85" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B85" s="24"/>
-      <c r="C85" s="60"/>
-      <c r="D85" s="24"/>
-      <c r="E85" s="24"/>
-      <c r="F85" s="24"/>
-      <c r="G85" s="24"/>
-      <c r="H85" s="24"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:H1"/>
-  </mergeCells>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F74:F1048576 H74:H1048576">
-      <formula1>"Yes,No,N/A"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F29:F34 F16:F27 F36:F46 F48:F53 F64:F72 F5:F14 F55:F62">
-      <formula1>"Pass,Fail,N/A"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="G16" r:id="rId1" location="testing-for-sensitive-data-in-local-storage"/>
-    <hyperlink ref="G17" r:id="rId2" location="testing-for-sensitive-data-in-logs"/>
-    <hyperlink ref="G18" r:id="rId3" location="testing-whether-sensitive-data-is-sent-to-third-parties"/>
-    <hyperlink ref="G19" r:id="rId4" location="testing-whether-the-keyboard-cache-is-disabled-for-text-input-fields"/>
-    <hyperlink ref="G20" r:id="rId5" location="testing-for-sensitive-data-in-the-clipboard"/>
-    <hyperlink ref="G21" r:id="rId6" location="testing-whether-sensitive-data-is-exposed-via-ipc-mechanisms"/>
-    <hyperlink ref="G23" r:id="rId7" location="testing-for-sensitive-data-in-backups"/>
-    <hyperlink ref="G24" r:id="rId8" location="testing-for-sensitive-information-in-auto-generated-screenshots"/>
-    <hyperlink ref="G25" r:id="rId9" location="testing-for-sensitive-data-in-memory"/>
-    <hyperlink ref="G26" r:id="rId10" location="testing-the-device-access-security-policy"/>
-    <hyperlink ref="G27" r:id="rId11" location="verifying-user-education-controls"/>
-    <hyperlink ref="G29" r:id="rId12" location="verifying-key-management"/>
-    <hyperlink ref="G30" r:id="rId13" location="testing-for-custom-implementations-of-cryptography"/>
-    <hyperlink ref="G31" r:id="rId14" location="verifying-the-configuration-of-cryptographic-standard-algorithms"/>
-    <hyperlink ref="G32" r:id="rId15" location="testing-for-insecure-andor-deprecated-cryptographic-algorithms"/>
-    <hyperlink ref="G33" r:id="rId16" location="testing-random-number-generation"/>
-    <hyperlink ref="G34" r:id="rId17" location="verifying-key-management"/>
-    <hyperlink ref="G41" r:id="rId18" location="testing-excessive-login-attempts"/>
-    <hyperlink ref="G42" r:id="rId19" location="testing-biometric-authentication"/>
-    <hyperlink ref="G43" r:id="rId20" location="testing-the-session-timeout"/>
-    <hyperlink ref="G44" r:id="rId21" location="testing-2-factor-authentication"/>
-    <hyperlink ref="G45" r:id="rId22" location="testing-step-up-authentication"/>
-    <hyperlink ref="G46" r:id="rId23" location="testing-user-device-management"/>
-    <hyperlink ref="G48" r:id="rId24" location="testing-for-unencrypted-sensitive-data-on-the-network"/>
-    <hyperlink ref="G49" r:id="rId25" location="verifying-the-tls-settings"/>
-    <hyperlink ref="G50" r:id="rId26" location="testing-endpoint-identify-verification"/>
-    <hyperlink ref="G51" r:id="rId27" location="testing-custom-certificate-stores-and-ssl-pinning"/>
-    <hyperlink ref="G55" r:id="rId28" location="testing-app-permissions"/>
-    <hyperlink ref="G56" r:id="rId29" location="testing-input-validation-and-sanitization"/>
-    <hyperlink ref="G57" r:id="rId30" location="testing-custom-url-schemes"/>
-    <hyperlink ref="G58" r:id="rId31" location="testing-for-sensitive-functionality-exposure-through-ipc"/>
-    <hyperlink ref="G59" r:id="rId32" location="testing-javascript-execution-in-webviews"/>
-    <hyperlink ref="G60" r:id="rId33" location="testing-webview-protocol-handlers"/>
-    <hyperlink ref="G61" r:id="rId34" location="testing-whether-java-objects-are-exposed-through-webviews"/>
-    <hyperlink ref="G62" r:id="rId35" location="testing-object-de-serialization"/>
-    <hyperlink ref="G64" r:id="rId36" location="verifying-that-the-app-is-properly-signed"/>
-    <hyperlink ref="G65" r:id="rId37" location="testing-if-the-app-is-debuggable"/>
-    <hyperlink ref="G66" r:id="rId38" location="testing-for-debugging-symbols"/>
-    <hyperlink ref="G67" r:id="rId39" location="testing-for-debugging-code-and-verbose-error-logging"/>
-    <hyperlink ref="G70" r:id="rId40" location="testing-exception-handling"/>
-    <hyperlink ref="G71" r:id="rId41" location="testing-for-memory-management-bugs"/>
-    <hyperlink ref="G72" r:id="rId42" location="verifying-compiler-settings"/>
-    <hyperlink ref="G36" r:id="rId43" location="verifying-that-users-are-properly-authenticated"/>
-    <hyperlink ref="G37" r:id="rId44" location="testing-session-management"/>
-    <hyperlink ref="G22" r:id="rId45"/>
-    <hyperlink ref="G40" r:id="rId46" location="testing-the-password-policy"/>
-    <hyperlink ref="G52" r:id="rId47" location="verifying-that-critical-operations-use-secure-communication-channels"/>
-    <hyperlink ref="G53" r:id="rId48"/>
-    <hyperlink ref="G39" r:id="rId49" location="testing-the-logout-functionality"/>
-    <hyperlink ref="G38" r:id="rId50" location="testing-session-management"/>
-    <hyperlink ref="G69" r:id="rId51" location="testing-exception-handling"/>
-  </hyperlinks>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:G29"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
@@ -6087,23 +4583,1558 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E17:E18 E15 E5:E13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E17:E18 E15 E5:E13" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>"Pass,Fail,N/A"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="F5" r:id="rId1" location="testing-advanced-root-detection"/>
-    <hyperlink ref="F6" r:id="rId2" location="testing-debugging-defenses"/>
-    <hyperlink ref="F7" r:id="rId3" location="testing-file-integrity-checks"/>
-    <hyperlink ref="F8" r:id="rId4" location="testing-detection-of-reverse-engineering-tools"/>
-    <hyperlink ref="F9" r:id="rId5" location="testing-simple-emulator-detection"/>
-    <hyperlink ref="F10" r:id="rId6" location="testing-memory-integrity-checks"/>
-    <hyperlink ref="F11" r:id="rId7" location="verifying-the-variablility-of-tampering-responses"/>
-    <hyperlink ref="F15" r:id="rId8" location="testing-device-binding"/>
-    <hyperlink ref="F17" r:id="rId9" location="testing-advanced-anti-emulation"/>
-    <hyperlink ref="F18" r:id="rId10" location="testing-advanced-anti-emulation"/>
-    <hyperlink ref="F12" r:id="rId11"/>
-    <hyperlink ref="F13" r:id="rId12" location="testing-simple-obfuscation"/>
+    <hyperlink ref="F5" r:id="rId1" location="testing-advanced-root-detection" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="F6" r:id="rId2" location="testing-debugging-defenses" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="F7" r:id="rId3" location="testing-file-integrity-checks" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="F8" r:id="rId4" location="testing-detection-of-reverse-engineering-tools" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink ref="F9" r:id="rId5" location="testing-simple-emulator-detection" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
+    <hyperlink ref="F10" r:id="rId6" location="testing-memory-integrity-checks" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
+    <hyperlink ref="F11" r:id="rId7" location="verifying-the-variablility-of-tampering-responses" xr:uid="{00000000-0004-0000-0300-000006000000}"/>
+    <hyperlink ref="F15" r:id="rId8" location="testing-device-binding" xr:uid="{00000000-0004-0000-0300-000007000000}"/>
+    <hyperlink ref="F17" r:id="rId9" location="testing-advanced-anti-emulation" xr:uid="{00000000-0004-0000-0300-000008000000}"/>
+    <hyperlink ref="F18" r:id="rId10" location="testing-advanced-anti-emulation" xr:uid="{00000000-0004-0000-0300-000009000000}"/>
+    <hyperlink ref="F12" r:id="rId11" xr:uid="{00000000-0004-0000-0300-00000A000000}"/>
+    <hyperlink ref="F13" r:id="rId12" location="testing-simple-obfuscation" xr:uid="{00000000-0004-0000-0300-00000B000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="B1:J85"/>
+  <sheetViews>
+    <sheetView topLeftCell="D31" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="1.83203125" customWidth="1"/>
+    <col min="2" max="2" width="8" customWidth="1"/>
+    <col min="3" max="3" width="96.6640625" style="61" customWidth="1"/>
+    <col min="7" max="7" width="53.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.83203125" customWidth="1"/>
+    <col min="10" max="11" width="10.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" ht="19" x14ac:dyDescent="0.2">
+      <c r="B1" s="113" t="s">
+        <v>177</v>
+      </c>
+      <c r="C1" s="113"/>
+      <c r="D1" s="113"/>
+      <c r="E1" s="113"/>
+      <c r="F1" s="113"/>
+      <c r="G1" s="113"/>
+      <c r="H1" s="113"/>
+    </row>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B2" s="50"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B3" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="29" t="s">
+        <v>166</v>
+      </c>
+      <c r="G3" s="29" t="s">
+        <v>180</v>
+      </c>
+      <c r="H3" s="30" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B4" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="34"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B5" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="37" t="s">
+        <v>168</v>
+      </c>
+      <c r="G5" s="52" t="s">
+        <v>192</v>
+      </c>
+      <c r="H5" s="74"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B6" s="35">
+        <v>1.2</v>
+      </c>
+      <c r="C6" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="37"/>
+      <c r="G6" s="52" t="s">
+        <v>192</v>
+      </c>
+      <c r="H6" s="74"/>
+    </row>
+    <row r="7" spans="2:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="B7" s="35">
+        <v>1.3</v>
+      </c>
+      <c r="C7" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="37"/>
+      <c r="G7" s="52" t="s">
+        <v>192</v>
+      </c>
+      <c r="H7" s="74"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B8" s="35">
+        <v>1.4</v>
+      </c>
+      <c r="C8" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="37"/>
+      <c r="G8" s="52" t="s">
+        <v>192</v>
+      </c>
+      <c r="H8" s="74"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B9" s="35">
+        <v>1.5</v>
+      </c>
+      <c r="C9" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="36"/>
+      <c r="E9" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="37" t="s">
+        <v>138</v>
+      </c>
+      <c r="G9" s="52" t="s">
+        <v>192</v>
+      </c>
+      <c r="H9" s="74"/>
+    </row>
+    <row r="10" spans="2:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="B10" s="35">
+        <v>1.6</v>
+      </c>
+      <c r="C10" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="36"/>
+      <c r="E10" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="37" t="s">
+        <v>138</v>
+      </c>
+      <c r="G10" s="52" t="s">
+        <v>192</v>
+      </c>
+      <c r="H10" s="74"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B11" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="53"/>
+      <c r="E11" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="37" t="s">
+        <v>138</v>
+      </c>
+      <c r="G11" s="52" t="s">
+        <v>192</v>
+      </c>
+      <c r="H11" s="74"/>
+    </row>
+    <row r="12" spans="2:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="B12" s="35">
+        <v>1.8</v>
+      </c>
+      <c r="C12" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="36"/>
+      <c r="E12" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="37" t="s">
+        <v>138</v>
+      </c>
+      <c r="G12" s="52" t="s">
+        <v>192</v>
+      </c>
+      <c r="H12" s="74"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B13" s="35">
+        <v>1.9</v>
+      </c>
+      <c r="C13" s="36" t="s">
+        <v>285</v>
+      </c>
+      <c r="D13" s="36"/>
+      <c r="E13" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="37" t="s">
+        <v>138</v>
+      </c>
+      <c r="G13" s="52" t="s">
+        <v>192</v>
+      </c>
+      <c r="H13" s="74"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B14" s="71" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="36" t="s">
+        <v>286</v>
+      </c>
+      <c r="D14" s="36"/>
+      <c r="E14" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="37" t="s">
+        <v>138</v>
+      </c>
+      <c r="G14" s="52" t="s">
+        <v>192</v>
+      </c>
+      <c r="H14" s="74"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B15" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="39"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="40"/>
+    </row>
+    <row r="16" spans="2:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="B16" s="55" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="56" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="37"/>
+      <c r="G16" s="58" t="s">
+        <v>188</v>
+      </c>
+      <c r="H16" s="74"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B17" s="55" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="56" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="37"/>
+      <c r="G17" s="58" t="s">
+        <v>189</v>
+      </c>
+      <c r="H17" s="74"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B18" s="55" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="56" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="37"/>
+      <c r="G18" s="58" t="s">
+        <v>190</v>
+      </c>
+      <c r="H18" s="74"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B19" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="56" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" s="37"/>
+      <c r="G19" s="58" t="s">
+        <v>191</v>
+      </c>
+      <c r="H19" s="74"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B20" s="55" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" s="56" t="s">
+        <v>74</v>
+      </c>
+      <c r="D20" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="37"/>
+      <c r="G20" s="58" t="s">
+        <v>193</v>
+      </c>
+      <c r="H20" s="74"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B21" s="55" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="56" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" s="37"/>
+      <c r="G21" s="58" t="s">
+        <v>194</v>
+      </c>
+      <c r="H21" s="74"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B22" s="55" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="56" t="s">
+        <v>287</v>
+      </c>
+      <c r="D22" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" s="37"/>
+      <c r="G22" s="58" t="s">
+        <v>251</v>
+      </c>
+      <c r="H22" s="74"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B23" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="56" t="s">
+        <v>288</v>
+      </c>
+      <c r="D23" s="56"/>
+      <c r="E23" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" s="37" t="s">
+        <v>138</v>
+      </c>
+      <c r="G23" s="58" t="s">
+        <v>195</v>
+      </c>
+      <c r="H23" s="74"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B24" s="55" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="56" t="s">
+        <v>76</v>
+      </c>
+      <c r="D24" s="56"/>
+      <c r="E24" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="37" t="s">
+        <v>138</v>
+      </c>
+      <c r="G24" s="58" t="s">
+        <v>196</v>
+      </c>
+      <c r="H24" s="74"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B25" s="55" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" s="56" t="s">
+        <v>77</v>
+      </c>
+      <c r="D25" s="56"/>
+      <c r="E25" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" s="37" t="s">
+        <v>138</v>
+      </c>
+      <c r="G25" s="58" t="s">
+        <v>197</v>
+      </c>
+      <c r="H25" s="74"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B26" s="55" t="s">
+        <v>69</v>
+      </c>
+      <c r="C26" s="56" t="s">
+        <v>78</v>
+      </c>
+      <c r="D26" s="56"/>
+      <c r="E26" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" s="37" t="s">
+        <v>138</v>
+      </c>
+      <c r="G26" s="58" t="s">
+        <v>198</v>
+      </c>
+      <c r="H26" s="74"/>
+    </row>
+    <row r="27" spans="2:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="B27" s="55" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="56" t="s">
+        <v>127</v>
+      </c>
+      <c r="D27" s="56"/>
+      <c r="E27" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" s="37" t="s">
+        <v>138</v>
+      </c>
+      <c r="G27" s="58" t="s">
+        <v>199</v>
+      </c>
+      <c r="H27" s="74"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B28" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="D28" s="39"/>
+      <c r="E28" s="54"/>
+      <c r="F28" s="39"/>
+      <c r="G28" s="39"/>
+      <c r="H28" s="40"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B29" s="55" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="D29" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" s="37"/>
+      <c r="G29" s="58" t="s">
+        <v>200</v>
+      </c>
+      <c r="H29" s="74"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B30" s="55" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" s="56" t="s">
+        <v>81</v>
+      </c>
+      <c r="D30" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F30" s="37"/>
+      <c r="G30" s="58" t="s">
+        <v>201</v>
+      </c>
+      <c r="H30" s="74"/>
+    </row>
+    <row r="31" spans="2:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="B31" s="55" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="D31" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F31" s="37"/>
+      <c r="G31" s="58" t="s">
+        <v>202</v>
+      </c>
+      <c r="H31" s="74"/>
+    </row>
+    <row r="32" spans="2:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="B32" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32" s="56" t="s">
+        <v>128</v>
+      </c>
+      <c r="D32" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" s="37"/>
+      <c r="G32" s="58" t="s">
+        <v>203</v>
+      </c>
+      <c r="H32" s="74"/>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B33" s="55" t="s">
+        <v>23</v>
+      </c>
+      <c r="C33" s="56" t="s">
+        <v>83</v>
+      </c>
+      <c r="D33" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F33" s="37"/>
+      <c r="G33" s="58" t="s">
+        <v>204</v>
+      </c>
+      <c r="H33" s="74"/>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B34" s="55" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34" s="56" t="s">
+        <v>84</v>
+      </c>
+      <c r="D34" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F34" s="37"/>
+      <c r="G34" s="58" t="s">
+        <v>200</v>
+      </c>
+      <c r="H34" s="74"/>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B35" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="C35" s="39" t="s">
+        <v>85</v>
+      </c>
+      <c r="D35" s="39"/>
+      <c r="E35" s="54"/>
+      <c r="F35" s="39"/>
+      <c r="G35" s="39"/>
+      <c r="H35" s="40"/>
+    </row>
+    <row r="36" spans="2:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="B36" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="C36" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="D36" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F36" s="37"/>
+      <c r="G36" s="58" t="s">
+        <v>205</v>
+      </c>
+      <c r="H36" s="74"/>
+    </row>
+    <row r="37" spans="2:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="B37" s="55" t="s">
+        <v>86</v>
+      </c>
+      <c r="C37" s="56" t="s">
+        <v>274</v>
+      </c>
+      <c r="D37" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F37" s="37"/>
+      <c r="G37" s="58" t="s">
+        <v>206</v>
+      </c>
+      <c r="H37" s="74"/>
+    </row>
+    <row r="38" spans="2:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="B38" s="55" t="s">
+        <v>87</v>
+      </c>
+      <c r="C38" s="56" t="s">
+        <v>272</v>
+      </c>
+      <c r="D38" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F38" s="37"/>
+      <c r="G38" s="58" t="s">
+        <v>206</v>
+      </c>
+      <c r="H38" s="74"/>
+      <c r="J38" s="58"/>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B39" s="55" t="s">
+        <v>27</v>
+      </c>
+      <c r="C39" s="56" t="s">
+        <v>289</v>
+      </c>
+      <c r="D39" s="26"/>
+      <c r="E39" s="51"/>
+      <c r="F39" s="37"/>
+      <c r="G39" s="58" t="s">
+        <v>208</v>
+      </c>
+      <c r="H39" s="74"/>
+      <c r="J39" s="58"/>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B40" s="55" t="s">
+        <v>28</v>
+      </c>
+      <c r="C40" s="56" t="s">
+        <v>91</v>
+      </c>
+      <c r="D40" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E40" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F40" s="37"/>
+      <c r="G40" s="58" t="s">
+        <v>207</v>
+      </c>
+      <c r="H40" s="74"/>
+    </row>
+    <row r="41" spans="2:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="B41" s="55" t="s">
+        <v>88</v>
+      </c>
+      <c r="C41" s="56" t="s">
+        <v>293</v>
+      </c>
+      <c r="D41" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F41" s="37"/>
+      <c r="G41" s="58" t="s">
+        <v>209</v>
+      </c>
+      <c r="H41" s="74"/>
+    </row>
+    <row r="42" spans="2:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="B42" s="55" t="s">
+        <v>89</v>
+      </c>
+      <c r="C42" s="56" t="s">
+        <v>92</v>
+      </c>
+      <c r="D42" s="56"/>
+      <c r="E42" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F42" s="37" t="s">
+        <v>138</v>
+      </c>
+      <c r="G42" s="58" t="s">
+        <v>210</v>
+      </c>
+      <c r="H42" s="74"/>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B43" s="55" t="s">
+        <v>29</v>
+      </c>
+      <c r="C43" s="56" t="s">
+        <v>290</v>
+      </c>
+      <c r="D43" s="56"/>
+      <c r="E43" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F43" s="37" t="s">
+        <v>138</v>
+      </c>
+      <c r="G43" s="58" t="s">
+        <v>211</v>
+      </c>
+      <c r="H43" s="74"/>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B44" s="55" t="s">
+        <v>30</v>
+      </c>
+      <c r="C44" s="56" t="s">
+        <v>93</v>
+      </c>
+      <c r="D44" s="56"/>
+      <c r="E44" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F44" s="37" t="s">
+        <v>138</v>
+      </c>
+      <c r="G44" s="58" t="s">
+        <v>212</v>
+      </c>
+      <c r="H44" s="74"/>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B45" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="C45" s="56" t="s">
+        <v>94</v>
+      </c>
+      <c r="D45" s="56"/>
+      <c r="E45" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F45" s="37" t="s">
+        <v>138</v>
+      </c>
+      <c r="G45" s="58" t="s">
+        <v>213</v>
+      </c>
+      <c r="H45" s="74"/>
+    </row>
+    <row r="46" spans="2:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="B46" s="55" t="s">
+        <v>273</v>
+      </c>
+      <c r="C46" s="56" t="s">
+        <v>95</v>
+      </c>
+      <c r="D46" s="56"/>
+      <c r="E46" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F46" s="37" t="s">
+        <v>138</v>
+      </c>
+      <c r="G46" s="58" t="s">
+        <v>214</v>
+      </c>
+      <c r="H46" s="74"/>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B47" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="C47" s="39" t="s">
+        <v>96</v>
+      </c>
+      <c r="D47" s="39"/>
+      <c r="E47" s="54"/>
+      <c r="F47" s="39"/>
+      <c r="G47" s="39"/>
+      <c r="H47" s="40"/>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B48" s="55" t="s">
+        <v>33</v>
+      </c>
+      <c r="C48" s="56" t="s">
+        <v>99</v>
+      </c>
+      <c r="D48" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E48" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F48" s="37"/>
+      <c r="G48" s="58" t="s">
+        <v>215</v>
+      </c>
+      <c r="H48" s="74"/>
+    </row>
+    <row r="49" spans="2:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="B49" s="55" t="s">
+        <v>97</v>
+      </c>
+      <c r="C49" s="56" t="s">
+        <v>129</v>
+      </c>
+      <c r="D49" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E49" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F49" s="37"/>
+      <c r="G49" s="58" t="s">
+        <v>216</v>
+      </c>
+      <c r="H49" s="74"/>
+    </row>
+    <row r="50" spans="2:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="B50" s="55" t="s">
+        <v>34</v>
+      </c>
+      <c r="C50" s="56" t="s">
+        <v>100</v>
+      </c>
+      <c r="D50" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E50" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F50" s="37"/>
+      <c r="G50" s="58" t="s">
+        <v>217</v>
+      </c>
+      <c r="H50" s="74"/>
+    </row>
+    <row r="51" spans="2:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="B51" s="55" t="s">
+        <v>98</v>
+      </c>
+      <c r="C51" s="56" t="s">
+        <v>101</v>
+      </c>
+      <c r="D51" s="56"/>
+      <c r="E51" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F51" s="37" t="s">
+        <v>138</v>
+      </c>
+      <c r="G51" s="58" t="s">
+        <v>218</v>
+      </c>
+      <c r="H51" s="74"/>
+    </row>
+    <row r="52" spans="2:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="B52" s="55" t="s">
+        <v>35</v>
+      </c>
+      <c r="C52" s="56" t="s">
+        <v>102</v>
+      </c>
+      <c r="D52" s="56"/>
+      <c r="E52" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F52" s="37" t="s">
+        <v>138</v>
+      </c>
+      <c r="G52" s="58" t="s">
+        <v>219</v>
+      </c>
+      <c r="H52" s="74"/>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B53" s="55">
+        <v>5.6</v>
+      </c>
+      <c r="C53" s="56" t="s">
+        <v>269</v>
+      </c>
+      <c r="D53" s="56"/>
+      <c r="E53" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F53" s="37" t="s">
+        <v>138</v>
+      </c>
+      <c r="G53" s="58" t="s">
+        <v>270</v>
+      </c>
+      <c r="H53" s="74"/>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B54" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="C54" s="39" t="s">
+        <v>236</v>
+      </c>
+      <c r="D54" s="39"/>
+      <c r="E54" s="54"/>
+      <c r="F54" s="39"/>
+      <c r="G54" s="39"/>
+      <c r="H54" s="40"/>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B55" s="55" t="s">
+        <v>103</v>
+      </c>
+      <c r="C55" s="56" t="s">
+        <v>109</v>
+      </c>
+      <c r="D55" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E55" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F55" s="37"/>
+      <c r="G55" s="58" t="s">
+        <v>220</v>
+      </c>
+      <c r="H55" s="74"/>
+    </row>
+    <row r="56" spans="2:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="B56" s="55" t="s">
+        <v>104</v>
+      </c>
+      <c r="C56" s="56" t="s">
+        <v>110</v>
+      </c>
+      <c r="D56" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E56" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F56" s="37"/>
+      <c r="G56" s="58" t="s">
+        <v>221</v>
+      </c>
+      <c r="H56" s="74"/>
+    </row>
+    <row r="57" spans="2:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="B57" s="55" t="s">
+        <v>105</v>
+      </c>
+      <c r="C57" s="56" t="s">
+        <v>111</v>
+      </c>
+      <c r="D57" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E57" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F57" s="37"/>
+      <c r="G57" s="58" t="s">
+        <v>222</v>
+      </c>
+      <c r="H57" s="74"/>
+    </row>
+    <row r="58" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B58" s="55" t="s">
+        <v>106</v>
+      </c>
+      <c r="C58" s="56" t="s">
+        <v>112</v>
+      </c>
+      <c r="D58" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E58" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F58" s="37"/>
+      <c r="G58" s="58" t="s">
+        <v>223</v>
+      </c>
+      <c r="H58" s="74"/>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B59" s="55" t="s">
+        <v>107</v>
+      </c>
+      <c r="C59" s="56" t="s">
+        <v>113</v>
+      </c>
+      <c r="D59" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E59" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F59" s="37"/>
+      <c r="G59" s="58" t="s">
+        <v>224</v>
+      </c>
+      <c r="H59" s="74"/>
+    </row>
+    <row r="60" spans="2:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="B60" s="55" t="s">
+        <v>108</v>
+      </c>
+      <c r="C60" s="56" t="s">
+        <v>114</v>
+      </c>
+      <c r="D60" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E60" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F60" s="37"/>
+      <c r="G60" s="58" t="s">
+        <v>225</v>
+      </c>
+      <c r="H60" s="74"/>
+    </row>
+    <row r="61" spans="2:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="B61" s="55" t="s">
+        <v>291</v>
+      </c>
+      <c r="C61" s="56" t="s">
+        <v>268</v>
+      </c>
+      <c r="D61" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E61" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F61" s="37"/>
+      <c r="G61" s="58" t="s">
+        <v>226</v>
+      </c>
+      <c r="H61" s="74"/>
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B62" s="55">
+        <v>6.8</v>
+      </c>
+      <c r="C62" s="56" t="s">
+        <v>115</v>
+      </c>
+      <c r="D62" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E62" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F62" s="37"/>
+      <c r="G62" s="58" t="s">
+        <v>227</v>
+      </c>
+      <c r="H62" s="74"/>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B63" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="C63" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="D63" s="39"/>
+      <c r="E63" s="54"/>
+      <c r="F63" s="39"/>
+      <c r="G63" s="39"/>
+      <c r="H63" s="40"/>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B64" s="55" t="s">
+        <v>116</v>
+      </c>
+      <c r="C64" s="56" t="s">
+        <v>121</v>
+      </c>
+      <c r="D64" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E64" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F64" s="37"/>
+      <c r="G64" s="58" t="s">
+        <v>228</v>
+      </c>
+      <c r="H64" s="74"/>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B65" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="C65" s="56" t="s">
+        <v>122</v>
+      </c>
+      <c r="D65" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E65" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F65" s="37"/>
+      <c r="G65" s="58" t="s">
+        <v>229</v>
+      </c>
+      <c r="H65" s="74"/>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B66" s="55" t="s">
+        <v>117</v>
+      </c>
+      <c r="C66" s="56" t="s">
+        <v>123</v>
+      </c>
+      <c r="D66" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E66" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F66" s="37"/>
+      <c r="G66" s="58" t="s">
+        <v>230</v>
+      </c>
+      <c r="H66" s="74"/>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B67" s="55" t="s">
+        <v>118</v>
+      </c>
+      <c r="C67" s="56" t="s">
+        <v>124</v>
+      </c>
+      <c r="D67" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E67" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F67" s="37"/>
+      <c r="G67" s="58" t="s">
+        <v>231</v>
+      </c>
+      <c r="H67" s="74"/>
+    </row>
+    <row r="68" spans="2:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="B68" s="55" t="s">
+        <v>119</v>
+      </c>
+      <c r="C68" s="56" t="s">
+        <v>283</v>
+      </c>
+      <c r="D68" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E68" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F68" s="37"/>
+      <c r="G68" s="58" t="s">
+        <v>284</v>
+      </c>
+      <c r="H68" s="74"/>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B69" s="55" t="s">
+        <v>39</v>
+      </c>
+      <c r="C69" s="56" t="s">
+        <v>125</v>
+      </c>
+      <c r="D69" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E69" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F69" s="37"/>
+      <c r="G69" s="58" t="s">
+        <v>233</v>
+      </c>
+      <c r="H69" s="74"/>
+    </row>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B70" s="55" t="s">
+        <v>40</v>
+      </c>
+      <c r="C70" s="56" t="s">
+        <v>42</v>
+      </c>
+      <c r="D70" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E70" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F70" s="37"/>
+      <c r="G70" s="58" t="s">
+        <v>234</v>
+      </c>
+      <c r="H70" s="74"/>
+    </row>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B71" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="C71" s="56" t="s">
+        <v>126</v>
+      </c>
+      <c r="D71" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E71" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F71" s="37"/>
+      <c r="G71" s="58" t="s">
+        <v>235</v>
+      </c>
+      <c r="H71" s="74"/>
+    </row>
+    <row r="72" spans="2:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="B72" s="55" t="s">
+        <v>282</v>
+      </c>
+      <c r="C72" s="56" t="s">
+        <v>264</v>
+      </c>
+      <c r="D72" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E72" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F72" s="37"/>
+      <c r="G72" s="58" t="s">
+        <v>271</v>
+      </c>
+      <c r="H72" s="74"/>
+    </row>
+    <row r="73" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B73" s="41"/>
+      <c r="C73" s="42"/>
+      <c r="D73" s="43"/>
+      <c r="E73" s="43"/>
+      <c r="F73" s="43"/>
+      <c r="G73" s="43"/>
+      <c r="H73" s="44"/>
+    </row>
+    <row r="74" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B74" s="45"/>
+      <c r="C74" s="47"/>
+      <c r="D74" s="45"/>
+      <c r="E74" s="45"/>
+      <c r="F74" s="45"/>
+      <c r="G74" s="45"/>
+      <c r="H74" s="45"/>
+    </row>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B75" s="45"/>
+      <c r="C75" s="56"/>
+      <c r="D75" s="45"/>
+      <c r="E75" s="45"/>
+      <c r="F75" s="45"/>
+      <c r="G75" s="45"/>
+      <c r="H75" s="45"/>
+    </row>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B76" s="45"/>
+      <c r="C76" s="47"/>
+      <c r="D76" s="45"/>
+      <c r="E76" s="45"/>
+      <c r="F76" s="45"/>
+      <c r="G76" s="45"/>
+      <c r="H76" s="45"/>
+    </row>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B77" s="46" t="s">
+        <v>134</v>
+      </c>
+      <c r="C77" s="47"/>
+      <c r="D77" s="45"/>
+      <c r="E77" s="45"/>
+      <c r="F77" s="45"/>
+      <c r="G77" s="45"/>
+      <c r="H77" s="45"/>
+    </row>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B78" s="48" t="s">
+        <v>135</v>
+      </c>
+      <c r="C78" s="48" t="s">
+        <v>136</v>
+      </c>
+      <c r="D78" s="45"/>
+      <c r="E78" s="45"/>
+      <c r="F78" s="45"/>
+      <c r="G78" s="45"/>
+      <c r="H78" s="45"/>
+    </row>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B79" s="49" t="s">
+        <v>168</v>
+      </c>
+      <c r="C79" s="49" t="s">
+        <v>137</v>
+      </c>
+      <c r="D79" s="45"/>
+      <c r="E79" s="45"/>
+      <c r="F79" s="45"/>
+      <c r="G79" s="45"/>
+      <c r="H79" s="45"/>
+    </row>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B80" s="49" t="s">
+        <v>169</v>
+      </c>
+      <c r="C80" s="49" t="s">
+        <v>140</v>
+      </c>
+      <c r="D80" s="45"/>
+      <c r="E80" s="45"/>
+      <c r="F80" s="45"/>
+      <c r="G80" s="45"/>
+      <c r="H80" s="45"/>
+    </row>
+    <row r="81" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B81" s="49" t="s">
+        <v>138</v>
+      </c>
+      <c r="C81" s="49" t="s">
+        <v>139</v>
+      </c>
+      <c r="D81" s="45"/>
+      <c r="E81" s="45"/>
+      <c r="F81" s="45"/>
+      <c r="G81" s="45"/>
+      <c r="H81" s="45"/>
+    </row>
+    <row r="82" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B82" s="45"/>
+      <c r="C82" s="47"/>
+      <c r="D82" s="45"/>
+      <c r="E82" s="45"/>
+      <c r="F82" s="45"/>
+      <c r="G82" s="45"/>
+      <c r="H82" s="24"/>
+    </row>
+    <row r="83" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B83" s="45"/>
+      <c r="C83" s="47"/>
+      <c r="D83" s="45"/>
+      <c r="E83" s="45"/>
+      <c r="F83" s="45"/>
+      <c r="G83" s="45"/>
+      <c r="H83" s="24"/>
+    </row>
+    <row r="84" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B84" s="45"/>
+      <c r="C84" s="47"/>
+      <c r="D84" s="45"/>
+      <c r="E84" s="45"/>
+      <c r="F84" s="45"/>
+      <c r="G84" s="45"/>
+      <c r="H84" s="24"/>
+    </row>
+    <row r="85" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B85" s="24"/>
+      <c r="C85" s="60"/>
+      <c r="D85" s="24"/>
+      <c r="E85" s="24"/>
+      <c r="F85" s="24"/>
+      <c r="G85" s="24"/>
+      <c r="H85" s="24"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:H1"/>
+  </mergeCells>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F74:F1048576 H74:H1048576" xr:uid="{00000000-0002-0000-0200-000000000000}">
+      <formula1>"Yes,No,N/A"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F29:F34 F16:F27 F36:F46 F48:F53 F64:F72 F5:F14 F55:F62" xr:uid="{00000000-0002-0000-0200-000001000000}">
+      <formula1>"Pass,Fail,N/A"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="G16" r:id="rId1" location="testing-for-sensitive-data-in-local-storage" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="G17" r:id="rId2" location="testing-for-sensitive-data-in-logs" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="G18" r:id="rId3" location="testing-whether-sensitive-data-is-sent-to-third-parties" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="G19" r:id="rId4" location="testing-whether-the-keyboard-cache-is-disabled-for-text-input-fields" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="G20" r:id="rId5" location="testing-for-sensitive-data-in-the-clipboard" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="G21" r:id="rId6" location="testing-whether-sensitive-data-is-exposed-via-ipc-mechanisms" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="G23" r:id="rId7" location="testing-for-sensitive-data-in-backups" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
+    <hyperlink ref="G24" r:id="rId8" location="testing-for-sensitive-information-in-auto-generated-screenshots" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
+    <hyperlink ref="G25" r:id="rId9" location="testing-for-sensitive-data-in-memory" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
+    <hyperlink ref="G26" r:id="rId10" location="testing-the-device-access-security-policy" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
+    <hyperlink ref="G27" r:id="rId11" location="verifying-user-education-controls" xr:uid="{00000000-0004-0000-0200-00000A000000}"/>
+    <hyperlink ref="G29" r:id="rId12" location="verifying-key-management" xr:uid="{00000000-0004-0000-0200-00000B000000}"/>
+    <hyperlink ref="G30" r:id="rId13" location="testing-for-custom-implementations-of-cryptography" xr:uid="{00000000-0004-0000-0200-00000C000000}"/>
+    <hyperlink ref="G31" r:id="rId14" location="verifying-the-configuration-of-cryptographic-standard-algorithms" xr:uid="{00000000-0004-0000-0200-00000D000000}"/>
+    <hyperlink ref="G32" r:id="rId15" location="testing-for-insecure-andor-deprecated-cryptographic-algorithms" xr:uid="{00000000-0004-0000-0200-00000E000000}"/>
+    <hyperlink ref="G33" r:id="rId16" location="testing-random-number-generation" xr:uid="{00000000-0004-0000-0200-00000F000000}"/>
+    <hyperlink ref="G34" r:id="rId17" location="verifying-key-management" xr:uid="{00000000-0004-0000-0200-000010000000}"/>
+    <hyperlink ref="G41" r:id="rId18" xr:uid="{00000000-0004-0000-0200-000011000000}"/>
+    <hyperlink ref="G42" r:id="rId19" location="testing-biometric-authentication" xr:uid="{00000000-0004-0000-0200-000012000000}"/>
+    <hyperlink ref="G43" r:id="rId20" xr:uid="{00000000-0004-0000-0200-000013000000}"/>
+    <hyperlink ref="G44" r:id="rId21" xr:uid="{00000000-0004-0000-0200-000014000000}"/>
+    <hyperlink ref="G45" r:id="rId22" xr:uid="{00000000-0004-0000-0200-000015000000}"/>
+    <hyperlink ref="G46" r:id="rId23" xr:uid="{00000000-0004-0000-0200-000016000000}"/>
+    <hyperlink ref="G48" r:id="rId24" location="testing-for-unencrypted-sensitive-data-on-the-network" xr:uid="{00000000-0004-0000-0200-000017000000}"/>
+    <hyperlink ref="G49" r:id="rId25" location="verifying-the-tls-settings" xr:uid="{00000000-0004-0000-0200-000018000000}"/>
+    <hyperlink ref="G50" r:id="rId26" location="testing-endpoint-identify-verification" xr:uid="{00000000-0004-0000-0200-000019000000}"/>
+    <hyperlink ref="G51" r:id="rId27" location="testing-custom-certificate-stores-and-ssl-pinning" xr:uid="{00000000-0004-0000-0200-00001A000000}"/>
+    <hyperlink ref="G55" r:id="rId28" location="testing-app-permissions" xr:uid="{00000000-0004-0000-0200-00001B000000}"/>
+    <hyperlink ref="G56" r:id="rId29" location="testing-input-validation-and-sanitization" xr:uid="{00000000-0004-0000-0200-00001C000000}"/>
+    <hyperlink ref="G57" r:id="rId30" location="testing-custom-url-schemes" xr:uid="{00000000-0004-0000-0200-00001D000000}"/>
+    <hyperlink ref="G58" r:id="rId31" location="testing-for-sensitive-functionality-exposure-through-ipc" xr:uid="{00000000-0004-0000-0200-00001E000000}"/>
+    <hyperlink ref="G59" r:id="rId32" location="testing-javascript-execution-in-webviews" xr:uid="{00000000-0004-0000-0200-00001F000000}"/>
+    <hyperlink ref="G60" r:id="rId33" location="testing-webview-protocol-handlers" xr:uid="{00000000-0004-0000-0200-000020000000}"/>
+    <hyperlink ref="G61" r:id="rId34" location="testing-whether-java-objects-are-exposed-through-webviews" xr:uid="{00000000-0004-0000-0200-000021000000}"/>
+    <hyperlink ref="G62" r:id="rId35" location="testing-object-de-serialization" xr:uid="{00000000-0004-0000-0200-000022000000}"/>
+    <hyperlink ref="G64" r:id="rId36" location="verifying-that-the-app-is-properly-signed" xr:uid="{00000000-0004-0000-0200-000023000000}"/>
+    <hyperlink ref="G65" r:id="rId37" location="testing-if-the-app-is-debuggable" xr:uid="{00000000-0004-0000-0200-000024000000}"/>
+    <hyperlink ref="G66" r:id="rId38" location="testing-for-debugging-symbols" xr:uid="{00000000-0004-0000-0200-000025000000}"/>
+    <hyperlink ref="G67" r:id="rId39" location="testing-for-debugging-code-and-verbose-error-logging" xr:uid="{00000000-0004-0000-0200-000026000000}"/>
+    <hyperlink ref="G70" r:id="rId40" location="testing-exception-handling" xr:uid="{00000000-0004-0000-0200-000027000000}"/>
+    <hyperlink ref="G71" r:id="rId41" location="testing-for-memory-management-bugs" xr:uid="{00000000-0004-0000-0200-000028000000}"/>
+    <hyperlink ref="G72" r:id="rId42" location="verifying-compiler-settings" xr:uid="{00000000-0004-0000-0200-000029000000}"/>
+    <hyperlink ref="G36" r:id="rId43" xr:uid="{00000000-0004-0000-0200-00002A000000}"/>
+    <hyperlink ref="G37" r:id="rId44" xr:uid="{00000000-0004-0000-0200-00002B000000}"/>
+    <hyperlink ref="G22" r:id="rId45" xr:uid="{00000000-0004-0000-0200-00002C000000}"/>
+    <hyperlink ref="G40" r:id="rId46" xr:uid="{00000000-0004-0000-0200-00002D000000}"/>
+    <hyperlink ref="G52" r:id="rId47" location="verifying-that-critical-operations-use-secure-communication-channels" xr:uid="{00000000-0004-0000-0200-00002E000000}"/>
+    <hyperlink ref="G53" r:id="rId48" xr:uid="{00000000-0004-0000-0200-00002F000000}"/>
+    <hyperlink ref="G39" r:id="rId49" xr:uid="{00000000-0004-0000-0200-000030000000}"/>
+    <hyperlink ref="G38" r:id="rId50" xr:uid="{00000000-0004-0000-0200-000031000000}"/>
+    <hyperlink ref="G69" r:id="rId51" location="testing-exception-handling" xr:uid="{00000000-0004-0000-0200-000032000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -6111,11 +6142,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B1:J85"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView topLeftCell="A21" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36:G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7159,7 +7190,7 @@
       </c>
       <c r="H57" s="74"/>
     </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B58" s="55" t="s">
         <v>106</v>
       </c>
@@ -7575,65 +7606,65 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F74:F1048576 H74:H1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F74:F1048576 H74:H1048576" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>"Yes,No,N/A"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F16:F27 F29:F34 F36:F46 F48:F53 F64:F72 F5:F14 F55:F62">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F16:F27 F29:F34 F36:F46 F48:F53 F64:F72 F5:F14 F55:F62" xr:uid="{00000000-0002-0000-0400-000001000000}">
       <formula1>"Pass,Fail,N/A"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="G16" r:id="rId1" location="testing-for-sensitive-data-disclosure-in-local-storage"/>
-    <hyperlink ref="G17" r:id="rId2" location="testing-for-sensitive-data-in-logs"/>
-    <hyperlink ref="G18" r:id="rId3" location="testing-whether-sensitive-data-is-sent-to-third-parties"/>
-    <hyperlink ref="G19" r:id="rId4" location="testing-for-sensitive-data-in-the-keyboard-cache"/>
-    <hyperlink ref="G20" r:id="rId5" location="testing-for-sensitive-data-in-the-clipboard"/>
-    <hyperlink ref="G21" r:id="rId6" location="testing-whether-sensitive-data-is-exposed-via-ipc-mechanisms"/>
-    <hyperlink ref="G22" r:id="rId7" location="testing-for-sensitive-data-disclosure-through-the-user-interface"/>
-    <hyperlink ref="G23" r:id="rId8" location="testing-for-sensitive-data-in-backups"/>
-    <hyperlink ref="G29" r:id="rId9" location="verifying-cryptographic-key-management"/>
-    <hyperlink ref="G30" r:id="rId10" location="testing-for-custom-implementations-of-cryptography"/>
-    <hyperlink ref="G31" r:id="rId11" location="verifying-the-configuration-of-cryptographic-standard-algorithms"/>
-    <hyperlink ref="G32" r:id="rId12" location="testing-for-insecure-andor-deprecated-cryptographic-primitives"/>
-    <hyperlink ref="G33" r:id="rId13" location="testing-random-number-generation"/>
-    <hyperlink ref="G34" r:id="rId14" location="verifying-cryptographic-key-management"/>
-    <hyperlink ref="G36" r:id="rId15"/>
-    <hyperlink ref="G37" r:id="rId16"/>
-    <hyperlink ref="G41" r:id="rId17"/>
-    <hyperlink ref="G42" r:id="rId18"/>
-    <hyperlink ref="G43" r:id="rId19"/>
-    <hyperlink ref="G44" r:id="rId20"/>
-    <hyperlink ref="G45" r:id="rId21"/>
-    <hyperlink ref="G46" r:id="rId22"/>
-    <hyperlink ref="G48" r:id="rId23" location="testing-for-unencrypted-sensitive-data-on-the-network"/>
-    <hyperlink ref="G49" r:id="rId24" location="verifying-the-tls-settings"/>
-    <hyperlink ref="G50" r:id="rId25" location="testing-endpoint-identity-verification"/>
-    <hyperlink ref="G55" r:id="rId26" location="testing-app-permissions"/>
-    <hyperlink ref="G56" r:id="rId27" location="testing-input-validation-and-sanitization"/>
-    <hyperlink ref="G57" r:id="rId28" location="testing-custom-url-schemes"/>
-    <hyperlink ref="G58" r:id="rId29" location="testing-for-sensitive-functionality-exposed-through-ipc"/>
-    <hyperlink ref="G59" r:id="rId30" location="testing-javascript-execution-in-webviews"/>
-    <hyperlink ref="G60" r:id="rId31" location="testing-webview-protocol-handlers"/>
-    <hyperlink ref="G61" r:id="rId32" location="testing-whether-java-objects-are-exposed-through-webviews"/>
-    <hyperlink ref="G62" r:id="rId33" location="testing-object-serialization"/>
-    <hyperlink ref="G64" r:id="rId34" location="verifying-that-the-app-is-properly-signed"/>
-    <hyperlink ref="G65" r:id="rId35" location="testing-whether-the-app-is-debuggable"/>
-    <hyperlink ref="G66" r:id="rId36" location="verifying-that-debugging-symbols-have-been-removed"/>
-    <hyperlink ref="G67" r:id="rId37" location="testing-for-debugging-code-and-verbose-error-logging"/>
-    <hyperlink ref="G70" r:id="rId38" location="verifying-that-the-app-fails-securely"/>
-    <hyperlink ref="G72" r:id="rId39" location="testing-compiler-settings"/>
-    <hyperlink ref="G24" r:id="rId40" location="testing-for-sensitive-information-in-auto-generated-screenshots"/>
-    <hyperlink ref="G25" r:id="rId41"/>
-    <hyperlink ref="G26" r:id="rId42" location="testing-the-device-access-security-policy"/>
-    <hyperlink ref="G27" r:id="rId43" location="verifying-user-education-controls"/>
-    <hyperlink ref="G71" r:id="rId44" location="testing-for-memory-management-bugs"/>
-    <hyperlink ref="G38" r:id="rId45"/>
-    <hyperlink ref="G40" r:id="rId46"/>
-    <hyperlink ref="G39" r:id="rId47"/>
-    <hyperlink ref="G51" r:id="rId48" location="verifying-that-critical-operations-use-secure-communication-channels" display="Verifying that Critical Operations Use Secure Communication Channels"/>
-    <hyperlink ref="G52" r:id="rId49" location="testing-app-permissions"/>
-    <hyperlink ref="G53" r:id="rId50" location="testing-app-permissions"/>
-    <hyperlink ref="G69" r:id="rId51" location="testing-exception-handling"/>
+    <hyperlink ref="G16" r:id="rId1" location="testing-for-sensitive-data-disclosure-in-local-storage" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="G17" r:id="rId2" location="testing-for-sensitive-data-in-logs" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="G18" r:id="rId3" location="testing-whether-sensitive-data-is-sent-to-third-parties" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
+    <hyperlink ref="G19" r:id="rId4" location="testing-for-sensitive-data-in-the-keyboard-cache" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
+    <hyperlink ref="G20" r:id="rId5" location="testing-for-sensitive-data-in-the-clipboard" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
+    <hyperlink ref="G21" r:id="rId6" location="testing-whether-sensitive-data-is-exposed-via-ipc-mechanisms" xr:uid="{00000000-0004-0000-0400-000005000000}"/>
+    <hyperlink ref="G22" r:id="rId7" location="testing-for-sensitive-data-disclosure-through-the-user-interface" xr:uid="{00000000-0004-0000-0400-000006000000}"/>
+    <hyperlink ref="G23" r:id="rId8" location="testing-for-sensitive-data-in-backups" xr:uid="{00000000-0004-0000-0400-000007000000}"/>
+    <hyperlink ref="G29" r:id="rId9" location="verifying-cryptographic-key-management" xr:uid="{00000000-0004-0000-0400-000008000000}"/>
+    <hyperlink ref="G30" r:id="rId10" location="testing-for-custom-implementations-of-cryptography" xr:uid="{00000000-0004-0000-0400-000009000000}"/>
+    <hyperlink ref="G31" r:id="rId11" location="verifying-the-configuration-of-cryptographic-standard-algorithms" xr:uid="{00000000-0004-0000-0400-00000A000000}"/>
+    <hyperlink ref="G32" r:id="rId12" location="testing-for-insecure-andor-deprecated-cryptographic-primitives" xr:uid="{00000000-0004-0000-0400-00000B000000}"/>
+    <hyperlink ref="G33" r:id="rId13" location="testing-random-number-generation" xr:uid="{00000000-0004-0000-0400-00000C000000}"/>
+    <hyperlink ref="G34" r:id="rId14" location="verifying-cryptographic-key-management" xr:uid="{00000000-0004-0000-0400-00000D000000}"/>
+    <hyperlink ref="G36" r:id="rId15" xr:uid="{00000000-0004-0000-0400-00000E000000}"/>
+    <hyperlink ref="G37" r:id="rId16" xr:uid="{00000000-0004-0000-0400-00000F000000}"/>
+    <hyperlink ref="G41" r:id="rId17" xr:uid="{00000000-0004-0000-0400-000010000000}"/>
+    <hyperlink ref="G42" r:id="rId18" xr:uid="{00000000-0004-0000-0400-000011000000}"/>
+    <hyperlink ref="G43" r:id="rId19" xr:uid="{00000000-0004-0000-0400-000012000000}"/>
+    <hyperlink ref="G44" r:id="rId20" xr:uid="{00000000-0004-0000-0400-000013000000}"/>
+    <hyperlink ref="G45" r:id="rId21" xr:uid="{00000000-0004-0000-0400-000014000000}"/>
+    <hyperlink ref="G48" r:id="rId22" location="testing-for-unencrypted-sensitive-data-on-the-network" xr:uid="{00000000-0004-0000-0400-000016000000}"/>
+    <hyperlink ref="G49" r:id="rId23" location="verifying-the-tls-settings" xr:uid="{00000000-0004-0000-0400-000017000000}"/>
+    <hyperlink ref="G50" r:id="rId24" location="testing-endpoint-identity-verification" xr:uid="{00000000-0004-0000-0400-000018000000}"/>
+    <hyperlink ref="G55" r:id="rId25" location="testing-app-permissions" xr:uid="{00000000-0004-0000-0400-000019000000}"/>
+    <hyperlink ref="G56" r:id="rId26" location="testing-input-validation-and-sanitization" xr:uid="{00000000-0004-0000-0400-00001A000000}"/>
+    <hyperlink ref="G57" r:id="rId27" location="testing-custom-url-schemes" xr:uid="{00000000-0004-0000-0400-00001B000000}"/>
+    <hyperlink ref="G58" r:id="rId28" location="testing-for-sensitive-functionality-exposed-through-ipc" xr:uid="{00000000-0004-0000-0400-00001C000000}"/>
+    <hyperlink ref="G59" r:id="rId29" location="testing-javascript-execution-in-webviews" xr:uid="{00000000-0004-0000-0400-00001D000000}"/>
+    <hyperlink ref="G60" r:id="rId30" location="testing-webview-protocol-handlers" xr:uid="{00000000-0004-0000-0400-00001E000000}"/>
+    <hyperlink ref="G61" r:id="rId31" location="testing-whether-java-objects-are-exposed-through-webviews" xr:uid="{00000000-0004-0000-0400-00001F000000}"/>
+    <hyperlink ref="G62" r:id="rId32" location="testing-object-serialization" xr:uid="{00000000-0004-0000-0400-000020000000}"/>
+    <hyperlink ref="G64" r:id="rId33" location="verifying-that-the-app-is-properly-signed" xr:uid="{00000000-0004-0000-0400-000021000000}"/>
+    <hyperlink ref="G65" r:id="rId34" location="testing-whether-the-app-is-debuggable" xr:uid="{00000000-0004-0000-0400-000022000000}"/>
+    <hyperlink ref="G66" r:id="rId35" location="verifying-that-debugging-symbols-have-been-removed" xr:uid="{00000000-0004-0000-0400-000023000000}"/>
+    <hyperlink ref="G67" r:id="rId36" location="testing-for-debugging-code-and-verbose-error-logging" xr:uid="{00000000-0004-0000-0400-000024000000}"/>
+    <hyperlink ref="G70" r:id="rId37" location="verifying-that-the-app-fails-securely" xr:uid="{00000000-0004-0000-0400-000025000000}"/>
+    <hyperlink ref="G72" r:id="rId38" location="testing-compiler-settings" xr:uid="{00000000-0004-0000-0400-000026000000}"/>
+    <hyperlink ref="G24" r:id="rId39" location="testing-for-sensitive-information-in-auto-generated-screenshots" xr:uid="{00000000-0004-0000-0400-000027000000}"/>
+    <hyperlink ref="G25" r:id="rId40" xr:uid="{00000000-0004-0000-0400-000028000000}"/>
+    <hyperlink ref="G26" r:id="rId41" location="testing-the-device-access-security-policy" xr:uid="{00000000-0004-0000-0400-000029000000}"/>
+    <hyperlink ref="G27" r:id="rId42" location="verifying-user-education-controls" xr:uid="{00000000-0004-0000-0400-00002A000000}"/>
+    <hyperlink ref="G71" r:id="rId43" location="testing-for-memory-management-bugs" xr:uid="{00000000-0004-0000-0400-00002B000000}"/>
+    <hyperlink ref="G38" r:id="rId44" xr:uid="{00000000-0004-0000-0400-00002C000000}"/>
+    <hyperlink ref="G40" r:id="rId45" xr:uid="{00000000-0004-0000-0400-00002D000000}"/>
+    <hyperlink ref="G39" r:id="rId46" xr:uid="{00000000-0004-0000-0400-00002E000000}"/>
+    <hyperlink ref="G51" r:id="rId47" location="verifying-that-critical-operations-use-secure-communication-channels" display="Verifying that Critical Operations Use Secure Communication Channels" xr:uid="{00000000-0004-0000-0400-00002F000000}"/>
+    <hyperlink ref="G52" r:id="rId48" location="testing-app-permissions" xr:uid="{00000000-0004-0000-0400-000030000000}"/>
+    <hyperlink ref="G53" r:id="rId49" location="testing-app-permissions" xr:uid="{00000000-0004-0000-0400-000031000000}"/>
+    <hyperlink ref="G69" r:id="rId50" location="testing-exception-handling" xr:uid="{00000000-0004-0000-0400-000032000000}"/>
+    <hyperlink ref="G46" r:id="rId51" xr:uid="{00000000-0004-0000-0400-000015000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -7641,7 +7672,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B1:G32"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
@@ -8059,23 +8090,23 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E15 E17:E18 E5:E13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E15 E17:E18 E5:E13" xr:uid="{00000000-0002-0000-0500-000000000000}">
       <formula1>"Pass,Fail,N/A"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="F5" r:id="rId1" location="testing-root-detection"/>
-    <hyperlink ref="F6" r:id="rId2" location="testing-debugging-defenses"/>
-    <hyperlink ref="F7" r:id="rId3" location="testing-file-integrity-checks"/>
-    <hyperlink ref="F8" r:id="rId4" location="testing-detection-of-reverse-engineering-tools"/>
-    <hyperlink ref="F9" r:id="rId5" location="testing-simple-emulator-detection"/>
-    <hyperlink ref="F10" r:id="rId6" location="testing-memory-integrity-checks"/>
-    <hyperlink ref="F11" r:id="rId7" location="verifying-variablility-of-tampering-responses"/>
-    <hyperlink ref="F15" r:id="rId8" location="testing-device-binding"/>
-    <hyperlink ref="F17" r:id="rId9" location="testing-advanced-anti-emulation"/>
-    <hyperlink ref="F18" r:id="rId10" location="testing-advanced-obfuscation"/>
-    <hyperlink ref="F12" r:id="rId11"/>
-    <hyperlink ref="F13" r:id="rId12" location="testing-simple-obfuscation"/>
+    <hyperlink ref="F5" r:id="rId1" location="testing-root-detection" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="F6" r:id="rId2" location="testing-debugging-defenses" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
+    <hyperlink ref="F7" r:id="rId3" location="testing-file-integrity-checks" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
+    <hyperlink ref="F8" r:id="rId4" location="testing-detection-of-reverse-engineering-tools" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
+    <hyperlink ref="F9" r:id="rId5" location="testing-simple-emulator-detection" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
+    <hyperlink ref="F10" r:id="rId6" location="testing-memory-integrity-checks" xr:uid="{00000000-0004-0000-0500-000005000000}"/>
+    <hyperlink ref="F11" r:id="rId7" location="verifying-variablility-of-tampering-responses" xr:uid="{00000000-0004-0000-0500-000006000000}"/>
+    <hyperlink ref="F15" r:id="rId8" location="testing-device-binding" xr:uid="{00000000-0004-0000-0500-000007000000}"/>
+    <hyperlink ref="F17" r:id="rId9" location="testing-advanced-anti-emulation" xr:uid="{00000000-0004-0000-0500-000008000000}"/>
+    <hyperlink ref="F18" r:id="rId10" location="testing-advanced-obfuscation" xr:uid="{00000000-0004-0000-0500-000009000000}"/>
+    <hyperlink ref="F12" r:id="rId11" xr:uid="{00000000-0004-0000-0500-00000A000000}"/>
+    <hyperlink ref="F13" r:id="rId12" location="testing-simple-obfuscation" xr:uid="{00000000-0004-0000-0500-00000B000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -8083,7 +8114,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">

</xml_diff>

<commit_message>
updated checklist to new gitbook links
</commit_message>
<xml_diff>
--- a/Checklists/Mobile_App_Security_Checklist.xlsx
+++ b/Checklists/Mobile_App_Security_Checklist.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10116"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10709"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sven/PentestTools/OWASP/owasp-mstg/Checklists/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16132CFB-3404-694C-A5C8-D9FF01769632}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="32180" windowHeight="21140" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="6" r:id="rId1"/>
@@ -23,7 +24,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Security Requirements - Android'!$B$3:$H$72</definedName>
   </definedNames>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="179021" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="294">
   <si>
     <t>ID</t>
   </si>
@@ -626,9 +627,6 @@
     <t>Testing the Device-Access-Security Policy</t>
   </si>
   <si>
-    <t>Verifying User Education Controls</t>
-  </si>
-  <si>
     <t>Verifying Key Management</t>
   </si>
   <si>
@@ -671,9 +669,6 @@
     <t>Testing Step-up Authentication</t>
   </si>
   <si>
-    <t>Testing User Device Management</t>
-  </si>
-  <si>
     <t>Testing for Unencrypted Sensitive Data on the Network</t>
   </si>
   <si>
@@ -755,24 +750,12 @@
     <t>Testing Simple Emulator Detection</t>
   </si>
   <si>
-    <t>Testing Memory Integrity Checks</t>
-  </si>
-  <si>
-    <t>Verifying the Variability of Tampering Responses</t>
-  </si>
-  <si>
     <t>Testing Simple Obfuscation</t>
   </si>
   <si>
     <t>Testing Device Binding</t>
   </si>
   <si>
-    <t>Testing Advanced Anti-Emulation</t>
-  </si>
-  <si>
-    <t>Testing Advanced Obfuscation</t>
-  </si>
-  <si>
     <t>Resiliency Against Reverse Engineering - iOS</t>
   </si>
   <si>
@@ -860,18 +843,12 @@
     <t>Verify that the detection mechanisms trigger responses of different types, including delayed and stealthy responses.</t>
   </si>
   <si>
-    <t xml:space="preserve">Testing Detection Mechanisms </t>
-  </si>
-  <si>
     <t>Verify that all executable files and libraries belonging to the app are either encrypted on the file level and/or important code and data segments inside the executables are encrypted or packed. Trivial static analysis does not reveal important code or data.</t>
   </si>
   <si>
     <t>Verify that if the goal of obfuscation is to protect sensitive computations, an obfuscation scheme is used that is both appropriate for the particular task and robust against manual and automated de-obfuscation methods, considering currently published research. The effectiveness of the obfuscation scheme must be verified through manual testing. Note that hardware-based isolation features are prefered over obfuscation whenever possible.</t>
   </si>
   <si>
-    <t>Testing Detection Mechanisms</t>
-  </si>
-  <si>
     <t>Sync with MASVS (update requirements of domain 4 and R)</t>
   </si>
   <si>
@@ -879,9 +856,6 @@
   </si>
   <si>
     <t>Verify that all third party components used by the mobile app, such as libraries and frameworks, are identified, and checked for known vulnerabilities.</t>
-  </si>
-  <si>
-    <t>Testing 3rd party libraries</t>
   </si>
   <si>
     <t>Verify that a mechanism for enforcing updates of the mobile app exists.</t>
@@ -948,6 +922,15 @@
       <t xml:space="preserve">
 Based on the OWASP Mobile Application Security Verification Standard 1.1</t>
     </r>
+  </si>
+  <si>
+    <t>Testing Stateless Authentication</t>
+  </si>
+  <si>
+    <t>Testing Root Detection</t>
+  </si>
+  <si>
+    <t>Testing Run-Time Integrity Checks</t>
   </si>
 </sst>
 </file>
@@ -1685,7 +1668,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="125">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -1879,6 +1862,36 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1939,6 +1952,46 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="21" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="20" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="22" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1948,81 +2001,14 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="21" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="20" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="22" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="62">
@@ -3277,48 +3263,48 @@
   <sheetData>
     <row r="1" spans="2:4" ht="8" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B2" s="86" t="s">
-        <v>299</v>
-      </c>
-      <c r="C2" s="87"/>
-      <c r="D2" s="88"/>
+      <c r="B2" s="96" t="s">
+        <v>290</v>
+      </c>
+      <c r="C2" s="97"/>
+      <c r="D2" s="98"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="89"/>
-      <c r="C3" s="90"/>
-      <c r="D3" s="91"/>
+      <c r="B3" s="99"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="101"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B4" s="89"/>
-      <c r="C4" s="90"/>
-      <c r="D4" s="91"/>
+      <c r="B4" s="99"/>
+      <c r="C4" s="100"/>
+      <c r="D4" s="101"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="89"/>
-      <c r="C5" s="90"/>
-      <c r="D5" s="91"/>
+      <c r="B5" s="99"/>
+      <c r="C5" s="100"/>
+      <c r="D5" s="101"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B6" s="89"/>
-      <c r="C6" s="90"/>
-      <c r="D6" s="91"/>
+      <c r="B6" s="99"/>
+      <c r="C6" s="100"/>
+      <c r="D6" s="101"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B7" s="89"/>
-      <c r="C7" s="90"/>
-      <c r="D7" s="91"/>
+      <c r="B7" s="99"/>
+      <c r="C7" s="100"/>
+      <c r="D7" s="101"/>
     </row>
     <row r="8" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="92"/>
-      <c r="C8" s="93"/>
-      <c r="D8" s="94"/>
+      <c r="B8" s="102"/>
+      <c r="C8" s="103"/>
+      <c r="D8" s="104"/>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B9" s="95" t="s">
+      <c r="B9" s="105" t="s">
         <v>162</v>
       </c>
-      <c r="C9" s="83"/>
-      <c r="D9" s="84"/>
+      <c r="C9" s="93"/>
+      <c r="D9" s="94"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
@@ -3328,62 +3314,62 @@
       <c r="D10" s="3"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B11" s="81" t="s">
+      <c r="B11" s="91" t="s">
         <v>140</v>
       </c>
-      <c r="C11" s="82"/>
+      <c r="C11" s="92"/>
       <c r="D11" s="13"/>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B12" s="76" t="s">
+      <c r="B12" s="86" t="s">
         <v>141</v>
       </c>
-      <c r="C12" s="85"/>
+      <c r="C12" s="95"/>
       <c r="D12" s="13"/>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B13" s="81" t="s">
+      <c r="B13" s="91" t="s">
         <v>151</v>
       </c>
-      <c r="C13" s="82"/>
+      <c r="C13" s="92"/>
       <c r="D13" s="13"/>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B14" s="81" t="s">
+      <c r="B14" s="91" t="s">
         <v>142</v>
       </c>
-      <c r="C14" s="82"/>
+      <c r="C14" s="92"/>
       <c r="D14" s="13"/>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B15" s="81" t="s">
-        <v>250</v>
-      </c>
-      <c r="C15" s="82"/>
+      <c r="B15" s="91" t="s">
+        <v>244</v>
+      </c>
+      <c r="C15" s="92"/>
       <c r="D15" s="13"/>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B16" s="81" t="s">
+      <c r="B16" s="91" t="s">
         <v>161</v>
       </c>
-      <c r="C16" s="82"/>
+      <c r="C16" s="92"/>
       <c r="D16" s="13" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="81" t="s">
+      <c r="B17" s="91" t="s">
         <v>163</v>
       </c>
-      <c r="C17" s="82"/>
+      <c r="C17" s="92"/>
       <c r="D17" s="13" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B18" s="83"/>
-      <c r="C18" s="83"/>
-      <c r="D18" s="84"/>
+      <c r="B18" s="93"/>
+      <c r="C18" s="93"/>
+      <c r="D18" s="94"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
@@ -3400,37 +3386,37 @@
       <c r="D20" s="13"/>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B21" s="81" t="s">
+      <c r="B21" s="91" t="s">
         <v>153</v>
       </c>
-      <c r="C21" s="82"/>
+      <c r="C21" s="92"/>
       <c r="D21" s="13"/>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B22" s="81" t="s">
+      <c r="B22" s="91" t="s">
         <v>154</v>
       </c>
-      <c r="C22" s="82"/>
+      <c r="C22" s="92"/>
       <c r="D22" s="13"/>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B23" s="81" t="s">
+      <c r="B23" s="91" t="s">
         <v>155</v>
       </c>
-      <c r="C23" s="82"/>
+      <c r="C23" s="92"/>
       <c r="D23" s="13"/>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B24" s="81" t="s">
+      <c r="B24" s="91" t="s">
         <v>156</v>
       </c>
-      <c r="C24" s="82"/>
+      <c r="C24" s="92"/>
       <c r="D24" s="13"/>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B25" s="83"/>
-      <c r="C25" s="83"/>
-      <c r="D25" s="84"/>
+      <c r="B25" s="93"/>
+      <c r="C25" s="93"/>
+      <c r="D25" s="94"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
@@ -3447,37 +3433,37 @@
       <c r="D27" s="13"/>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B28" s="81" t="s">
+      <c r="B28" s="91" t="s">
         <v>144</v>
       </c>
-      <c r="C28" s="82"/>
+      <c r="C28" s="92"/>
       <c r="D28" s="13"/>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B29" s="81" t="s">
+      <c r="B29" s="91" t="s">
         <v>154</v>
       </c>
-      <c r="C29" s="82"/>
+      <c r="C29" s="92"/>
       <c r="D29" s="13"/>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B30" s="81" t="s">
+      <c r="B30" s="91" t="s">
         <v>155</v>
       </c>
-      <c r="C30" s="82"/>
+      <c r="C30" s="92"/>
       <c r="D30" s="13"/>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B31" s="81" t="s">
+      <c r="B31" s="91" t="s">
         <v>158</v>
       </c>
-      <c r="C31" s="82"/>
+      <c r="C31" s="92"/>
       <c r="D31" s="13"/>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B32" s="83"/>
-      <c r="C32" s="83"/>
-      <c r="D32" s="84"/>
+      <c r="B32" s="93"/>
+      <c r="C32" s="93"/>
+      <c r="D32" s="94"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
@@ -3487,83 +3473,83 @@
       <c r="D33" s="3"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B34" s="78"/>
-      <c r="C34" s="79"/>
-      <c r="D34" s="80"/>
+      <c r="B34" s="88"/>
+      <c r="C34" s="89"/>
+      <c r="D34" s="90"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B35" s="76" t="s">
+      <c r="B35" s="86" t="s">
         <v>146</v>
       </c>
-      <c r="C35" s="77"/>
+      <c r="C35" s="87"/>
       <c r="D35" s="62"/>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B36" s="76" t="s">
+      <c r="B36" s="86" t="s">
         <v>147</v>
       </c>
-      <c r="C36" s="77"/>
+      <c r="C36" s="87"/>
       <c r="D36" s="62"/>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B37" s="76" t="s">
+      <c r="B37" s="86" t="s">
         <v>148</v>
       </c>
-      <c r="C37" s="77"/>
+      <c r="C37" s="87"/>
       <c r="D37" s="62"/>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B38" s="76" t="s">
+      <c r="B38" s="86" t="s">
         <v>149</v>
       </c>
-      <c r="C38" s="77"/>
+      <c r="C38" s="87"/>
       <c r="D38" s="63"/>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B39" s="76" t="s">
+      <c r="B39" s="86" t="s">
         <v>150</v>
       </c>
-      <c r="C39" s="77"/>
+      <c r="C39" s="87"/>
       <c r="D39" s="62"/>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B40" s="78"/>
-      <c r="C40" s="79"/>
-      <c r="D40" s="80"/>
+      <c r="B40" s="88"/>
+      <c r="C40" s="89"/>
+      <c r="D40" s="90"/>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B41" s="76" t="s">
+      <c r="B41" s="86" t="s">
         <v>146</v>
       </c>
-      <c r="C41" s="77"/>
+      <c r="C41" s="87"/>
       <c r="D41" s="62"/>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B42" s="76" t="s">
+      <c r="B42" s="86" t="s">
         <v>147</v>
       </c>
-      <c r="C42" s="77"/>
+      <c r="C42" s="87"/>
       <c r="D42" s="62"/>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B43" s="76" t="s">
+      <c r="B43" s="86" t="s">
         <v>148</v>
       </c>
-      <c r="C43" s="77"/>
+      <c r="C43" s="87"/>
       <c r="D43" s="62"/>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B44" s="76" t="s">
+      <c r="B44" s="86" t="s">
         <v>149</v>
       </c>
-      <c r="C44" s="77"/>
+      <c r="C44" s="87"/>
       <c r="D44" s="63"/>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B45" s="76" t="s">
+      <c r="B45" s="86" t="s">
         <v>150</v>
       </c>
-      <c r="C45" s="77"/>
+      <c r="C45" s="87"/>
       <c r="D45" s="62"/>
     </row>
   </sheetData>
@@ -3612,7 +3598,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:X50"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="L43" sqref="L43"/>
     </sheetView>
   </sheetViews>
@@ -3646,11 +3632,11 @@
       <c r="F3" s="9"/>
     </row>
     <row r="4" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B4" s="112"/>
-      <c r="C4" s="112"/>
-      <c r="D4" s="112"/>
-      <c r="E4" s="112"/>
-      <c r="F4" s="112"/>
+      <c r="B4" s="110"/>
+      <c r="C4" s="110"/>
+      <c r="D4" s="110"/>
+      <c r="E4" s="110"/>
+      <c r="F4" s="110"/>
     </row>
     <row r="5" spans="2:24" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B5" s="21"/>
@@ -3665,16 +3651,16 @@
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
       <c r="F6" s="22"/>
-      <c r="G6" s="96" t="s">
+      <c r="G6" s="120" t="s">
         <v>174</v>
       </c>
-      <c r="H6" s="97"/>
-      <c r="I6" s="98"/>
-      <c r="V6" s="96" t="s">
+      <c r="H6" s="121"/>
+      <c r="I6" s="122"/>
+      <c r="V6" s="120" t="s">
         <v>174</v>
       </c>
-      <c r="W6" s="97"/>
-      <c r="X6" s="98"/>
+      <c r="W6" s="121"/>
+      <c r="X6" s="122"/>
     </row>
     <row r="7" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B7" s="14"/>
@@ -3689,18 +3675,18 @@
       <c r="D8" s="21"/>
       <c r="E8" s="21"/>
       <c r="F8" s="21"/>
-      <c r="G8" s="99">
+      <c r="G8" s="111">
         <f>AVERAGE(G43:G50)*5</f>
         <v>0</v>
       </c>
-      <c r="H8" s="100"/>
-      <c r="I8" s="101"/>
-      <c r="V8" s="99">
+      <c r="H8" s="112"/>
+      <c r="I8" s="113"/>
+      <c r="V8" s="111">
         <f>AVERAGE(K43:K50)*5</f>
         <v>0</v>
       </c>
-      <c r="W8" s="100"/>
-      <c r="X8" s="101"/>
+      <c r="W8" s="112"/>
+      <c r="X8" s="113"/>
     </row>
     <row r="9" spans="2:24" ht="91" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="22"/>
@@ -3708,12 +3694,12 @@
       <c r="D9" s="22"/>
       <c r="E9" s="22"/>
       <c r="F9" s="22"/>
-      <c r="G9" s="102"/>
-      <c r="H9" s="103"/>
-      <c r="I9" s="104"/>
-      <c r="V9" s="102"/>
-      <c r="W9" s="103"/>
-      <c r="X9" s="104"/>
+      <c r="G9" s="114"/>
+      <c r="H9" s="115"/>
+      <c r="I9" s="116"/>
+      <c r="V9" s="114"/>
+      <c r="W9" s="115"/>
+      <c r="X9" s="116"/>
     </row>
     <row r="10" spans="2:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="14"/>
@@ -3721,12 +3707,12 @@
       <c r="D10" s="14"/>
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
-      <c r="G10" s="102"/>
-      <c r="H10" s="103"/>
-      <c r="I10" s="104"/>
-      <c r="V10" s="102"/>
-      <c r="W10" s="103"/>
-      <c r="X10" s="104"/>
+      <c r="G10" s="114"/>
+      <c r="H10" s="115"/>
+      <c r="I10" s="116"/>
+      <c r="V10" s="114"/>
+      <c r="W10" s="115"/>
+      <c r="X10" s="116"/>
     </row>
     <row r="11" spans="2:24" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B11" s="14"/>
@@ -3734,19 +3720,19 @@
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
-      <c r="G11" s="105"/>
-      <c r="H11" s="106"/>
-      <c r="I11" s="107"/>
-      <c r="V11" s="105"/>
-      <c r="W11" s="106"/>
-      <c r="X11" s="107"/>
+      <c r="G11" s="117"/>
+      <c r="H11" s="118"/>
+      <c r="I11" s="119"/>
+      <c r="V11" s="117"/>
+      <c r="W11" s="118"/>
+      <c r="X11" s="119"/>
     </row>
     <row r="12" spans="2:24" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B12" s="108"/>
-      <c r="C12" s="108"/>
-      <c r="D12" s="108"/>
-      <c r="E12" s="108"/>
-      <c r="F12" s="108"/>
+      <c r="B12" s="106"/>
+      <c r="C12" s="106"/>
+      <c r="D12" s="106"/>
+      <c r="E12" s="106"/>
+      <c r="F12" s="106"/>
     </row>
     <row r="13" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B13" s="15"/>
@@ -3770,11 +3756,11 @@
       <c r="F15" s="14"/>
     </row>
     <row r="16" spans="2:24" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="108"/>
-      <c r="C16" s="108"/>
-      <c r="D16" s="108"/>
-      <c r="E16" s="108"/>
-      <c r="F16" s="108"/>
+      <c r="B16" s="106"/>
+      <c r="C16" s="106"/>
+      <c r="D16" s="106"/>
+      <c r="E16" s="106"/>
+      <c r="F16" s="106"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B17" s="15"/>
@@ -3827,18 +3813,18 @@
     </row>
     <row r="35" spans="3:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="41" spans="3:11" x14ac:dyDescent="0.15">
-      <c r="D41" s="109" t="s">
+      <c r="D41" s="107" t="s">
         <v>172</v>
       </c>
-      <c r="E41" s="110"/>
-      <c r="F41" s="110"/>
-      <c r="G41" s="111"/>
-      <c r="H41" s="109" t="s">
+      <c r="E41" s="108"/>
+      <c r="F41" s="108"/>
+      <c r="G41" s="109"/>
+      <c r="H41" s="107" t="s">
         <v>173</v>
       </c>
-      <c r="I41" s="110"/>
-      <c r="J41" s="110"/>
-      <c r="K41" s="111"/>
+      <c r="I41" s="108"/>
+      <c r="J41" s="108"/>
+      <c r="K41" s="109"/>
     </row>
     <row r="42" spans="3:11" x14ac:dyDescent="0.15">
       <c r="D42" s="18" t="s">
@@ -4053,7 +4039,7 @@
     </row>
     <row r="48" spans="3:11" x14ac:dyDescent="0.15">
       <c r="C48" s="12" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="D48" s="10">
         <f>COUNTIFS('Security Requirements - Android'!F55:F62,'Security Requirements - Android'!B79)</f>
@@ -4164,15 +4150,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="G8:I11"/>
-    <mergeCell ref="G6:I6"/>
     <mergeCell ref="V6:X6"/>
     <mergeCell ref="V8:X11"/>
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="B16:F16"/>
     <mergeCell ref="D41:G41"/>
     <mergeCell ref="H41:K41"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="G8:I11"/>
+    <mergeCell ref="G6:I6"/>
   </mergeCells>
   <conditionalFormatting sqref="F14">
     <cfRule type="iconSet" priority="3">
@@ -4213,8 +4199,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B1:J85"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView showGridLines="0" topLeftCell="A41" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="G58" sqref="G58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4230,15 +4216,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="19" x14ac:dyDescent="0.2">
-      <c r="B1" s="113" t="s">
+      <c r="B1" s="123" t="s">
         <v>175</v>
       </c>
-      <c r="C1" s="113"/>
-      <c r="D1" s="113"/>
-      <c r="E1" s="113"/>
-      <c r="F1" s="113"/>
-      <c r="G1" s="113"/>
-      <c r="H1" s="113"/>
+      <c r="C1" s="123"/>
+      <c r="D1" s="123"/>
+      <c r="E1" s="123"/>
+      <c r="F1" s="123"/>
+      <c r="G1" s="123"/>
+      <c r="H1" s="123"/>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B2" s="50"/>
@@ -4442,7 +4428,7 @@
         <v>1.9</v>
       </c>
       <c r="C13" s="36" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="D13" s="36"/>
       <c r="E13" s="51" t="s">
@@ -4461,7 +4447,7 @@
         <v>9</v>
       </c>
       <c r="C14" s="36" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="D14" s="36"/>
       <c r="E14" s="51" t="s">
@@ -4493,7 +4479,7 @@
         <v>11</v>
       </c>
       <c r="C16" s="56" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="D16" s="26" t="s">
         <v>7</v>
@@ -4512,12 +4498,14 @@
         <v>65</v>
       </c>
       <c r="C17" s="56" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="D17" s="26"/>
       <c r="E17" s="51"/>
       <c r="F17" s="37"/>
-      <c r="G17" s="58"/>
+      <c r="G17" s="58" t="s">
+        <v>186</v>
+      </c>
       <c r="H17" s="74"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.2">
@@ -4601,7 +4589,7 @@
         <v>14</v>
       </c>
       <c r="C22" s="56" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="D22" s="26" t="s">
         <v>7</v>
@@ -4611,7 +4599,7 @@
       </c>
       <c r="F22" s="37"/>
       <c r="G22" s="58" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="H22" s="74"/>
     </row>
@@ -4620,7 +4608,7 @@
         <v>15</v>
       </c>
       <c r="C23" s="56" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="D23" s="56"/>
       <c r="E23" s="51" t="s">
@@ -4736,7 +4724,7 @@
       </c>
       <c r="F29" s="37"/>
       <c r="G29" s="58" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H29" s="74"/>
     </row>
@@ -4755,7 +4743,7 @@
       </c>
       <c r="F30" s="37"/>
       <c r="G30" s="58" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H30" s="74"/>
     </row>
@@ -4774,7 +4762,7 @@
       </c>
       <c r="F31" s="37"/>
       <c r="G31" s="58" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H31" s="74"/>
     </row>
@@ -4793,7 +4781,7 @@
       </c>
       <c r="F32" s="37"/>
       <c r="G32" s="58" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H32" s="74"/>
     </row>
@@ -4812,7 +4800,7 @@
       </c>
       <c r="F33" s="37"/>
       <c r="G33" s="58" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="H33" s="74"/>
     </row>
@@ -4831,7 +4819,7 @@
       </c>
       <c r="F34" s="37"/>
       <c r="G34" s="58" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="H34" s="74"/>
     </row>
@@ -4863,7 +4851,7 @@
       </c>
       <c r="F36" s="37"/>
       <c r="G36" s="58" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H36" s="74"/>
     </row>
@@ -4872,7 +4860,7 @@
         <v>84</v>
       </c>
       <c r="C37" s="56" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D37" s="26" t="s">
         <v>7</v>
@@ -4882,7 +4870,7 @@
       </c>
       <c r="F37" s="37"/>
       <c r="G37" s="58" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H37" s="74"/>
     </row>
@@ -4891,7 +4879,7 @@
         <v>85</v>
       </c>
       <c r="C38" s="56" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="D38" s="26" t="s">
         <v>7</v>
@@ -4901,7 +4889,7 @@
       </c>
       <c r="F38" s="37"/>
       <c r="G38" s="58" t="s">
-        <v>203</v>
+        <v>291</v>
       </c>
       <c r="H38" s="74"/>
       <c r="J38" s="58"/>
@@ -4911,13 +4899,13 @@
         <v>27</v>
       </c>
       <c r="C39" s="56" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="D39" s="26"/>
       <c r="E39" s="51"/>
       <c r="F39" s="37"/>
       <c r="G39" s="58" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H39" s="74"/>
       <c r="J39" s="58"/>
@@ -4937,7 +4925,7 @@
       </c>
       <c r="F40" s="37"/>
       <c r="G40" s="58" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H40" s="74"/>
     </row>
@@ -4946,7 +4934,7 @@
         <v>86</v>
       </c>
       <c r="C41" s="56" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="D41" s="26" t="s">
         <v>7</v>
@@ -4956,7 +4944,7 @@
       </c>
       <c r="F41" s="37"/>
       <c r="G41" s="58" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H41" s="74"/>
     </row>
@@ -4965,7 +4953,7 @@
         <v>87</v>
       </c>
       <c r="C42" s="56" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="D42" s="26" t="s">
         <v>7</v>
@@ -4975,7 +4963,7 @@
       </c>
       <c r="F42" s="37"/>
       <c r="G42" s="58" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H42" s="58"/>
     </row>
@@ -4994,7 +4982,7 @@
         <v>136</v>
       </c>
       <c r="G43" s="58" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H43" s="74"/>
     </row>
@@ -5013,7 +5001,7 @@
         <v>136</v>
       </c>
       <c r="G44" s="58" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H44" s="74"/>
     </row>
@@ -5032,13 +5020,13 @@
         <v>136</v>
       </c>
       <c r="G45" s="58" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H45" s="74"/>
     </row>
     <row r="46" spans="2:10" ht="30" x14ac:dyDescent="0.2">
       <c r="B46" s="55" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="C46" s="56" t="s">
         <v>93</v>
@@ -5050,9 +5038,7 @@
       <c r="F46" s="37" t="s">
         <v>136</v>
       </c>
-      <c r="G46" s="58" t="s">
-        <v>211</v>
-      </c>
+      <c r="G46" s="58"/>
       <c r="H46" s="74"/>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.2">
@@ -5083,11 +5069,11 @@
       </c>
       <c r="F48" s="37"/>
       <c r="G48" s="58" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="H48" s="74"/>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B49" s="55" t="s">
         <v>95</v>
       </c>
@@ -5102,7 +5088,7 @@
       </c>
       <c r="F49" s="37"/>
       <c r="G49" s="58" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H49" s="74"/>
     </row>
@@ -5121,7 +5107,7 @@
       </c>
       <c r="F50" s="37"/>
       <c r="G50" s="58" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="H50" s="74"/>
     </row>
@@ -5140,7 +5126,7 @@
         <v>136</v>
       </c>
       <c r="G51" s="58" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="H51" s="74"/>
     </row>
@@ -5159,7 +5145,7 @@
         <v>136</v>
       </c>
       <c r="G52" s="58" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="H52" s="74"/>
     </row>
@@ -5168,7 +5154,7 @@
         <v>5.6</v>
       </c>
       <c r="C53" s="56" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="D53" s="56"/>
       <c r="E53" s="51" t="s">
@@ -5178,7 +5164,7 @@
         <v>136</v>
       </c>
       <c r="G53" s="58" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="H53" s="74"/>
     </row>
@@ -5187,7 +5173,7 @@
         <v>36</v>
       </c>
       <c r="C54" s="39" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D54" s="39"/>
       <c r="E54" s="54"/>
@@ -5210,7 +5196,7 @@
       </c>
       <c r="F55" s="37"/>
       <c r="G55" s="58" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="H55" s="74"/>
     </row>
@@ -5229,7 +5215,7 @@
       </c>
       <c r="F56" s="37"/>
       <c r="G56" s="58" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="H56" s="74"/>
     </row>
@@ -5248,7 +5234,7 @@
       </c>
       <c r="F57" s="37"/>
       <c r="G57" s="58" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="H57" s="74"/>
     </row>
@@ -5267,7 +5253,7 @@
       </c>
       <c r="F58" s="37"/>
       <c r="G58" s="58" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H58" s="74"/>
     </row>
@@ -5286,7 +5272,7 @@
       </c>
       <c r="F59" s="37"/>
       <c r="G59" s="58" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="H59" s="74"/>
     </row>
@@ -5305,16 +5291,16 @@
       </c>
       <c r="F60" s="37"/>
       <c r="G60" s="58" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="H60" s="74"/>
     </row>
     <row r="61" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B61" s="55" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="C61" s="56" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="D61" s="26" t="s">
         <v>7</v>
@@ -5324,7 +5310,7 @@
       </c>
       <c r="F61" s="37"/>
       <c r="G61" s="58" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="H61" s="74"/>
     </row>
@@ -5343,7 +5329,7 @@
       </c>
       <c r="F62" s="37"/>
       <c r="G62" s="58" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="H62" s="74"/>
     </row>
@@ -5375,7 +5361,7 @@
       </c>
       <c r="F64" s="37"/>
       <c r="G64" s="58" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="H64" s="74"/>
     </row>
@@ -5394,7 +5380,7 @@
       </c>
       <c r="F65" s="37"/>
       <c r="G65" s="58" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="H65" s="74"/>
     </row>
@@ -5413,7 +5399,7 @@
       </c>
       <c r="F66" s="37"/>
       <c r="G66" s="58" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="H66" s="74"/>
     </row>
@@ -5432,7 +5418,7 @@
       </c>
       <c r="F67" s="37"/>
       <c r="G67" s="58" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H67" s="74"/>
     </row>
@@ -5441,7 +5427,7 @@
         <v>117</v>
       </c>
       <c r="C68" s="56" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="D68" s="26" t="s">
         <v>7</v>
@@ -5450,9 +5436,7 @@
         <v>7</v>
       </c>
       <c r="F68" s="37"/>
-      <c r="G68" s="58" t="s">
-        <v>281</v>
-      </c>
+      <c r="G68" s="58"/>
       <c r="H68" s="74"/>
     </row>
     <row r="69" spans="2:8" x14ac:dyDescent="0.2">
@@ -5470,7 +5454,7 @@
       </c>
       <c r="F69" s="37"/>
       <c r="G69" s="58" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="H69" s="74"/>
     </row>
@@ -5489,7 +5473,7 @@
       </c>
       <c r="F70" s="37"/>
       <c r="G70" s="58" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="H70" s="74"/>
     </row>
@@ -5508,16 +5492,16 @@
       </c>
       <c r="F71" s="37"/>
       <c r="G71" s="58" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="H71" s="74"/>
     </row>
     <row r="72" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B72" s="55" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="C72" s="56" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="D72" s="26" t="s">
         <v>7</v>
@@ -5527,7 +5511,7 @@
       </c>
       <c r="F72" s="37"/>
       <c r="G72" s="58" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="H72" s="74"/>
     </row>
@@ -5679,55 +5663,55 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="G16" r:id="rId1" location="testing-for-sensitive-data-in-local-storage" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x05d-Testing-Data-Storage.html - testing-for-sensitive-data-in-local-storage" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="G18" r:id="rId2" location="testing-for-sensitive-data-in-logs" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x05d-Testing-Data-Storage.html - testing-for-sensitive-data-in-logs" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="G19" r:id="rId3" location="testing-whether-sensitive-data-is-sent-to-third-parties" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x05d-Testing-Data-Storage.html - testing-whether-sensitive-data-is-sent-to-third-parties" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink ref="G20" r:id="rId4" location="testing-whether-the-keyboard-cache-is-disabled-for-text-input-fields" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x05d-Testing-Data-Storage.html - testing-whether-the-keyboard-cache-is-disabled-for-text-input-fields" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
-    <hyperlink ref="G21" r:id="rId5" location="testing-whether-sensitive-data-is-exposed-via-ipc-mechanisms" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x05d-Testing-Data-Storage.html - testing-whether-sensitive-data-is-exposed-via-ipc-mechanisms" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
-    <hyperlink ref="G23" r:id="rId6" location="testing-for-sensitive-data-in-backups" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x05d-Testing-Data-Storage.html - testing-for-sensitive-data-in-backups" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
-    <hyperlink ref="G24" r:id="rId7" location="testing-for-sensitive-information-in-auto-generated-screenshots" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x05d-Testing-Data-Storage.html - testing-for-sensitive-information-in-auto-generated-screenshots" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
-    <hyperlink ref="G25" r:id="rId8" location="testing-for-sensitive-data-in-memory" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x05d-Testing-Data-Storage.html - testing-for-sensitive-data-in-memory" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
-    <hyperlink ref="G26" r:id="rId9" location="testing-the-device-access-security-policy" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x05d-Testing-Data-Storage.html - testing-the-device-access-security-policy" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
-    <hyperlink ref="G29" r:id="rId10" location="verifying-key-management" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x05e-Testing-Cryptography.html - verifying-key-management" xr:uid="{00000000-0004-0000-0200-00000B000000}"/>
-    <hyperlink ref="G30" r:id="rId11" location="testing-for-custom-implementations-of-cryptography" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x05e-Testing-Cryptography.html - testing-for-custom-implementations-of-cryptography" xr:uid="{00000000-0004-0000-0200-00000C000000}"/>
-    <hyperlink ref="G31" r:id="rId12" location="verifying-the-configuration-of-cryptographic-standard-algorithms" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x05e-Testing-Cryptography.html - verifying-the-configuration-of-cryptographic-standard-algorithms" xr:uid="{00000000-0004-0000-0200-00000D000000}"/>
-    <hyperlink ref="G32" r:id="rId13" location="testing-for-insecure-andor-deprecated-cryptographic-algorithms" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x05e-Testing-Cryptography.html - testing-for-insecure-andor-deprecated-cryptographic-algorithms" xr:uid="{00000000-0004-0000-0200-00000E000000}"/>
-    <hyperlink ref="G33" r:id="rId14" location="testing-random-number-generation" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x05e-Testing-Cryptography.html - testing-random-number-generation" xr:uid="{00000000-0004-0000-0200-00000F000000}"/>
-    <hyperlink ref="G34" r:id="rId15" location="verifying-key-management" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x05e-Testing-Cryptography.html - verifying-key-management" xr:uid="{00000000-0004-0000-0200-000010000000}"/>
-    <hyperlink ref="G41" r:id="rId16" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x04e-Testing-Authentication-and-Session-Management.html" xr:uid="{00000000-0004-0000-0200-000011000000}"/>
-    <hyperlink ref="G44" r:id="rId17" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x04e-Testing-Authentication-and-Session-Management.html" xr:uid="{00000000-0004-0000-0200-000014000000}"/>
-    <hyperlink ref="G45" r:id="rId18" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x04e-Testing-Authentication-and-Session-Management.html" xr:uid="{00000000-0004-0000-0200-000015000000}"/>
-    <hyperlink ref="G46" r:id="rId19" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x04e-Testing-Authentication-and-Session-Management.html" xr:uid="{00000000-0004-0000-0200-000016000000}"/>
-    <hyperlink ref="G48" r:id="rId20" location="testing-for-unencrypted-sensitive-data-on-the-network" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x05g-Testing-Network-Communication.html - testing-for-unencrypted-sensitive-data-on-the-network" xr:uid="{00000000-0004-0000-0200-000017000000}"/>
-    <hyperlink ref="G49" r:id="rId21" location="verifying-the-tls-settings" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x05g-Testing-Network-Communication.html - verifying-the-tls-settings" xr:uid="{00000000-0004-0000-0200-000018000000}"/>
-    <hyperlink ref="G50" r:id="rId22" location="testing-endpoint-identify-verification" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x05g-Testing-Network-Communication.html - testing-endpoint-identify-verification" xr:uid="{00000000-0004-0000-0200-000019000000}"/>
-    <hyperlink ref="G51" r:id="rId23" location="testing-custom-certificate-stores-and-ssl-pinning" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x05g-Testing-Network-Communication.html - testing-custom-certificate-stores-and-ssl-pinning" xr:uid="{00000000-0004-0000-0200-00001A000000}"/>
-    <hyperlink ref="G55" r:id="rId24" location="testing-app-permissions" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x05h-Testing-Platform-Interaction.html - testing-app-permissions" xr:uid="{00000000-0004-0000-0200-00001B000000}"/>
-    <hyperlink ref="G56" r:id="rId25" location="testing-input-validation-and-sanitization" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x05h-Testing-Platform-Interaction.html - testing-input-validation-and-sanitization" xr:uid="{00000000-0004-0000-0200-00001C000000}"/>
-    <hyperlink ref="G57" r:id="rId26" location="testing-custom-url-schemes" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x05h-Testing-Platform-Interaction.html - testing-custom-url-schemes" xr:uid="{00000000-0004-0000-0200-00001D000000}"/>
-    <hyperlink ref="G58" r:id="rId27" location="testing-for-sensitive-functionality-exposure-through-ipc" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x05h-Testing-Platform-Interaction.html - testing-for-sensitive-functionality-exposure-through-ipc" xr:uid="{00000000-0004-0000-0200-00001E000000}"/>
-    <hyperlink ref="G59" r:id="rId28" location="testing-javascript-execution-in-webviews" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x05h-Testing-Platform-Interaction.html - testing-javascript-execution-in-webviews" xr:uid="{00000000-0004-0000-0200-00001F000000}"/>
-    <hyperlink ref="G60" r:id="rId29" location="testing-webview-protocol-handlers" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x05h-Testing-Platform-Interaction.html - testing-webview-protocol-handlers" xr:uid="{00000000-0004-0000-0200-000020000000}"/>
-    <hyperlink ref="G61" r:id="rId30" location="testing-whether-java-objects-are-exposed-through-webviews" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x05h-Testing-Platform-Interaction.html - testing-whether-java-objects-are-exposed-through-webviews" xr:uid="{00000000-0004-0000-0200-000021000000}"/>
-    <hyperlink ref="G62" r:id="rId31" location="testing-object-de-serialization" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x05h-Testing-Platform-Interaction.html - testing-object-de-serialization" xr:uid="{00000000-0004-0000-0200-000022000000}"/>
-    <hyperlink ref="G64" r:id="rId32" location="verifying-that-the-app-is-properly-signed" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x05i-Testing-Code-Quality-and-Build-Settings.html - verifying-that-the-app-is-properly-signed" xr:uid="{00000000-0004-0000-0200-000023000000}"/>
-    <hyperlink ref="G65" r:id="rId33" location="testing-if-the-app-is-debuggable" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x05i-Testing-Code-Quality-and-Build-Settings.html - testing-if-the-app-is-debuggable" xr:uid="{00000000-0004-0000-0200-000024000000}"/>
-    <hyperlink ref="G66" r:id="rId34" location="testing-for-debugging-symbols" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x05i-Testing-Code-Quality-and-Build-Settings.html - testing-for-debugging-symbols" xr:uid="{00000000-0004-0000-0200-000025000000}"/>
-    <hyperlink ref="G67" r:id="rId35" location="testing-for-debugging-code-and-verbose-error-logging" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x05i-Testing-Code-Quality-and-Build-Settings.html - testing-for-debugging-code-and-verbose-error-logging" xr:uid="{00000000-0004-0000-0200-000026000000}"/>
-    <hyperlink ref="G70" r:id="rId36" location="testing-exception-handling" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x05i-Testing-Code-Quality-and-Build-Settings.html - testing-exception-handling" xr:uid="{00000000-0004-0000-0200-000027000000}"/>
-    <hyperlink ref="G71" r:id="rId37" location="testing-for-memory-management-bugs" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x05i-Testing-Code-Quality-and-Build-Settings.html - testing-for-memory-management-bugs" xr:uid="{00000000-0004-0000-0200-000028000000}"/>
-    <hyperlink ref="G72" r:id="rId38" location="verifying-compiler-settings" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x05i-Testing-Code-Quality-and-Build-Settings.html - verifying-compiler-settings" xr:uid="{00000000-0004-0000-0200-000029000000}"/>
-    <hyperlink ref="G36" r:id="rId39" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x04e-Testing-Authentication-and-Session-Management.html" xr:uid="{00000000-0004-0000-0200-00002A000000}"/>
-    <hyperlink ref="G37" r:id="rId40" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x04e-Testing-Authentication-and-Session-Management.html" xr:uid="{00000000-0004-0000-0200-00002B000000}"/>
-    <hyperlink ref="G22" r:id="rId41" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x05d-Testing-Data-Storage.html" xr:uid="{00000000-0004-0000-0200-00002C000000}"/>
-    <hyperlink ref="G40" r:id="rId42" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x04e-Testing-Authentication-and-Session-Management.html" xr:uid="{00000000-0004-0000-0200-00002D000000}"/>
-    <hyperlink ref="G52" r:id="rId43" location="verifying-that-critical-operations-use-secure-communication-channels" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x05g-Testing-Network-Communication.html - verifying-that-critical-operations-use-secure-communication-channels" xr:uid="{00000000-0004-0000-0200-00002E000000}"/>
-    <hyperlink ref="G53" r:id="rId44" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/" xr:uid="{00000000-0004-0000-0200-00002F000000}"/>
-    <hyperlink ref="G39" r:id="rId45" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x04e-Testing-Authentication-and-Session-Management.html" xr:uid="{00000000-0004-0000-0200-000030000000}"/>
-    <hyperlink ref="G38" r:id="rId46" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x04e-Testing-Authentication-and-Session-Management.html" xr:uid="{00000000-0004-0000-0200-000031000000}"/>
-    <hyperlink ref="G69" r:id="rId47" location="testing-exception-handling" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x06i-Testing-Code-Quality-and-Build-Settings.html - testing-exception-handling" xr:uid="{00000000-0004-0000-0200-000032000000}"/>
-    <hyperlink ref="G43" r:id="rId48" location="testing-biometric-authentication" xr:uid="{EBF9369A-936B-C346-817B-D5DDC634B24B}"/>
-    <hyperlink ref="G42" r:id="rId49" xr:uid="{E55F9D7C-4C71-DA4E-A565-A7F508DC387C}"/>
+    <hyperlink ref="G16" r:id="rId1" location="testing-local-storage-for-sensitive-data" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="G18" r:id="rId2" location="testing-logs-for-sensitive-data" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="G19" r:id="rId3" location="determining-whether-sensitive-data-is-sent-to-third-parties" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="G20" r:id="rId4" location="determining-whether-the-keyboard-cache-is-disabled-for-text-input-fields" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="G21" r:id="rId5" location="determining-whether-sensitive-stored-data-has-been-exposed-via-ipc-mechanisms" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="G23" r:id="rId6" location="testing-backups-for-sensitive-data" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
+    <hyperlink ref="G24" r:id="rId7" location="finding-sensitive-information-in-auto-generated-screenshots" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
+    <hyperlink ref="G25" r:id="rId8" location="checking-memory-for-sensitive-data" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
+    <hyperlink ref="G26" r:id="rId9" location="testing-the-device-access-security-policy" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
+    <hyperlink ref="G29" r:id="rId10" location="testing-key-management" xr:uid="{00000000-0004-0000-0200-00000B000000}"/>
+    <hyperlink ref="G30" r:id="rId11" location="custom-implementations-of-cryptography" xr:uid="{00000000-0004-0000-0200-00000C000000}"/>
+    <hyperlink ref="G41" r:id="rId12" location="running-a-password-dictionary-attack" xr:uid="{00000000-0004-0000-0200-000011000000}"/>
+    <hyperlink ref="G44" r:id="rId13" location="verifying-that-2fa-is-enforced" xr:uid="{00000000-0004-0000-0200-000014000000}"/>
+    <hyperlink ref="G45" r:id="rId14" location="verifying-that-2fa-is-enforced" xr:uid="{00000000-0004-0000-0200-000015000000}"/>
+    <hyperlink ref="G48" r:id="rId15" location="verifying-data-encryption-on-the-network" xr:uid="{00000000-0004-0000-0200-000017000000}"/>
+    <hyperlink ref="G49" r:id="rId16" location="verifying-data-encryption-on-the-network" xr:uid="{00000000-0004-0000-0200-000018000000}"/>
+    <hyperlink ref="G50" r:id="rId17" location="testing-endpoint-identify-verification" xr:uid="{00000000-0004-0000-0200-000019000000}"/>
+    <hyperlink ref="G51" r:id="rId18" location="testing-custom-certificate-stores-and-certificate-pinning" xr:uid="{00000000-0004-0000-0200-00001A000000}"/>
+    <hyperlink ref="G55" r:id="rId19" location="testing-app-permissions" xr:uid="{00000000-0004-0000-0200-00001B000000}"/>
+    <hyperlink ref="G56" r:id="rId20" location="injection-flaws" xr:uid="{00000000-0004-0000-0200-00001C000000}"/>
+    <hyperlink ref="G57" r:id="rId21" location="testing-custom-url-schemes" xr:uid="{00000000-0004-0000-0200-00001D000000}"/>
+    <hyperlink ref="G58" r:id="rId22" location="testing-for-sensitive-functionality-exposure-through-ipc" xr:uid="{00000000-0004-0000-0200-00001E000000}"/>
+    <hyperlink ref="G59" r:id="rId23" location="testing-javascript-execution-in-webviews" xr:uid="{00000000-0004-0000-0200-00001F000000}"/>
+    <hyperlink ref="G60" r:id="rId24" location="testing-webview-protocol-handlers" xr:uid="{00000000-0004-0000-0200-000020000000}"/>
+    <hyperlink ref="G61" r:id="rId25" location="determining-whether-java-objects-are-exposed-through-webviews" xr:uid="{00000000-0004-0000-0200-000021000000}"/>
+    <hyperlink ref="G62" r:id="rId26" location="testing-object-persistence" xr:uid="{00000000-0004-0000-0200-000022000000}"/>
+    <hyperlink ref="G64" r:id="rId27" location="making-sure-that-the-app-is-properly-signed" xr:uid="{00000000-0004-0000-0200-000023000000}"/>
+    <hyperlink ref="G65" r:id="rId28" location="determining-whether-the-app-is-debuggable" xr:uid="{00000000-0004-0000-0200-000024000000}"/>
+    <hyperlink ref="G66" r:id="rId29" location="finding-debugging-symbols" xr:uid="{00000000-0004-0000-0200-000025000000}"/>
+    <hyperlink ref="G70" r:id="rId30" location="testing-exception-handling" xr:uid="{00000000-0004-0000-0200-000027000000}"/>
+    <hyperlink ref="G71" r:id="rId31" location="testing-exception-handling" xr:uid="{00000000-0004-0000-0200-000028000000}"/>
+    <hyperlink ref="G72" r:id="rId32" location="make-sure-that-free-security-features-are-activated" xr:uid="{00000000-0004-0000-0200-000029000000}"/>
+    <hyperlink ref="G36" r:id="rId33" location="testing-authentication" xr:uid="{00000000-0004-0000-0200-00002A000000}"/>
+    <hyperlink ref="G22" r:id="rId34" location="checking-for-sensitive-data-disclosure-through-the-user-interface" xr:uid="{00000000-0004-0000-0200-00002C000000}"/>
+    <hyperlink ref="G40" r:id="rId35" location="best-practices-for-passwords" xr:uid="{00000000-0004-0000-0200-00002D000000}"/>
+    <hyperlink ref="G52" r:id="rId36" location="making-sure-that-critical-operations-use-secure-communication-channels" xr:uid="{00000000-0004-0000-0200-00002E000000}"/>
+    <hyperlink ref="G53" r:id="rId37" location="testing-the-security-provider" xr:uid="{00000000-0004-0000-0200-00002F000000}"/>
+    <hyperlink ref="G39" r:id="rId38" location="user-logout-and-session-timeouts" xr:uid="{00000000-0004-0000-0200-000030000000}"/>
+    <hyperlink ref="G38" r:id="rId39" location="testing-stateless-token-based-authentication" xr:uid="{00000000-0004-0000-0200-000031000000}"/>
+    <hyperlink ref="G69" r:id="rId40" location="testing-exception-handling" xr:uid="{00000000-0004-0000-0200-000032000000}"/>
+    <hyperlink ref="G43" r:id="rId41" location="testing-biometric-authentication" xr:uid="{EBF9369A-936B-C346-817B-D5DDC634B24B}"/>
+    <hyperlink ref="G42" r:id="rId42" location="session-timeout" xr:uid="{E55F9D7C-4C71-DA4E-A565-A7F508DC387C}"/>
+    <hyperlink ref="G17" r:id="rId43" location="testing-local-storage-for-sensitive-data" xr:uid="{BAAA2175-724E-4546-BA03-45D92E6BBE47}"/>
+    <hyperlink ref="G33" r:id="rId44" location="testing-key-management" xr:uid="{E4D159B7-2715-3841-A281-522A1903D4E1}"/>
+    <hyperlink ref="G37" r:id="rId45" location="testing-stateful-session-management" xr:uid="{00000000-0004-0000-0200-00002B000000}"/>
+    <hyperlink ref="G67" r:id="rId46" location="finding-debugging-code-and-verbose-error-logging" xr:uid="{00000000-0004-0000-0200-000026000000}"/>
+    <hyperlink ref="G32" r:id="rId47" location="identifying-insecure-and-or-deprecated-cryptographic-algorithms" xr:uid="{00000000-0004-0000-0200-00000E000000}"/>
+    <hyperlink ref="G31" r:id="rId48" location="verifying-the-configuration-of-cryptographic-standard-algorithms" xr:uid="{00000000-0004-0000-0200-00000D000000}"/>
+    <hyperlink ref="G34" r:id="rId49" location="testing-random-number-generation" xr:uid="{81447B33-421B-0848-B5DE-FB6C35E5366F}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -5740,7 +5724,7 @@
   <dimension ref="B1:G29"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5756,7 +5740,7 @@
   <sheetData>
     <row r="1" spans="2:7" ht="19" x14ac:dyDescent="0.25">
       <c r="B1" s="7" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="C1" s="24"/>
       <c r="D1" s="24"/>
@@ -5773,276 +5757,268 @@
       <c r="G2" s="24"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B3" s="115"/>
-      <c r="C3" s="116" t="s">
+      <c r="B3" s="76"/>
+      <c r="C3" s="77" t="s">
         <v>52</v>
       </c>
-      <c r="D3" s="115" t="s">
+      <c r="D3" s="76" t="s">
         <v>53</v>
       </c>
-      <c r="E3" s="115" t="s">
+      <c r="E3" s="76" t="s">
         <v>164</v>
       </c>
-      <c r="F3" s="115" t="s">
+      <c r="F3" s="76" t="s">
         <v>178</v>
       </c>
-      <c r="G3" s="115" t="s">
+      <c r="G3" s="76" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B4" s="117"/>
-      <c r="C4" s="118" t="s">
+      <c r="B4" s="78"/>
+      <c r="C4" s="79" t="s">
         <v>55</v>
       </c>
-      <c r="D4" s="118"/>
-      <c r="E4" s="118"/>
-      <c r="F4" s="118"/>
-      <c r="G4" s="118"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="79"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="79"/>
     </row>
     <row r="5" spans="2:7" ht="30" x14ac:dyDescent="0.2">
-      <c r="B5" s="119">
+      <c r="B5" s="80">
         <v>8.1</v>
       </c>
-      <c r="C5" s="120" t="s">
+      <c r="C5" s="81" t="s">
         <v>57</v>
       </c>
-      <c r="D5" s="121" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="122" t="s">
+      <c r="D5" s="82" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="83" t="s">
         <v>136</v>
       </c>
-      <c r="F5" s="123" t="s">
+      <c r="F5" s="84" t="s">
+        <v>292</v>
+      </c>
+      <c r="G5" s="81"/>
+    </row>
+    <row r="6" spans="2:7" ht="45" x14ac:dyDescent="0.2">
+      <c r="B6" s="80">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="C6" s="81" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="82" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="83" t="s">
+        <v>136</v>
+      </c>
+      <c r="F6" s="84" t="s">
+        <v>233</v>
+      </c>
+      <c r="G6" s="81"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B7" s="80">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="C7" s="81" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="82" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="83" t="s">
+        <v>136</v>
+      </c>
+      <c r="F7" s="84" t="s">
         <v>234</v>
       </c>
-      <c r="G5" s="120"/>
-    </row>
-    <row r="6" spans="2:7" ht="45" x14ac:dyDescent="0.2">
-      <c r="B6" s="119">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="C6" s="120" t="s">
-        <v>58</v>
-      </c>
-      <c r="D6" s="121" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="122" t="s">
+      <c r="G7" s="81"/>
+    </row>
+    <row r="8" spans="2:7" ht="30" x14ac:dyDescent="0.2">
+      <c r="B8" s="80">
+        <v>8.4</v>
+      </c>
+      <c r="C8" s="81" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="82" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="83" t="s">
         <v>136</v>
       </c>
-      <c r="F6" s="123" t="s">
+      <c r="F8" s="84" t="s">
         <v>235</v>
       </c>
-      <c r="G6" s="120"/>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B7" s="119">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="C7" s="120" t="s">
-        <v>59</v>
-      </c>
-      <c r="D7" s="121" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="122" t="s">
+      <c r="G8" s="81"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B9" s="80">
+        <v>8.5</v>
+      </c>
+      <c r="C9" s="81" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="82" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="83" t="s">
         <v>136</v>
       </c>
-      <c r="F7" s="123" t="s">
+      <c r="F9" s="84" t="s">
         <v>236</v>
       </c>
-      <c r="G7" s="120"/>
-    </row>
-    <row r="8" spans="2:7" ht="30" x14ac:dyDescent="0.2">
-      <c r="B8" s="119">
-        <v>8.4</v>
-      </c>
-      <c r="C8" s="120" t="s">
-        <v>60</v>
-      </c>
-      <c r="D8" s="121" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="122" t="s">
+      <c r="G9" s="81"/>
+    </row>
+    <row r="10" spans="2:7" ht="30" x14ac:dyDescent="0.2">
+      <c r="B10" s="80">
+        <v>8.6</v>
+      </c>
+      <c r="C10" s="81" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="82" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="83" t="s">
         <v>136</v>
       </c>
-      <c r="F8" s="123" t="s">
+      <c r="F10" s="84" t="s">
+        <v>293</v>
+      </c>
+      <c r="G10" s="81"/>
+    </row>
+    <row r="11" spans="2:7" ht="30" x14ac:dyDescent="0.2">
+      <c r="B11" s="80">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="C11" s="81" t="s">
+        <v>266</v>
+      </c>
+      <c r="D11" s="82" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="83" t="s">
+        <v>136</v>
+      </c>
+      <c r="F11" s="84"/>
+      <c r="G11" s="81"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B12" s="80">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="C12" s="81" t="s">
+        <v>267</v>
+      </c>
+      <c r="D12" s="82" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="83" t="s">
+        <v>136</v>
+      </c>
+      <c r="F12" s="84"/>
+      <c r="G12" s="81"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B13" s="80">
+        <v>8.9</v>
+      </c>
+      <c r="C13" s="81" t="s">
+        <v>282</v>
+      </c>
+      <c r="D13" s="82" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="83" t="s">
+        <v>136</v>
+      </c>
+      <c r="F13" s="84" t="s">
         <v>237</v>
       </c>
-      <c r="G8" s="120"/>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B9" s="119">
-        <v>8.5</v>
-      </c>
-      <c r="C9" s="120" t="s">
-        <v>61</v>
-      </c>
-      <c r="D9" s="121" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="122" t="s">
+      <c r="G13" s="81"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B14" s="78"/>
+      <c r="C14" s="79" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="79"/>
+      <c r="E14" s="79"/>
+      <c r="F14" s="79"/>
+      <c r="G14" s="79"/>
+    </row>
+    <row r="15" spans="2:7" ht="30" x14ac:dyDescent="0.2">
+      <c r="B15" s="85" t="s">
+        <v>128</v>
+      </c>
+      <c r="C15" s="81" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" s="82" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="83" t="s">
         <v>136</v>
       </c>
-      <c r="F9" s="123" t="s">
+      <c r="F15" s="84" t="s">
         <v>238</v>
       </c>
-      <c r="G9" s="120"/>
-    </row>
-    <row r="10" spans="2:7" ht="30" x14ac:dyDescent="0.2">
-      <c r="B10" s="119">
-        <v>8.6</v>
-      </c>
-      <c r="C10" s="120" t="s">
-        <v>62</v>
-      </c>
-      <c r="D10" s="121" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="122" t="s">
+      <c r="G15" s="81"/>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B16" s="78"/>
+      <c r="C16" s="79" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="79"/>
+      <c r="E16" s="79"/>
+      <c r="F16" s="79"/>
+      <c r="G16" s="79"/>
+    </row>
+    <row r="17" spans="2:7" ht="45" x14ac:dyDescent="0.2">
+      <c r="B17" s="80">
+        <v>8.11</v>
+      </c>
+      <c r="C17" s="81" t="s">
+        <v>268</v>
+      </c>
+      <c r="D17" s="82" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="83" t="s">
         <v>136</v>
       </c>
-      <c r="F10" s="123" t="s">
-        <v>239</v>
-      </c>
-      <c r="G10" s="120"/>
-    </row>
-    <row r="11" spans="2:7" ht="30" x14ac:dyDescent="0.2">
-      <c r="B11" s="119">
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="C11" s="120" t="s">
-        <v>272</v>
-      </c>
-      <c r="D11" s="121" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="122" t="s">
+      <c r="F17" s="84"/>
+      <c r="G17" s="81"/>
+    </row>
+    <row r="18" spans="2:7" ht="60" x14ac:dyDescent="0.2">
+      <c r="B18" s="80">
+        <v>8.1199999999999992</v>
+      </c>
+      <c r="C18" s="81" t="s">
+        <v>269</v>
+      </c>
+      <c r="D18" s="82" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="83" t="s">
         <v>136</v>
       </c>
-      <c r="F11" s="123" t="s">
-        <v>240</v>
-      </c>
-      <c r="G11" s="120"/>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B12" s="119">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="C12" s="120" t="s">
-        <v>273</v>
-      </c>
-      <c r="D12" s="121" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="122" t="s">
-        <v>136</v>
-      </c>
-      <c r="F12" s="123" t="s">
-        <v>274</v>
-      </c>
-      <c r="G12" s="120"/>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B13" s="119">
-        <v>8.9</v>
-      </c>
-      <c r="C13" s="120" t="s">
-        <v>291</v>
-      </c>
-      <c r="D13" s="121" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="122" t="s">
-        <v>136</v>
-      </c>
-      <c r="F13" s="123" t="s">
-        <v>241</v>
-      </c>
-      <c r="G13" s="120"/>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B14" s="117"/>
-      <c r="C14" s="118" t="s">
-        <v>54</v>
-      </c>
-      <c r="D14" s="118"/>
-      <c r="E14" s="118"/>
-      <c r="F14" s="118"/>
-      <c r="G14" s="118"/>
-    </row>
-    <row r="15" spans="2:7" ht="30" x14ac:dyDescent="0.2">
-      <c r="B15" s="124" t="s">
-        <v>128</v>
-      </c>
-      <c r="C15" s="120" t="s">
-        <v>64</v>
-      </c>
-      <c r="D15" s="121" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="122" t="s">
-        <v>136</v>
-      </c>
-      <c r="F15" s="123" t="s">
-        <v>242</v>
-      </c>
-      <c r="G15" s="120"/>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B16" s="117"/>
-      <c r="C16" s="118" t="s">
-        <v>56</v>
-      </c>
-      <c r="D16" s="118"/>
-      <c r="E16" s="118"/>
-      <c r="F16" s="118"/>
-      <c r="G16" s="118"/>
-    </row>
-    <row r="17" spans="2:7" ht="45" x14ac:dyDescent="0.2">
-      <c r="B17" s="119">
-        <v>8.11</v>
-      </c>
-      <c r="C17" s="120" t="s">
-        <v>275</v>
-      </c>
-      <c r="D17" s="121" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" s="122" t="s">
-        <v>136</v>
-      </c>
-      <c r="F17" s="123" t="s">
-        <v>243</v>
-      </c>
-      <c r="G17" s="120"/>
-    </row>
-    <row r="18" spans="2:7" ht="60" x14ac:dyDescent="0.2">
-      <c r="B18" s="119">
-        <v>8.1199999999999992</v>
-      </c>
-      <c r="C18" s="120" t="s">
-        <v>276</v>
-      </c>
-      <c r="D18" s="121" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18" s="122" t="s">
-        <v>136</v>
-      </c>
-      <c r="F18" s="123" t="s">
-        <v>244</v>
-      </c>
-      <c r="G18" s="120"/>
+      <c r="F18" s="84"/>
+      <c r="G18" s="81"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B19" s="115"/>
-      <c r="C19" s="116"/>
-      <c r="D19" s="115"/>
-      <c r="E19" s="115"/>
-      <c r="F19" s="115"/>
-      <c r="G19" s="115"/>
+      <c r="B19" s="76"/>
+      <c r="C19" s="77"/>
+      <c r="D19" s="76"/>
+      <c r="E19" s="76"/>
+      <c r="F19" s="76"/>
+      <c r="G19" s="76"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B20" s="45"/>
@@ -6149,18 +6125,14 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="F5" r:id="rId1" location="testing-advanced-root-detection" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x05j-Testing-Resiliency-Against-Reverse-Engineering.html - testing-advanced-root-detection" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink ref="F6" r:id="rId2" location="testing-debugging-defenses" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x05j-Testing-Resiliency-Against-Reverse-Engineering.html - testing-debugging-defenses" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
-    <hyperlink ref="F7" r:id="rId3" location="testing-file-integrity-checks" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x05j-Testing-Resiliency-Against-Reverse-Engineering.html - testing-file-integrity-checks" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
-    <hyperlink ref="F8" r:id="rId4" location="testing-detection-of-reverse-engineering-tools" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x05j-Testing-Resiliency-Against-Reverse-Engineering.html - testing-detection-of-reverse-engineering-tools" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
-    <hyperlink ref="F9" r:id="rId5" location="testing-simple-emulator-detection" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x05j-Testing-Resiliency-Against-Reverse-Engineering.html - testing-simple-emulator-detection" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
-    <hyperlink ref="F10" r:id="rId6" location="testing-memory-integrity-checks" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x05j-Testing-Resiliency-Against-Reverse-Engineering.html - testing-memory-integrity-checks" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
-    <hyperlink ref="F11" r:id="rId7" location="verifying-the-variablility-of-tampering-responses" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x05j-Testing-Resiliency-Against-Reverse-Engineering.html - verifying-the-variablility-of-tampering-responses" xr:uid="{00000000-0004-0000-0300-000006000000}"/>
-    <hyperlink ref="F15" r:id="rId8" location="testing-device-binding" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x05j-Testing-Resiliency-Against-Reverse-Engineering.html - testing-device-binding" xr:uid="{00000000-0004-0000-0300-000007000000}"/>
-    <hyperlink ref="F17" r:id="rId9" location="testing-advanced-anti-emulation" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x05j-Testing-Resiliency-Against-Reverse-Engineering.html - testing-advanced-anti-emulation" xr:uid="{00000000-0004-0000-0300-000008000000}"/>
-    <hyperlink ref="F18" r:id="rId10" location="testing-advanced-anti-emulation" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x05j-Testing-Resiliency-Against-Reverse-Engineering.html - testing-advanced-anti-emulation" xr:uid="{00000000-0004-0000-0300-000009000000}"/>
-    <hyperlink ref="F12" r:id="rId11" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x05j-Testing-Resiliency-Against-Reverse-Engineering.html" xr:uid="{00000000-0004-0000-0300-00000A000000}"/>
-    <hyperlink ref="F13" r:id="rId12" location="testing-simple-obfuscation" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x06j-Testing-Resiliency-Against-Reverse-Engineering.html - testing-simple-obfuscation" xr:uid="{00000000-0004-0000-0300-00000B000000}"/>
+    <hyperlink ref="F5" r:id="rId1" location="testing-root-detection" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="F6" r:id="rId2" location="testing-anti-debugging" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="F7" r:id="rId3" location="testing-file-integrity-checks" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="F8" r:id="rId4" location="testing-the-detection-of-reverse-engineering-tools" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink ref="F9" r:id="rId5" location="testing-emulator-detection" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
+    <hyperlink ref="F10" r:id="rId6" location="testing-run-time-integrity-checks" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
+    <hyperlink ref="F15" r:id="rId7" location="testing-device-binding" xr:uid="{00000000-0004-0000-0300-000007000000}"/>
+    <hyperlink ref="F13" r:id="rId8" location="testing-obfuscation" xr:uid="{00000000-0004-0000-0300-00000B000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -6173,7 +6145,7 @@
   <dimension ref="B1:J85"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6190,7 +6162,7 @@
   <sheetData>
     <row r="1" spans="2:8" ht="19" x14ac:dyDescent="0.25">
       <c r="B1" s="57" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="C1" s="50"/>
       <c r="D1" s="50"/>
@@ -6401,7 +6373,7 @@
         <v>1.9</v>
       </c>
       <c r="C13" s="36" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="D13" s="36"/>
       <c r="E13" s="51" t="s">
@@ -6420,7 +6392,7 @@
         <v>9</v>
       </c>
       <c r="C14" s="36" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="D14" s="36"/>
       <c r="E14" s="51" t="s">
@@ -6452,7 +6424,7 @@
         <v>11</v>
       </c>
       <c r="C16" s="56" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="D16" s="26" t="s">
         <v>7</v>
@@ -6471,12 +6443,14 @@
         <v>65</v>
       </c>
       <c r="C17" s="56" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="D17" s="26"/>
       <c r="E17" s="51"/>
       <c r="F17" s="37"/>
-      <c r="G17" s="58"/>
+      <c r="G17" s="58" t="s">
+        <v>186</v>
+      </c>
       <c r="H17" s="74"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.2">
@@ -6560,7 +6534,7 @@
         <v>14</v>
       </c>
       <c r="C22" s="56" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="D22" s="26" t="s">
         <v>7</v>
@@ -6572,7 +6546,7 @@
         <v>136</v>
       </c>
       <c r="G22" s="58" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="H22" s="74"/>
     </row>
@@ -6581,7 +6555,7 @@
         <v>15</v>
       </c>
       <c r="C23" s="56" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="D23" s="56"/>
       <c r="E23" s="51" t="s">
@@ -6645,9 +6619,7 @@
         <v>7</v>
       </c>
       <c r="F26" s="37"/>
-      <c r="G26" s="58" t="s">
-        <v>195</v>
-      </c>
+      <c r="G26" s="58"/>
       <c r="H26" s="74"/>
     </row>
     <row r="27" spans="2:8" ht="30" x14ac:dyDescent="0.2">
@@ -6664,9 +6636,7 @@
       <c r="F27" s="37" t="s">
         <v>136</v>
       </c>
-      <c r="G27" s="58" t="s">
-        <v>196</v>
-      </c>
+      <c r="G27" s="58"/>
       <c r="H27" s="74"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.2">
@@ -6697,7 +6667,7 @@
       </c>
       <c r="F29" s="37"/>
       <c r="G29" s="58" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H29" s="74"/>
     </row>
@@ -6716,7 +6686,7 @@
       </c>
       <c r="F30" s="37"/>
       <c r="G30" s="58" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H30" s="74"/>
     </row>
@@ -6735,7 +6705,7 @@
       </c>
       <c r="F31" s="37"/>
       <c r="G31" s="58" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H31" s="74"/>
     </row>
@@ -6754,7 +6724,7 @@
       </c>
       <c r="F32" s="37"/>
       <c r="G32" s="58" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H32" s="74"/>
     </row>
@@ -6773,7 +6743,7 @@
       </c>
       <c r="F33" s="37"/>
       <c r="G33" s="58" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="H33" s="74"/>
     </row>
@@ -6792,7 +6762,7 @@
       </c>
       <c r="F34" s="37"/>
       <c r="G34" s="58" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="H34" s="74"/>
     </row>
@@ -6824,7 +6794,7 @@
       </c>
       <c r="F36" s="37"/>
       <c r="G36" s="58" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H36" s="74"/>
     </row>
@@ -6833,7 +6803,7 @@
         <v>84</v>
       </c>
       <c r="C37" s="56" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D37" s="26" t="s">
         <v>7</v>
@@ -6843,7 +6813,7 @@
       </c>
       <c r="F37" s="37"/>
       <c r="G37" s="58" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H37" s="74"/>
     </row>
@@ -6852,7 +6822,7 @@
         <v>85</v>
       </c>
       <c r="C38" s="56" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="D38" s="26" t="s">
         <v>7</v>
@@ -6862,7 +6832,7 @@
       </c>
       <c r="F38" s="37"/>
       <c r="G38" s="58" t="s">
-        <v>205</v>
+        <v>291</v>
       </c>
       <c r="H38" s="74"/>
     </row>
@@ -6871,13 +6841,13 @@
         <v>27</v>
       </c>
       <c r="C39" s="56" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="D39" s="26"/>
       <c r="E39" s="51"/>
       <c r="F39" s="37"/>
       <c r="G39" s="58" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H39" s="74"/>
       <c r="J39" s="58"/>
@@ -6897,7 +6867,7 @@
       </c>
       <c r="F40" s="37"/>
       <c r="G40" s="58" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H40" s="74"/>
       <c r="J40" s="58"/>
@@ -6907,7 +6877,7 @@
         <v>86</v>
       </c>
       <c r="C41" s="56" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="D41" s="26" t="s">
         <v>7</v>
@@ -6917,7 +6887,7 @@
       </c>
       <c r="F41" s="37"/>
       <c r="G41" s="58" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H41" s="74"/>
     </row>
@@ -6926,7 +6896,7 @@
         <v>87</v>
       </c>
       <c r="C42" s="56" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="D42" s="26" t="s">
         <v>7</v>
@@ -6936,7 +6906,7 @@
       </c>
       <c r="F42" s="37"/>
       <c r="G42" s="58" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H42" s="58"/>
     </row>
@@ -6954,8 +6924,8 @@
       <c r="F43" s="37" t="s">
         <v>136</v>
       </c>
-      <c r="G43" s="58" t="s">
-        <v>207</v>
+      <c r="G43" s="125" t="s">
+        <v>206</v>
       </c>
       <c r="H43" s="74"/>
     </row>
@@ -6974,7 +6944,7 @@
         <v>136</v>
       </c>
       <c r="G44" s="58" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H44" s="74"/>
     </row>
@@ -6993,13 +6963,13 @@
         <v>136</v>
       </c>
       <c r="G45" s="58" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H45" s="74"/>
     </row>
     <row r="46" spans="2:10" ht="30" x14ac:dyDescent="0.2">
       <c r="B46" s="55" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="C46" s="56" t="s">
         <v>93</v>
@@ -7011,9 +6981,7 @@
       <c r="F46" s="37" t="s">
         <v>136</v>
       </c>
-      <c r="G46" s="58" t="s">
-        <v>211</v>
-      </c>
+      <c r="G46" s="58"/>
       <c r="H46" s="74"/>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.2">
@@ -7044,7 +7012,7 @@
       </c>
       <c r="F48" s="37"/>
       <c r="G48" s="58" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="H48" s="74"/>
     </row>
@@ -7063,7 +7031,7 @@
       </c>
       <c r="F49" s="37"/>
       <c r="G49" s="58" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H49" s="74"/>
     </row>
@@ -7082,7 +7050,7 @@
       </c>
       <c r="F50" s="37"/>
       <c r="G50" s="58" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="H50" s="74"/>
     </row>
@@ -7101,7 +7069,7 @@
         <v>136</v>
       </c>
       <c r="G51" s="58" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="H51" s="74"/>
     </row>
@@ -7120,7 +7088,7 @@
         <v>136</v>
       </c>
       <c r="G52" s="58" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="H52" s="74"/>
     </row>
@@ -7129,7 +7097,7 @@
         <v>5.6</v>
       </c>
       <c r="C53" s="56" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="D53" s="56"/>
       <c r="E53" s="51" t="s">
@@ -7138,9 +7106,7 @@
       <c r="F53" s="37" t="s">
         <v>136</v>
       </c>
-      <c r="G53" s="58" t="s">
-        <v>267</v>
-      </c>
+      <c r="G53" s="58"/>
       <c r="H53" s="74"/>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.2">
@@ -7148,7 +7114,7 @@
         <v>36</v>
       </c>
       <c r="C54" s="39" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D54" s="39"/>
       <c r="E54" s="54"/>
@@ -7170,9 +7136,7 @@
         <v>7</v>
       </c>
       <c r="F55" s="37"/>
-      <c r="G55" s="58" t="s">
-        <v>217</v>
-      </c>
+      <c r="G55" s="58"/>
       <c r="H55" s="74"/>
     </row>
     <row r="56" spans="2:8" ht="30" x14ac:dyDescent="0.2">
@@ -7190,7 +7154,7 @@
       </c>
       <c r="F56" s="37"/>
       <c r="G56" s="58" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="H56" s="74"/>
     </row>
@@ -7209,7 +7173,7 @@
       </c>
       <c r="F57" s="37"/>
       <c r="G57" s="58" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="H57" s="74"/>
     </row>
@@ -7227,9 +7191,7 @@
         <v>7</v>
       </c>
       <c r="F58" s="37"/>
-      <c r="G58" s="58" t="s">
-        <v>220</v>
-      </c>
+      <c r="G58" s="58"/>
       <c r="H58" s="74"/>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.2">
@@ -7247,7 +7209,7 @@
       </c>
       <c r="F59" s="37"/>
       <c r="G59" s="58" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="H59" s="74"/>
     </row>
@@ -7265,9 +7227,7 @@
         <v>7</v>
       </c>
       <c r="F60" s="37"/>
-      <c r="G60" s="58" t="s">
-        <v>222</v>
-      </c>
+      <c r="G60" s="58"/>
       <c r="H60" s="74"/>
     </row>
     <row r="61" spans="2:8" ht="30" x14ac:dyDescent="0.2">
@@ -7275,7 +7235,7 @@
         <v>6.7</v>
       </c>
       <c r="C61" s="56" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="D61" s="26" t="s">
         <v>7</v>
@@ -7284,9 +7244,7 @@
         <v>7</v>
       </c>
       <c r="F61" s="37"/>
-      <c r="G61" s="58" t="s">
-        <v>223</v>
-      </c>
+      <c r="G61" s="58"/>
       <c r="H61" s="74"/>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.2">
@@ -7303,9 +7261,7 @@
         <v>7</v>
       </c>
       <c r="F62" s="37"/>
-      <c r="G62" s="58" t="s">
-        <v>224</v>
-      </c>
+      <c r="G62" s="58"/>
       <c r="H62" s="74"/>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.2">
@@ -7336,7 +7292,7 @@
       </c>
       <c r="F64" s="37"/>
       <c r="G64" s="58" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="H64" s="74"/>
     </row>
@@ -7354,9 +7310,7 @@
         <v>7</v>
       </c>
       <c r="F65" s="37"/>
-      <c r="G65" s="58" t="s">
-        <v>226</v>
-      </c>
+      <c r="G65" s="58"/>
       <c r="H65" s="74"/>
     </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.2">
@@ -7374,7 +7328,7 @@
       </c>
       <c r="F66" s="37"/>
       <c r="G66" s="58" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="H66" s="74"/>
     </row>
@@ -7393,7 +7347,7 @@
       </c>
       <c r="F67" s="37"/>
       <c r="G67" s="58" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H67" s="74"/>
     </row>
@@ -7402,7 +7356,7 @@
         <v>117</v>
       </c>
       <c r="C68" s="56" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="D68" s="26" t="s">
         <v>7</v>
@@ -7411,9 +7365,7 @@
         <v>7</v>
       </c>
       <c r="F68" s="37"/>
-      <c r="G68" s="58" t="s">
-        <v>281</v>
-      </c>
+      <c r="G68" s="58"/>
       <c r="H68" s="74"/>
     </row>
     <row r="69" spans="2:8" x14ac:dyDescent="0.2">
@@ -7431,7 +7383,7 @@
       </c>
       <c r="F69" s="37"/>
       <c r="G69" s="58" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="H69" s="74"/>
     </row>
@@ -7450,7 +7402,7 @@
       </c>
       <c r="F70" s="37"/>
       <c r="G70" s="58" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="H70" s="74"/>
     </row>
@@ -7468,17 +7420,15 @@
         <v>7</v>
       </c>
       <c r="F71" s="37"/>
-      <c r="G71" s="58" t="s">
-        <v>232</v>
-      </c>
+      <c r="G71" s="58"/>
       <c r="H71" s="74"/>
     </row>
     <row r="72" spans="2:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B72" s="55" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="C72" s="56" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="D72" s="26" t="s">
         <v>7</v>
@@ -7488,7 +7438,7 @@
       </c>
       <c r="F72" s="37"/>
       <c r="G72" s="58" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H72" s="74"/>
     </row>
@@ -7637,56 +7587,46 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="G16" r:id="rId1" location="testing-for-sensitive-data-disclosure-in-local-storage" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x06d-Testing-Data-Storage.html - testing-for-sensitive-data-disclosure-in-local-storage" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
-    <hyperlink ref="G29" r:id="rId2" location="verifying-cryptographic-key-management" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x06e-Testing-Cryptography.html - verifying-cryptographic-key-management" xr:uid="{00000000-0004-0000-0400-000008000000}"/>
-    <hyperlink ref="G30" r:id="rId3" location="testing-for-custom-implementations-of-cryptography" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x06e-Testing-Cryptography.html - testing-for-custom-implementations-of-cryptography" xr:uid="{00000000-0004-0000-0400-000009000000}"/>
-    <hyperlink ref="G31" r:id="rId4" location="verifying-the-configuration-of-cryptographic-standard-algorithms" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x06e-Testing-Cryptography.html - verifying-the-configuration-of-cryptographic-standard-algorithms" xr:uid="{00000000-0004-0000-0400-00000A000000}"/>
-    <hyperlink ref="G32" r:id="rId5" location="testing-for-insecure-andor-deprecated-cryptographic-primitives" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x06e-Testing-Cryptography.html - testing-for-insecure-andor-deprecated-cryptographic-primitives" xr:uid="{00000000-0004-0000-0400-00000B000000}"/>
-    <hyperlink ref="G33" r:id="rId6" location="testing-random-number-generation" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x06e-Testing-Cryptography.html - testing-random-number-generation" xr:uid="{00000000-0004-0000-0400-00000C000000}"/>
-    <hyperlink ref="G34" r:id="rId7" location="verifying-cryptographic-key-management" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x06e-Testing-Cryptography.html - verifying-cryptographic-key-management" xr:uid="{00000000-0004-0000-0400-00000D000000}"/>
-    <hyperlink ref="G36" r:id="rId8" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x04e-Testing-Authentication-and-Session-Management.html" xr:uid="{00000000-0004-0000-0400-00000E000000}"/>
-    <hyperlink ref="G37" r:id="rId9" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x04e-Testing-Authentication-and-Session-Management.html" xr:uid="{00000000-0004-0000-0400-00000F000000}"/>
-    <hyperlink ref="G41" r:id="rId10" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x04e-Testing-Authentication-and-Session-Management.html" xr:uid="{00000000-0004-0000-0400-000010000000}"/>
-    <hyperlink ref="G44" r:id="rId11" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x04e-Testing-Authentication-and-Session-Management.html" xr:uid="{00000000-0004-0000-0400-000013000000}"/>
-    <hyperlink ref="G45" r:id="rId12" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x04e-Testing-Authentication-and-Session-Management.html" xr:uid="{00000000-0004-0000-0400-000014000000}"/>
-    <hyperlink ref="G48" r:id="rId13" location="testing-for-unencrypted-sensitive-data-on-the-network" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x06g-Testing-Network-Communication.html - testing-for-unencrypted-sensitive-data-on-the-network" xr:uid="{00000000-0004-0000-0400-000016000000}"/>
-    <hyperlink ref="G49" r:id="rId14" location="verifying-the-tls-settings" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x06g-Testing-Network-Communication.html - verifying-the-tls-settings" xr:uid="{00000000-0004-0000-0400-000017000000}"/>
-    <hyperlink ref="G50" r:id="rId15" location="testing-endpoint-identity-verification" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x06g-Testing-Network-Communication.html - testing-endpoint-identity-verification" xr:uid="{00000000-0004-0000-0400-000018000000}"/>
-    <hyperlink ref="G55" r:id="rId16" location="testing-app-permissions" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x06h-Testing-Platform-Interaction.html - testing-app-permissions" xr:uid="{00000000-0004-0000-0400-000019000000}"/>
-    <hyperlink ref="G56" r:id="rId17" location="testing-input-validation-and-sanitization" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x06h-Testing-Platform-Interaction.html - testing-input-validation-and-sanitization" xr:uid="{00000000-0004-0000-0400-00001A000000}"/>
-    <hyperlink ref="G57" r:id="rId18" location="testing-custom-url-schemes" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x06h-Testing-Platform-Interaction.html - testing-custom-url-schemes" xr:uid="{00000000-0004-0000-0400-00001B000000}"/>
-    <hyperlink ref="G58" r:id="rId19" location="testing-for-sensitive-functionality-exposed-through-ipc" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x06h-Testing-Platform-Interaction.html - testing-for-sensitive-functionality-exposed-through-ipc" xr:uid="{00000000-0004-0000-0400-00001C000000}"/>
-    <hyperlink ref="G59" r:id="rId20" location="testing-javascript-execution-in-webviews" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x06h-Testing-Platform-Interaction.html - testing-javascript-execution-in-webviews" xr:uid="{00000000-0004-0000-0400-00001D000000}"/>
-    <hyperlink ref="G60" r:id="rId21" location="testing-webview-protocol-handlers" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x06h-Testing-Platform-Interaction.html - testing-webview-protocol-handlers" xr:uid="{00000000-0004-0000-0400-00001E000000}"/>
-    <hyperlink ref="G61" r:id="rId22" location="testing-whether-java-objects-are-exposed-through-webviews" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x06h-Testing-Platform-Interaction.html - testing-whether-java-objects-are-exposed-through-webviews" xr:uid="{00000000-0004-0000-0400-00001F000000}"/>
-    <hyperlink ref="G62" r:id="rId23" location="testing-object-serialization" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x06h-Testing-Platform-Interaction.html - testing-object-serialization" xr:uid="{00000000-0004-0000-0400-000020000000}"/>
-    <hyperlink ref="G64" r:id="rId24" location="verifying-that-the-app-is-properly-signed" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x06i-Testing-Code-Quality-and-Build-Settings.html - verifying-that-the-app-is-properly-signed" xr:uid="{00000000-0004-0000-0400-000021000000}"/>
-    <hyperlink ref="G65" r:id="rId25" location="testing-whether-the-app-is-debuggable" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x06i-Testing-Code-Quality-and-Build-Settings.html - testing-whether-the-app-is-debuggable" xr:uid="{00000000-0004-0000-0400-000022000000}"/>
-    <hyperlink ref="G66" r:id="rId26" location="verifying-that-debugging-symbols-have-been-removed" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x06i-Testing-Code-Quality-and-Build-Settings.html - verifying-that-debugging-symbols-have-been-removed" xr:uid="{00000000-0004-0000-0400-000023000000}"/>
-    <hyperlink ref="G67" r:id="rId27" location="testing-for-debugging-code-and-verbose-error-logging" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x06i-Testing-Code-Quality-and-Build-Settings.html - testing-for-debugging-code-and-verbose-error-logging" xr:uid="{00000000-0004-0000-0400-000024000000}"/>
-    <hyperlink ref="G70" r:id="rId28" location="verifying-that-the-app-fails-securely" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x06i-Testing-Code-Quality-and-Build-Settings.html - verifying-that-the-app-fails-securely" xr:uid="{00000000-0004-0000-0400-000025000000}"/>
-    <hyperlink ref="G72" r:id="rId29" location="testing-compiler-settings" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x06i-Testing-Code-Quality-and-Build-Settings.html - testing-compiler-settings" xr:uid="{00000000-0004-0000-0400-000026000000}"/>
-    <hyperlink ref="G27" r:id="rId30" location="verifying-user-education-controls" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x06d-Testing-Data-Storage.html - verifying-user-education-controls" xr:uid="{00000000-0004-0000-0400-00002A000000}"/>
-    <hyperlink ref="G71" r:id="rId31" location="testing-for-memory-management-bugs" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x06i-Testing-Code-Quality-and-Build-Settings.html - testing-for-memory-management-bugs" xr:uid="{00000000-0004-0000-0400-00002B000000}"/>
-    <hyperlink ref="G38" r:id="rId32" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x04e-Testing-Authentication-and-Session-Management.html" xr:uid="{00000000-0004-0000-0400-00002C000000}"/>
-    <hyperlink ref="G40" r:id="rId33" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x04e-Testing-Authentication-and-Session-Management.html" xr:uid="{00000000-0004-0000-0400-00002D000000}"/>
-    <hyperlink ref="G39" r:id="rId34" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x04e-Testing-Authentication-and-Session-Management.html" xr:uid="{00000000-0004-0000-0400-00002E000000}"/>
-    <hyperlink ref="G51" r:id="rId35" location="verifying-that-critical-operations-use-secure-communication-channels" display="Verifying that Critical Operations Use Secure Communication Channels" xr:uid="{00000000-0004-0000-0400-00002F000000}"/>
-    <hyperlink ref="G52" r:id="rId36" location="testing-app-permissions" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x06h-Testing-Platform-Interaction.html - testing-app-permissions" xr:uid="{00000000-0004-0000-0400-000030000000}"/>
-    <hyperlink ref="G53" r:id="rId37" location="testing-app-permissions" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x06h-Testing-Platform-Interaction.html - testing-app-permissions" xr:uid="{00000000-0004-0000-0400-000031000000}"/>
-    <hyperlink ref="G69" r:id="rId38" location="testing-exception-handling" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x06i-Testing-Code-Quality-and-Build-Settings.html - testing-exception-handling" xr:uid="{00000000-0004-0000-0400-000032000000}"/>
-    <hyperlink ref="G46" r:id="rId39" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x04e-Testing-Authentication-and-Session-Management.html" xr:uid="{00000000-0004-0000-0400-000015000000}"/>
-    <hyperlink ref="G18" r:id="rId40" location="testing-for-sensitive-data-in-logs" xr:uid="{46731861-EBBD-3340-B6B4-166DCFAD95AE}"/>
-    <hyperlink ref="G19" r:id="rId41" location="verifying-cryptographic-key-management" display="Verifying Key Management" xr:uid="{AE7B6F9B-7236-FD4A-8CDD-4D8C964B4EED}"/>
-    <hyperlink ref="G20" r:id="rId42" location="testing-for-custom-implementations-of-cryptography" display="Testing for Custom Implementations of Cryptography" xr:uid="{9AE35269-EFC8-E643-9FCD-79431130C877}"/>
-    <hyperlink ref="G21" r:id="rId43" location="verifying-the-configuration-of-cryptographic-standard-algorithms" display="Verifying the Configuration of Cryptographic Standard Algorithms" xr:uid="{F3ED19E9-DBDC-8E4E-A5B6-FA8D0E47AE00}"/>
-    <hyperlink ref="G22" r:id="rId44" location="testing-for-insecure-andor-deprecated-cryptographic-primitives" display="Testing for Insecure and/or Deprecated Cryptographic Algorithms" xr:uid="{4A839362-4FC0-0546-AD7C-1E9C63A9CA53}"/>
-    <hyperlink ref="G23" r:id="rId45" location="testing-random-number-generation" display="Testing Random Number Generation" xr:uid="{6035E15B-33A5-9E4F-B19C-87D4A1286459}"/>
-    <hyperlink ref="G24" r:id="rId46" location="verifying-that-critical-operations-use-secure-communication-channels" display="Verifying that Critical Operations Use Secure Communication Channels" xr:uid="{3E9B0B2B-9503-CA4B-AEDB-CCB996D6DEBF}"/>
-    <hyperlink ref="G25" r:id="rId47" location="testing-app-permissions" display="Verifying that Critical Operations Use Secure Communication Channels" xr:uid="{FBEB4D5D-9B5F-5E4E-B240-556982D6D6B5}"/>
-    <hyperlink ref="G26" r:id="rId48" location="testing-app-permissions" display="Verifying the Security Provider" xr:uid="{79715E5B-396A-9C49-9A89-6B54D194E598}"/>
-    <hyperlink ref="G43" r:id="rId49" xr:uid="{280EFCC5-10BC-A045-92DF-D92EE814FB92}"/>
-    <hyperlink ref="G42" r:id="rId50" xr:uid="{D92AB868-720F-964D-B105-FE65BD0DD871}"/>
+    <hyperlink ref="G16" r:id="rId1" location="testing-local-data-storage" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="G57" r:id="rId2" location="testing-custom-url-schemes" xr:uid="{00000000-0004-0000-0400-00001B000000}"/>
+    <hyperlink ref="G59" r:id="rId3" location="testing-ios-webviews" xr:uid="{00000000-0004-0000-0400-00001D000000}"/>
+    <hyperlink ref="G64" r:id="rId4" location="making-sure-that-the-app-is-properly-signed" xr:uid="{00000000-0004-0000-0400-000021000000}"/>
+    <hyperlink ref="G66" r:id="rId5" location="finding-debugging-symbols" xr:uid="{00000000-0004-0000-0400-000023000000}"/>
+    <hyperlink ref="G67" r:id="rId6" location="finding-debugging-code-and-verbose-error-logging" xr:uid="{00000000-0004-0000-0400-000024000000}"/>
+    <hyperlink ref="G72" r:id="rId7" location="make-sure-that-free-security-features-are-activated" xr:uid="{00000000-0004-0000-0400-000026000000}"/>
+    <hyperlink ref="G51" r:id="rId8" location="testing-custom-certificate-stores-and-certificate-pinning" xr:uid="{00000000-0004-0000-0400-00002F000000}"/>
+    <hyperlink ref="G69" r:id="rId9" location="testing-exception-handling" xr:uid="{00000000-0004-0000-0400-000032000000}"/>
+    <hyperlink ref="G18" r:id="rId10" location="checking-logs-for-sensitive-data" xr:uid="{46731861-EBBD-3340-B6B4-166DCFAD95AE}"/>
+    <hyperlink ref="G19" r:id="rId11" location="determining-whether-sensitive-data-is-sent-to-third-parties" xr:uid="{AE7B6F9B-7236-FD4A-8CDD-4D8C964B4EED}"/>
+    <hyperlink ref="G20" r:id="rId12" location="finding-sensitive-data-in-the-keyboard-cache" xr:uid="{9AE35269-EFC8-E643-9FCD-79431130C877}"/>
+    <hyperlink ref="G21" r:id="rId13" location="determining-whether-sensitive-data-is-exposed-via-ipc-mechanisms" xr:uid="{F3ED19E9-DBDC-8E4E-A5B6-FA8D0E47AE00}"/>
+    <hyperlink ref="G22" r:id="rId14" location="checking-for-sensitive-data-disclosed-through-the-user-interface" xr:uid="{4A839362-4FC0-0546-AD7C-1E9C63A9CA53}"/>
+    <hyperlink ref="G23" r:id="rId15" location="testing-backups-for-sensitive-data" xr:uid="{6035E15B-33A5-9E4F-B19C-87D4A1286459}"/>
+    <hyperlink ref="G24" r:id="rId16" location="testing-auto-generated-screenshots-for-sensitive-information" xr:uid="{3E9B0B2B-9503-CA4B-AEDB-CCB996D6DEBF}"/>
+    <hyperlink ref="G25" r:id="rId17" location="testing-memory-for-sensitive-data" xr:uid="{FBEB4D5D-9B5F-5E4E-B240-556982D6D6B5}"/>
+    <hyperlink ref="G43" r:id="rId18" location="testing-local-authentication" xr:uid="{280EFCC5-10BC-A045-92DF-D92EE814FB92}"/>
+    <hyperlink ref="G17" r:id="rId19" location="testing-local-data-storage" xr:uid="{DCDB9649-8EB0-2A41-84DB-35E9D40A5832}"/>
+    <hyperlink ref="G30" r:id="rId20" location="custom-implementations-of-cryptography" xr:uid="{00000000-0004-0000-0400-000009000000}"/>
+    <hyperlink ref="G32" r:id="rId21" location="identifying-insecure-and-or-deprecated-cryptographic-algorithms" xr:uid="{00000000-0004-0000-0400-00000B000000}"/>
+    <hyperlink ref="G31" r:id="rId22" location="common-configuration-issues" xr:uid="{00000000-0004-0000-0400-00000A000000}"/>
+    <hyperlink ref="G29" r:id="rId23" location="key-concepts" xr:uid="{00000000-0004-0000-0400-000008000000}"/>
+    <hyperlink ref="G34" r:id="rId24" location="random-number-generation-on-ios" xr:uid="{9F72DE31-A63E-F142-95B7-00687A8836E3}"/>
+    <hyperlink ref="G33" r:id="rId25" location="key-concepts" xr:uid="{857E130A-F093-294E-A0EB-D1CB72C7F260}"/>
+    <hyperlink ref="G41" r:id="rId26" location="running-a-password-dictionary-attack" xr:uid="{E2CB986A-236D-324E-BC9D-70BB7DDF6AF1}"/>
+    <hyperlink ref="G36" r:id="rId27" location="testing-authentication" xr:uid="{46A815C2-7719-7440-A3DA-ECFE48503304}"/>
+    <hyperlink ref="G40" r:id="rId28" location="best-practices-for-passwords" xr:uid="{71F2E91B-4865-944E-B512-CA7AAEC7DF58}"/>
+    <hyperlink ref="G39" r:id="rId29" location="user-logout-and-session-timeouts" xr:uid="{C3A0E459-A842-734A-9A34-A73770867D09}"/>
+    <hyperlink ref="G38" r:id="rId30" location="testing-stateless-token-based-authentication" xr:uid="{4E1DF7BA-5D00-4449-AA84-0CA84D2CFE0B}"/>
+    <hyperlink ref="G42" r:id="rId31" location="session-timeout" xr:uid="{50F3CC18-440C-724F-8BA2-E41AEFD19C7E}"/>
+    <hyperlink ref="G37" r:id="rId32" location="testing-stateful-session-management" xr:uid="{2DC02B43-93BE-0248-B857-8DC49E761130}"/>
+    <hyperlink ref="G44" r:id="rId33" location="verifying-that-2fa-is-enforced" xr:uid="{F329C298-6BE9-F845-B0B0-5D9492022AE3}"/>
+    <hyperlink ref="G45" r:id="rId34" location="verifying-that-2fa-is-enforced" xr:uid="{6B1C9CEB-A3B0-D449-BF6B-36ED8EC3C07E}"/>
+    <hyperlink ref="G50" r:id="rId35" location="app-transport-security" xr:uid="{00000000-0004-0000-0400-000018000000}"/>
+    <hyperlink ref="G48" r:id="rId36" location="verifying-data-encryption-on-the-network" xr:uid="{19091139-DCA3-1141-A151-E2172DBE92C3}"/>
+    <hyperlink ref="G49" r:id="rId37" location="verifying-data-encryption-on-the-network" xr:uid="{32DB5B9E-A743-114D-9239-8C43612B6BE7}"/>
+    <hyperlink ref="G52" r:id="rId38" location="making-sure-that-critical-operations-use-secure-communication-channels" xr:uid="{F320939B-B772-6944-8A7B-6CB1CC0EC617}"/>
+    <hyperlink ref="G56" r:id="rId39" location="injection-flaws" xr:uid="{7D24DE41-9983-AC42-A320-F51AAF1E7964}"/>
+    <hyperlink ref="G70" r:id="rId40" location="testing-exception-handling" xr:uid="{937EA1CD-B7DF-F44A-8618-52496B470E29}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -7699,7 +7639,7 @@
   <dimension ref="B1:G32"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7715,7 +7655,7 @@
   <sheetData>
     <row r="1" spans="2:7" ht="19" x14ac:dyDescent="0.25">
       <c r="B1" s="7" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="G1" s="24"/>
     </row>
@@ -7764,7 +7704,7 @@
         <v>136</v>
       </c>
       <c r="F5" s="58" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="G5" s="74"/>
     </row>
@@ -7782,7 +7722,7 @@
         <v>136</v>
       </c>
       <c r="F6" s="58" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G6" s="74"/>
     </row>
@@ -7800,7 +7740,7 @@
         <v>136</v>
       </c>
       <c r="F7" s="58" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G7" s="74"/>
     </row>
@@ -7817,9 +7757,7 @@
       <c r="E8" s="37" t="s">
         <v>136</v>
       </c>
-      <c r="F8" s="58" t="s">
-        <v>237</v>
-      </c>
+      <c r="F8" s="58"/>
       <c r="G8" s="74"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.2">
@@ -7835,9 +7773,7 @@
       <c r="E9" s="37" t="s">
         <v>136</v>
       </c>
-      <c r="F9" s="58" t="s">
-        <v>238</v>
-      </c>
+      <c r="F9" s="58"/>
       <c r="G9" s="74"/>
     </row>
     <row r="10" spans="2:7" ht="30" x14ac:dyDescent="0.2">
@@ -7853,9 +7789,7 @@
       <c r="E10" s="37" t="s">
         <v>136</v>
       </c>
-      <c r="F10" s="58" t="s">
-        <v>239</v>
-      </c>
+      <c r="F10" s="58"/>
       <c r="G10" s="74"/>
     </row>
     <row r="11" spans="2:7" ht="30" x14ac:dyDescent="0.2">
@@ -7863,7 +7797,7 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="C11" s="36" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D11" s="25" t="s">
         <v>7</v>
@@ -7871,9 +7805,7 @@
       <c r="E11" s="37" t="s">
         <v>136</v>
       </c>
-      <c r="F11" s="58" t="s">
-        <v>240</v>
-      </c>
+      <c r="F11" s="58"/>
       <c r="G11" s="74"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.2">
@@ -7881,7 +7813,7 @@
         <v>8.8000000000000007</v>
       </c>
       <c r="C12" s="36" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="D12" s="25" t="s">
         <v>7</v>
@@ -7889,14 +7821,12 @@
       <c r="E12" s="37" t="s">
         <v>136</v>
       </c>
-      <c r="F12" s="58" t="s">
-        <v>277</v>
-      </c>
+      <c r="F12" s="58"/>
       <c r="G12" s="74"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B13" s="71" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="C13" s="36" t="s">
         <v>63</v>
@@ -7907,9 +7837,7 @@
       <c r="E13" s="37" t="s">
         <v>136</v>
       </c>
-      <c r="F13" s="58" t="s">
-        <v>241</v>
-      </c>
+      <c r="F13" s="58"/>
       <c r="G13" s="74"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.2">
@@ -7936,7 +7864,7 @@
         <v>136</v>
       </c>
       <c r="F15" s="58" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="G15" s="74"/>
     </row>
@@ -7955,7 +7883,7 @@
         <v>8.11</v>
       </c>
       <c r="C17" s="36" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="D17" s="25" t="s">
         <v>7</v>
@@ -7963,9 +7891,7 @@
       <c r="E17" s="37" t="s">
         <v>136</v>
       </c>
-      <c r="F17" s="58" t="s">
-        <v>243</v>
-      </c>
+      <c r="F17" s="58"/>
       <c r="G17" s="74"/>
     </row>
     <row r="18" spans="2:7" ht="60" x14ac:dyDescent="0.2">
@@ -7973,7 +7899,7 @@
         <v>8.1199999999999992</v>
       </c>
       <c r="C18" s="36" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="D18" s="25" t="s">
         <v>7</v>
@@ -7981,9 +7907,7 @@
       <c r="E18" s="37" t="s">
         <v>136</v>
       </c>
-      <c r="F18" s="58" t="s">
-        <v>244</v>
-      </c>
+      <c r="F18" s="58"/>
       <c r="G18" s="74"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.2">
@@ -8114,24 +8038,16 @@
       <c r="F32" s="45"/>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E15 E17:E18 E5:E13" xr:uid="{00000000-0002-0000-0500-000000000000}">
       <formula1>"Pass,Fail,N/A"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="F5" r:id="rId1" location="testing-root-detection" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x06j-Testing-Resiliency-Against-Reverse-Engineering.html - testing-root-detection" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
-    <hyperlink ref="F6" r:id="rId2" location="testing-debugging-defenses" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x06j-Testing-Resiliency-Against-Reverse-Engineering.html - testing-debugging-defenses" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
-    <hyperlink ref="F7" r:id="rId3" location="testing-file-integrity-checks" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x06j-Testing-Resiliency-Against-Reverse-Engineering.html - testing-file-integrity-checks" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
-    <hyperlink ref="F8" r:id="rId4" location="testing-detection-of-reverse-engineering-tools" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x06j-Testing-Resiliency-Against-Reverse-Engineering.html - testing-detection-of-reverse-engineering-tools" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
-    <hyperlink ref="F9" r:id="rId5" location="testing-simple-emulator-detection" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x06j-Testing-Resiliency-Against-Reverse-Engineering.html - testing-simple-emulator-detection" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
-    <hyperlink ref="F10" r:id="rId6" location="testing-memory-integrity-checks" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x06j-Testing-Resiliency-Against-Reverse-Engineering.html - testing-memory-integrity-checks" xr:uid="{00000000-0004-0000-0500-000005000000}"/>
-    <hyperlink ref="F11" r:id="rId7" location="verifying-variablility-of-tampering-responses" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x06j-Testing-Resiliency-Against-Reverse-Engineering.html - verifying-variablility-of-tampering-responses" xr:uid="{00000000-0004-0000-0500-000006000000}"/>
-    <hyperlink ref="F15" r:id="rId8" location="testing-device-binding" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x06j-Testing-Resiliency-Against-Reverse-Engineering.html - testing-device-binding" xr:uid="{00000000-0004-0000-0500-000007000000}"/>
-    <hyperlink ref="F17" r:id="rId9" location="testing-advanced-anti-emulation" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x06j-Testing-Resiliency-Against-Reverse-Engineering.html - testing-advanced-anti-emulation" xr:uid="{00000000-0004-0000-0500-000008000000}"/>
-    <hyperlink ref="F18" r:id="rId10" location="testing-advanced-obfuscation" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x06j-Testing-Resiliency-Against-Reverse-Engineering.html - testing-advanced-obfuscation" xr:uid="{00000000-0004-0000-0500-000009000000}"/>
-    <hyperlink ref="F12" r:id="rId11" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x06j-Testing-Resiliency-Against-Reverse-Engineering.html" xr:uid="{00000000-0004-0000-0500-00000A000000}"/>
-    <hyperlink ref="F13" r:id="rId12" location="testing-simple-obfuscation" display="https://sushi2k.gitbooks.io/the-owasp-mobile-security-testing-guide/content/0x06j-Testing-Resiliency-Against-Reverse-Engineering.html - testing-simple-obfuscation" xr:uid="{00000000-0004-0000-0500-00000B000000}"/>
+    <hyperlink ref="F5" r:id="rId1" location="jailbreak-detection" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="F6" r:id="rId2" location="anti-debugging-checks" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
+    <hyperlink ref="F7" r:id="rId3" location="file-integrity-checks" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
+    <hyperlink ref="F15" r:id="rId4" location="device-binding" xr:uid="{00000000-0004-0000-0500-000007000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -8143,8 +8059,8 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8154,22 +8070,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="114" t="s">
+      <c r="A1" s="124" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="114"/>
+      <c r="B1" s="124"/>
       <c r="C1" s="50"/>
       <c r="D1" s="50"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="67" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="B2" s="67" t="s">
         <v>155</v>
       </c>
       <c r="C2" s="67" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D2" s="68" t="s">
         <v>165</v>
@@ -8186,7 +8102,7 @@
         <v>42765</v>
       </c>
       <c r="D3" s="64" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -8200,7 +8116,7 @@
         <v>42766</v>
       </c>
       <c r="D4" s="64" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -8214,7 +8130,7 @@
         <v>42778</v>
       </c>
       <c r="D5" s="64" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -8222,13 +8138,13 @@
         <v>177</v>
       </c>
       <c r="B6" s="69" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="C6" s="66">
         <v>42780</v>
       </c>
       <c r="D6" s="64" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -8236,13 +8152,13 @@
         <v>131</v>
       </c>
       <c r="B7" s="70" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="C7" s="66">
         <v>42781</v>
       </c>
       <c r="D7" s="64" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -8250,13 +8166,13 @@
         <v>177</v>
       </c>
       <c r="B8" s="70" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="C8" s="66">
         <v>42829</v>
       </c>
       <c r="D8" s="64" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -8264,13 +8180,13 @@
         <v>131</v>
       </c>
       <c r="B9" s="70" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="C9" s="66">
         <v>42919</v>
       </c>
       <c r="D9" s="64" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -8278,13 +8194,13 @@
         <v>131</v>
       </c>
       <c r="B10" s="70" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="C10" s="66">
         <v>42963</v>
       </c>
       <c r="D10" s="64" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -8292,13 +8208,13 @@
         <v>131</v>
       </c>
       <c r="B11" s="75" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="C11" s="66">
         <v>43113</v>
       </c>
       <c r="D11" s="64" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -8312,7 +8228,7 @@
         <v>43289</v>
       </c>
       <c r="D12" s="64" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
     </row>
   </sheetData>

</xml_diff>